<commit_message>
Added buttons. Added & ordered metadata
</commit_message>
<xml_diff>
--- a/documentation/Gantt.xlsx
+++ b/documentation/Gantt.xlsx
@@ -674,32 +674,65 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -728,62 +761,29 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1131,28 +1131,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ED108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="CH34" sqref="CH34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="126" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="126" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="105" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
@@ -1163,168 +1163,168 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="69">
+      <c r="G1" s="99">
         <v>42803</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="69">
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="99">
         <v>42804</v>
       </c>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="69">
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
+      <c r="U1" s="102"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="99">
         <v>42809</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="71"/>
-      <c r="AE1" s="69">
+      <c r="X1" s="102"/>
+      <c r="Y1" s="102"/>
+      <c r="Z1" s="102"/>
+      <c r="AA1" s="102"/>
+      <c r="AB1" s="102"/>
+      <c r="AC1" s="102"/>
+      <c r="AD1" s="103"/>
+      <c r="AE1" s="99">
         <v>42810</v>
       </c>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="71"/>
-      <c r="AM1" s="69">
+      <c r="AF1" s="102"/>
+      <c r="AG1" s="102"/>
+      <c r="AH1" s="102"/>
+      <c r="AI1" s="102"/>
+      <c r="AJ1" s="102"/>
+      <c r="AK1" s="102"/>
+      <c r="AL1" s="103"/>
+      <c r="AM1" s="99">
         <v>42811</v>
       </c>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="70"/>
-      <c r="AR1" s="70"/>
-      <c r="AS1" s="70"/>
-      <c r="AT1" s="71"/>
-      <c r="AU1" s="69">
+      <c r="AN1" s="102"/>
+      <c r="AO1" s="102"/>
+      <c r="AP1" s="102"/>
+      <c r="AQ1" s="102"/>
+      <c r="AR1" s="102"/>
+      <c r="AS1" s="102"/>
+      <c r="AT1" s="103"/>
+      <c r="AU1" s="99">
         <v>42816</v>
       </c>
-      <c r="AV1" s="70"/>
-      <c r="AW1" s="70"/>
-      <c r="AX1" s="70"/>
-      <c r="AY1" s="70"/>
-      <c r="AZ1" s="70"/>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="71"/>
-      <c r="BC1" s="69">
+      <c r="AV1" s="102"/>
+      <c r="AW1" s="102"/>
+      <c r="AX1" s="102"/>
+      <c r="AY1" s="102"/>
+      <c r="AZ1" s="102"/>
+      <c r="BA1" s="102"/>
+      <c r="BB1" s="103"/>
+      <c r="BC1" s="99">
         <v>42817</v>
       </c>
-      <c r="BD1" s="70"/>
-      <c r="BE1" s="70"/>
-      <c r="BF1" s="70"/>
-      <c r="BG1" s="70"/>
-      <c r="BH1" s="70"/>
-      <c r="BI1" s="70"/>
-      <c r="BJ1" s="71"/>
-      <c r="BK1" s="69">
+      <c r="BD1" s="102"/>
+      <c r="BE1" s="102"/>
+      <c r="BF1" s="102"/>
+      <c r="BG1" s="102"/>
+      <c r="BH1" s="102"/>
+      <c r="BI1" s="102"/>
+      <c r="BJ1" s="103"/>
+      <c r="BK1" s="99">
         <v>42818</v>
       </c>
-      <c r="BL1" s="70"/>
-      <c r="BM1" s="70"/>
-      <c r="BN1" s="70"/>
-      <c r="BO1" s="70"/>
-      <c r="BP1" s="70"/>
-      <c r="BQ1" s="70"/>
-      <c r="BR1" s="71"/>
-      <c r="BS1" s="69">
+      <c r="BL1" s="102"/>
+      <c r="BM1" s="102"/>
+      <c r="BN1" s="102"/>
+      <c r="BO1" s="102"/>
+      <c r="BP1" s="102"/>
+      <c r="BQ1" s="102"/>
+      <c r="BR1" s="103"/>
+      <c r="BS1" s="99">
         <v>42823</v>
       </c>
-      <c r="BT1" s="70"/>
-      <c r="BU1" s="70"/>
-      <c r="BV1" s="70"/>
-      <c r="BW1" s="70"/>
-      <c r="BX1" s="70"/>
-      <c r="BY1" s="70"/>
-      <c r="BZ1" s="71"/>
-      <c r="CA1" s="69">
+      <c r="BT1" s="102"/>
+      <c r="BU1" s="102"/>
+      <c r="BV1" s="102"/>
+      <c r="BW1" s="102"/>
+      <c r="BX1" s="102"/>
+      <c r="BY1" s="102"/>
+      <c r="BZ1" s="103"/>
+      <c r="CA1" s="99">
         <v>42824</v>
       </c>
-      <c r="CB1" s="74"/>
-      <c r="CC1" s="74"/>
-      <c r="CD1" s="74"/>
-      <c r="CE1" s="74"/>
-      <c r="CF1" s="74"/>
-      <c r="CG1" s="74"/>
-      <c r="CH1" s="75"/>
-      <c r="CI1" s="69">
+      <c r="CB1" s="100"/>
+      <c r="CC1" s="100"/>
+      <c r="CD1" s="100"/>
+      <c r="CE1" s="100"/>
+      <c r="CF1" s="100"/>
+      <c r="CG1" s="100"/>
+      <c r="CH1" s="101"/>
+      <c r="CI1" s="99">
         <v>42825</v>
       </c>
-      <c r="CJ1" s="74"/>
-      <c r="CK1" s="74"/>
-      <c r="CL1" s="74"/>
-      <c r="CM1" s="74"/>
-      <c r="CN1" s="74"/>
-      <c r="CO1" s="74"/>
-      <c r="CP1" s="75"/>
-      <c r="CQ1" s="69">
+      <c r="CJ1" s="100"/>
+      <c r="CK1" s="100"/>
+      <c r="CL1" s="100"/>
+      <c r="CM1" s="100"/>
+      <c r="CN1" s="100"/>
+      <c r="CO1" s="100"/>
+      <c r="CP1" s="101"/>
+      <c r="CQ1" s="99">
         <v>42826</v>
       </c>
-      <c r="CR1" s="74"/>
-      <c r="CS1" s="74"/>
-      <c r="CT1" s="74"/>
-      <c r="CU1" s="74"/>
-      <c r="CV1" s="74"/>
-      <c r="CW1" s="74"/>
-      <c r="CX1" s="75"/>
-      <c r="CY1" s="69">
+      <c r="CR1" s="100"/>
+      <c r="CS1" s="100"/>
+      <c r="CT1" s="100"/>
+      <c r="CU1" s="100"/>
+      <c r="CV1" s="100"/>
+      <c r="CW1" s="100"/>
+      <c r="CX1" s="101"/>
+      <c r="CY1" s="99">
         <v>42830</v>
       </c>
-      <c r="CZ1" s="74"/>
-      <c r="DA1" s="74"/>
-      <c r="DB1" s="74"/>
-      <c r="DC1" s="74"/>
-      <c r="DD1" s="74"/>
-      <c r="DE1" s="74"/>
-      <c r="DF1" s="75"/>
-      <c r="DG1" s="69">
+      <c r="CZ1" s="100"/>
+      <c r="DA1" s="100"/>
+      <c r="DB1" s="100"/>
+      <c r="DC1" s="100"/>
+      <c r="DD1" s="100"/>
+      <c r="DE1" s="100"/>
+      <c r="DF1" s="101"/>
+      <c r="DG1" s="99">
         <v>42831</v>
       </c>
-      <c r="DH1" s="74"/>
-      <c r="DI1" s="74"/>
-      <c r="DJ1" s="74"/>
-      <c r="DK1" s="74"/>
-      <c r="DL1" s="74"/>
-      <c r="DM1" s="74"/>
-      <c r="DN1" s="75"/>
-      <c r="DO1" s="69">
+      <c r="DH1" s="100"/>
+      <c r="DI1" s="100"/>
+      <c r="DJ1" s="100"/>
+      <c r="DK1" s="100"/>
+      <c r="DL1" s="100"/>
+      <c r="DM1" s="100"/>
+      <c r="DN1" s="101"/>
+      <c r="DO1" s="99">
         <v>42832</v>
       </c>
-      <c r="DP1" s="74"/>
-      <c r="DQ1" s="74"/>
-      <c r="DR1" s="74"/>
-      <c r="DS1" s="74"/>
-      <c r="DT1" s="74"/>
-      <c r="DU1" s="74"/>
-      <c r="DV1" s="75"/>
-      <c r="DW1" s="69"/>
-      <c r="DX1" s="74"/>
-      <c r="DY1" s="74"/>
-      <c r="DZ1" s="74"/>
-      <c r="EA1" s="74"/>
-      <c r="EB1" s="74"/>
-      <c r="EC1" s="74"/>
-      <c r="ED1" s="75"/>
+      <c r="DP1" s="100"/>
+      <c r="DQ1" s="100"/>
+      <c r="DR1" s="100"/>
+      <c r="DS1" s="100"/>
+      <c r="DT1" s="100"/>
+      <c r="DU1" s="100"/>
+      <c r="DV1" s="101"/>
+      <c r="DW1" s="99"/>
+      <c r="DX1" s="100"/>
+      <c r="DY1" s="100"/>
+      <c r="DZ1" s="100"/>
+      <c r="EA1" s="100"/>
+      <c r="EB1" s="100"/>
+      <c r="EC1" s="100"/>
+      <c r="ED1" s="101"/>
     </row>
-    <row r="2" spans="1:134" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
+    <row r="2" spans="1:134" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="104"/>
+      <c r="B2" s="105"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1705,19 +1705,19 @@
       <c r="ED2" s="9"/>
     </row>
     <row r="3" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A3" s="76">
+      <c r="A3" s="85">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="82"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="60" t="s">
         <v>31</v>
       </c>
@@ -1851,11 +1851,11 @@
       <c r="ED3" s="12"/>
     </row>
     <row r="4" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84"/>
+      <c r="A4" s="85"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="61"/>
       <c r="G4" s="65"/>
       <c r="H4" s="16"/>
@@ -1987,11 +1987,11 @@
       <c r="ED4" s="18"/>
     </row>
     <row r="5" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="95"/>
       <c r="F5" s="62" t="s">
         <v>32</v>
       </c>
@@ -2125,11 +2125,11 @@
       <c r="ED5" s="18"/>
     </row>
     <row r="6" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
       <c r="F6" s="61"/>
       <c r="G6" s="67"/>
       <c r="H6" s="22"/>
@@ -2261,17 +2261,17 @@
       <c r="ED6" s="18"/>
     </row>
     <row r="7" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A7" s="76">
+      <c r="A7" s="85">
         <v>2</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="87" t="s">
+      <c r="B7" s="98"/>
+      <c r="C7" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="91"/>
+      <c r="E7" s="80"/>
       <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
@@ -2405,11 +2405,11 @@
       <c r="ED7" s="25"/>
     </row>
     <row r="8" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="82"/>
       <c r="F8" s="61"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -2541,11 +2541,11 @@
       <c r="ED8" s="28"/>
     </row>
     <row r="9" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="93"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="82"/>
       <c r="F9" s="62" t="s">
         <v>32</v>
       </c>
@@ -2679,11 +2679,11 @@
       <c r="ED9" s="28"/>
     </row>
     <row r="10" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="84"/>
       <c r="F10" s="61"/>
       <c r="G10" s="26"/>
       <c r="H10" s="27"/>
@@ -2815,17 +2815,17 @@
       <c r="ED10" s="28"/>
     </row>
     <row r="11" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A11" s="76">
+      <c r="A11" s="85">
         <v>3</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78" t="s">
+      <c r="B11" s="98"/>
+      <c r="C11" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="81" t="s">
+      <c r="D11" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="82"/>
+      <c r="E11" s="93"/>
       <c r="F11" s="60" t="s">
         <v>31</v>
       </c>
@@ -2959,11 +2959,11 @@
       <c r="ED11" s="12"/>
     </row>
     <row r="12" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="84"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="95"/>
       <c r="F12" s="61"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3095,11 +3095,11 @@
       <c r="ED12" s="18"/>
     </row>
     <row r="13" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="84"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="62" t="s">
         <v>32</v>
       </c>
@@ -3233,11 +3233,11 @@
       <c r="ED13" s="18"/>
     </row>
     <row r="14" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="86"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="97"/>
       <c r="F14" s="61"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3369,17 +3369,17 @@
       <c r="ED14" s="18"/>
     </row>
     <row r="15" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A15" s="76">
+      <c r="A15" s="85">
         <v>4</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="87" t="s">
+      <c r="B15" s="98"/>
+      <c r="C15" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="91"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="60" t="s">
         <v>31</v>
       </c>
@@ -3513,11 +3513,11 @@
       <c r="ED15" s="25"/>
     </row>
     <row r="16" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="61"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -3649,11 +3649,11 @@
       <c r="ED16" s="28"/>
     </row>
     <row r="17" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A17" s="76"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="93"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="82"/>
       <c r="F17" s="62" t="s">
         <v>32</v>
       </c>
@@ -3787,11 +3787,11 @@
       <c r="ED17" s="28"/>
     </row>
     <row r="18" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A18" s="76"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="84"/>
       <c r="F18" s="61"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27"/>
@@ -3923,17 +3923,17 @@
       <c r="ED18" s="28"/>
     </row>
     <row r="19" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A19" s="76">
+      <c r="A19" s="85">
         <v>5</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="78" t="s">
+      <c r="B19" s="98"/>
+      <c r="C19" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="81" t="s">
+      <c r="D19" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="82"/>
+      <c r="E19" s="93"/>
       <c r="F19" s="60" t="s">
         <v>31</v>
       </c>
@@ -4067,11 +4067,11 @@
       <c r="ED19" s="12"/>
     </row>
     <row r="20" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="95"/>
       <c r="F20" s="61"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -4203,11 +4203,11 @@
       <c r="ED20" s="18"/>
     </row>
     <row r="21" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="84"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="62" t="s">
         <v>32</v>
       </c>
@@ -4341,11 +4341,11 @@
       <c r="ED21" s="18"/>
     </row>
     <row r="22" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="97"/>
       <c r="F22" s="61"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -4477,19 +4477,19 @@
       <c r="ED22" s="18"/>
     </row>
     <row r="23" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A23" s="76">
+      <c r="A23" s="85">
         <v>6</v>
       </c>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="97" t="s">
+      <c r="D23" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="91"/>
+      <c r="E23" s="80"/>
       <c r="F23" s="60" t="s">
         <v>31</v>
       </c>
@@ -4623,11 +4623,11 @@
       <c r="ED23" s="25"/>
     </row>
     <row r="24" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A24" s="76"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="93"/>
+      <c r="A24" s="85"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
       <c r="F24" s="61"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -4759,11 +4759,11 @@
       <c r="ED24" s="28"/>
     </row>
     <row r="25" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A25" s="76"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="93"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="82"/>
       <c r="F25" s="62" t="s">
         <v>32</v>
       </c>
@@ -4897,11 +4897,11 @@
       <c r="ED25" s="28"/>
     </row>
     <row r="26" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A26" s="76"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="95"/>
+      <c r="A26" s="85"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="84"/>
       <c r="F26" s="61"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
@@ -5033,17 +5033,17 @@
       <c r="ED26" s="28"/>
     </row>
     <row r="27" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A27" s="76">
+      <c r="A27" s="85">
         <v>7</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="78" t="s">
+      <c r="B27" s="86"/>
+      <c r="C27" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="82"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="60" t="s">
         <v>31</v>
       </c>
@@ -5177,11 +5177,11 @@
       <c r="ED27" s="12"/>
     </row>
     <row r="28" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A28" s="76"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="84"/>
+      <c r="A28" s="85"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="95"/>
       <c r="F28" s="61"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -5313,11 +5313,11 @@
       <c r="ED28" s="18"/>
     </row>
     <row r="29" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A29" s="76"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="84"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="95"/>
       <c r="F29" s="62" t="s">
         <v>32</v>
       </c>
@@ -5369,16 +5369,16 @@
       <c r="AZ29" s="19"/>
       <c r="BA29" s="19"/>
       <c r="BB29" s="30"/>
-      <c r="BC29" s="17"/>
-      <c r="BD29" s="17"/>
-      <c r="BE29" s="17"/>
-      <c r="BF29" s="17"/>
-      <c r="BG29" s="17"/>
-      <c r="BH29" s="17"/>
-      <c r="BI29" s="17"/>
-      <c r="BJ29" s="18"/>
-      <c r="BK29" s="17"/>
-      <c r="BL29" s="17"/>
+      <c r="BC29" s="19"/>
+      <c r="BD29" s="19"/>
+      <c r="BE29" s="19"/>
+      <c r="BF29" s="19"/>
+      <c r="BG29" s="19"/>
+      <c r="BH29" s="19"/>
+      <c r="BI29" s="19"/>
+      <c r="BJ29" s="30"/>
+      <c r="BK29" s="19"/>
+      <c r="BL29" s="19"/>
       <c r="BM29" s="17"/>
       <c r="BN29" s="17"/>
       <c r="BO29" s="17"/>
@@ -5451,11 +5451,11 @@
       <c r="ED29" s="18"/>
     </row>
     <row r="30" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A30" s="76"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="86"/>
+      <c r="A30" s="85"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="97"/>
       <c r="F30" s="61"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5505,16 +5505,16 @@
       <c r="AZ30" s="19"/>
       <c r="BA30" s="19"/>
       <c r="BB30" s="30"/>
-      <c r="BC30" s="17"/>
-      <c r="BD30" s="17"/>
-      <c r="BE30" s="17"/>
-      <c r="BF30" s="17"/>
-      <c r="BG30" s="17"/>
-      <c r="BH30" s="17"/>
-      <c r="BI30" s="17"/>
-      <c r="BJ30" s="18"/>
-      <c r="BK30" s="17"/>
-      <c r="BL30" s="17"/>
+      <c r="BC30" s="19"/>
+      <c r="BD30" s="19"/>
+      <c r="BE30" s="19"/>
+      <c r="BF30" s="19"/>
+      <c r="BG30" s="19"/>
+      <c r="BH30" s="19"/>
+      <c r="BI30" s="19"/>
+      <c r="BJ30" s="30"/>
+      <c r="BK30" s="19"/>
+      <c r="BL30" s="19"/>
       <c r="BM30" s="17"/>
       <c r="BN30" s="17"/>
       <c r="BO30" s="17"/>
@@ -5587,17 +5587,17 @@
       <c r="ED30" s="18"/>
     </row>
     <row r="31" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A31" s="76">
+      <c r="A31" s="85">
         <v>8</v>
       </c>
-      <c r="B31" s="96"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="86"/>
+      <c r="C31" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="97" t="s">
+      <c r="D31" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="91"/>
+      <c r="E31" s="80"/>
       <c r="F31" s="60" t="s">
         <v>31</v>
       </c>
@@ -5731,11 +5731,11 @@
       <c r="ED31" s="25"/>
     </row>
     <row r="32" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="93"/>
+      <c r="A32" s="85"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="82"/>
       <c r="F32" s="61"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -5867,11 +5867,11 @@
       <c r="ED32" s="28"/>
     </row>
     <row r="33" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="93"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="82"/>
       <c r="F33" s="62" t="s">
         <v>32</v>
       </c>
@@ -5933,12 +5933,12 @@
       <c r="BJ33" s="28"/>
       <c r="BK33" s="26"/>
       <c r="BL33" s="27"/>
-      <c r="BM33" s="27"/>
-      <c r="BN33" s="27"/>
-      <c r="BO33" s="27"/>
-      <c r="BP33" s="27"/>
-      <c r="BQ33" s="27"/>
-      <c r="BR33" s="28"/>
+      <c r="BM33" s="19"/>
+      <c r="BN33" s="19"/>
+      <c r="BO33" s="19"/>
+      <c r="BP33" s="19"/>
+      <c r="BQ33" s="19"/>
+      <c r="BR33" s="30"/>
       <c r="BS33" s="26"/>
       <c r="BT33" s="27"/>
       <c r="BU33" s="27"/>
@@ -6005,11 +6005,11 @@
       <c r="ED33" s="28"/>
     </row>
     <row r="34" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="95"/>
+      <c r="A34" s="85"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="84"/>
       <c r="F34" s="61"/>
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
@@ -6069,12 +6069,12 @@
       <c r="BJ34" s="28"/>
       <c r="BK34" s="26"/>
       <c r="BL34" s="27"/>
-      <c r="BM34" s="27"/>
-      <c r="BN34" s="27"/>
-      <c r="BO34" s="27"/>
-      <c r="BP34" s="27"/>
-      <c r="BQ34" s="27"/>
-      <c r="BR34" s="28"/>
+      <c r="BM34" s="19"/>
+      <c r="BN34" s="19"/>
+      <c r="BO34" s="19"/>
+      <c r="BP34" s="19"/>
+      <c r="BQ34" s="19"/>
+      <c r="BR34" s="30"/>
       <c r="BS34" s="26"/>
       <c r="BT34" s="27"/>
       <c r="BU34" s="27"/>
@@ -6141,17 +6141,17 @@
       <c r="ED34" s="28"/>
     </row>
     <row r="35" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A35" s="76">
+      <c r="A35" s="85">
         <v>9</v>
       </c>
-      <c r="B35" s="96"/>
-      <c r="C35" s="78" t="s">
+      <c r="B35" s="86"/>
+      <c r="C35" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D35" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="82"/>
+      <c r="E35" s="93"/>
       <c r="F35" s="60" t="s">
         <v>31</v>
       </c>
@@ -6285,11 +6285,11 @@
       <c r="ED35" s="12"/>
     </row>
     <row r="36" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
+      <c r="A36" s="85"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="95"/>
       <c r="F36" s="61"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -6421,11 +6421,11 @@
       <c r="ED36" s="18"/>
     </row>
     <row r="37" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="84"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="95"/>
       <c r="F37" s="62" t="s">
         <v>32</v>
       </c>
@@ -6559,11 +6559,11 @@
       <c r="ED37" s="18"/>
     </row>
     <row r="38" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="86"/>
+      <c r="A38" s="85"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="97"/>
       <c r="F38" s="61"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -6696,14 +6696,14 @@
     </row>
     <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="86"/>
+      <c r="C39" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="97" t="s">
+      <c r="D39" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="91"/>
+      <c r="E39" s="80"/>
       <c r="F39" s="60" t="s">
         <v>31</v>
       </c>
@@ -6838,10 +6838,10 @@
     </row>
     <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="93"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="82"/>
       <c r="F40" s="61"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -6974,10 +6974,10 @@
     </row>
     <row r="41" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="88"/>
-      <c r="D41" s="98"/>
-      <c r="E41" s="93"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="82"/>
       <c r="F41" s="62" t="s">
         <v>32</v>
       </c>
@@ -7112,10 +7112,10 @@
     </row>
     <row r="42" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="95"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="61"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -7248,14 +7248,14 @@
     </row>
     <row r="43" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="78" t="s">
+      <c r="B43" s="86"/>
+      <c r="C43" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="D43" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="82"/>
+      <c r="E43" s="93"/>
       <c r="F43" s="60" t="s">
         <v>31</v>
       </c>
@@ -7390,10 +7390,10 @@
     </row>
     <row r="44" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="83"/>
-      <c r="E44" s="84"/>
+      <c r="B44" s="86"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="95"/>
       <c r="F44" s="61"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -7526,10 +7526,10 @@
     </row>
     <row r="45" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="84"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="95"/>
       <c r="F45" s="62" t="s">
         <v>32</v>
       </c>
@@ -7664,10 +7664,10 @@
     </row>
     <row r="46" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="85"/>
-      <c r="E46" s="86"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="97"/>
       <c r="F46" s="61"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -7800,14 +7800,14 @@
     </row>
     <row r="47" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="87" t="s">
+      <c r="B47" s="86"/>
+      <c r="C47" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="97" t="s">
+      <c r="D47" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="91"/>
+      <c r="E47" s="80"/>
       <c r="F47" s="60" t="s">
         <v>31</v>
       </c>
@@ -7942,10 +7942,10 @@
     </row>
     <row r="48" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="93"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="82"/>
       <c r="F48" s="61"/>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -8078,10 +8078,10 @@
     </row>
     <row r="49" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="93"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="82"/>
       <c r="F49" s="62" t="s">
         <v>32</v>
       </c>
@@ -8216,10 +8216,10 @@
     </row>
     <row r="50" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="94"/>
-      <c r="E50" s="95"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="84"/>
       <c r="F50" s="61"/>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -8352,14 +8352,14 @@
     </row>
     <row r="51" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
-      <c r="B51" s="96"/>
+      <c r="B51" s="86"/>
       <c r="C51" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="81" t="s">
+      <c r="D51" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="82"/>
+      <c r="E51" s="93"/>
       <c r="F51" s="60" t="s">
         <v>31</v>
       </c>
@@ -8494,10 +8494,10 @@
     </row>
     <row r="52" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
-      <c r="B52" s="96"/>
+      <c r="B52" s="86"/>
       <c r="C52" s="53"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="84"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="95"/>
       <c r="F52" s="61"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
@@ -8630,10 +8630,10 @@
     </row>
     <row r="53" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
-      <c r="B53" s="96"/>
+      <c r="B53" s="86"/>
       <c r="C53" s="53"/>
-      <c r="D53" s="83"/>
-      <c r="E53" s="84"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="95"/>
       <c r="F53" s="62" t="s">
         <v>32</v>
       </c>
@@ -8768,10 +8768,10 @@
     </row>
     <row r="54" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
-      <c r="B54" s="96"/>
+      <c r="B54" s="86"/>
       <c r="C54" s="54"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="86"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="97"/>
       <c r="F54" s="61"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -8904,14 +8904,14 @@
     </row>
     <row r="55" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
-      <c r="B55" s="96"/>
+      <c r="B55" s="86"/>
       <c r="C55" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="97" t="s">
+      <c r="D55" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="91"/>
+      <c r="E55" s="80"/>
       <c r="F55" s="60" t="s">
         <v>31</v>
       </c>
@@ -9046,10 +9046,10 @@
     </row>
     <row r="56" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
-      <c r="B56" s="96"/>
+      <c r="B56" s="86"/>
       <c r="C56" s="56"/>
-      <c r="D56" s="98"/>
-      <c r="E56" s="93"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="82"/>
       <c r="F56" s="61"/>
       <c r="G56" s="26"/>
       <c r="H56" s="27"/>
@@ -9182,10 +9182,10 @@
     </row>
     <row r="57" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
-      <c r="B57" s="96"/>
+      <c r="B57" s="86"/>
       <c r="C57" s="56"/>
-      <c r="D57" s="98"/>
-      <c r="E57" s="93"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="82"/>
       <c r="F57" s="62" t="s">
         <v>32</v>
       </c>
@@ -9320,10 +9320,10 @@
     </row>
     <row r="58" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
-      <c r="B58" s="96"/>
+      <c r="B58" s="86"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="94"/>
-      <c r="E58" s="95"/>
+      <c r="D58" s="83"/>
+      <c r="E58" s="84"/>
       <c r="F58" s="61"/>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -9456,14 +9456,14 @@
     </row>
     <row r="59" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A59" s="51"/>
-      <c r="B59" s="96"/>
+      <c r="B59" s="86"/>
       <c r="C59" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="81" t="s">
+      <c r="D59" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="82"/>
+      <c r="E59" s="93"/>
       <c r="F59" s="60" t="s">
         <v>31</v>
       </c>
@@ -9598,10 +9598,10 @@
     </row>
     <row r="60" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A60" s="51"/>
-      <c r="B60" s="96"/>
+      <c r="B60" s="86"/>
       <c r="C60" s="53"/>
-      <c r="D60" s="83"/>
-      <c r="E60" s="84"/>
+      <c r="D60" s="94"/>
+      <c r="E60" s="95"/>
       <c r="F60" s="61"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -9734,10 +9734,10 @@
     </row>
     <row r="61" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
-      <c r="B61" s="96"/>
+      <c r="B61" s="86"/>
       <c r="C61" s="53"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="84"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="95"/>
       <c r="F61" s="62" t="s">
         <v>32</v>
       </c>
@@ -9872,10 +9872,10 @@
     </row>
     <row r="62" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
-      <c r="B62" s="96"/>
+      <c r="B62" s="86"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="86"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="97"/>
       <c r="F62" s="61"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -10008,10 +10008,10 @@
     </row>
     <row r="63" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="87"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="91"/>
+      <c r="B63" s="86"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="80"/>
       <c r="F63" s="60" t="s">
         <v>31</v>
       </c>
@@ -10146,10 +10146,10 @@
     </row>
     <row r="64" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="93"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="77"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="82"/>
       <c r="F64" s="61"/>
       <c r="G64" s="26"/>
       <c r="H64" s="27"/>
@@ -10282,10 +10282,10 @@
     </row>
     <row r="65" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="88"/>
-      <c r="D65" s="98"/>
-      <c r="E65" s="93"/>
+      <c r="B65" s="86"/>
+      <c r="C65" s="77"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="82"/>
       <c r="F65" s="62" t="s">
         <v>32</v>
       </c>
@@ -10420,10 +10420,10 @@
     </row>
     <row r="66" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="89"/>
-      <c r="D66" s="94"/>
-      <c r="E66" s="95"/>
+      <c r="B66" s="86"/>
+      <c r="C66" s="78"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="84"/>
       <c r="F66" s="61"/>
       <c r="G66" s="26"/>
       <c r="H66" s="27"/>
@@ -10556,10 +10556,10 @@
     </row>
     <row r="67" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A67" s="51"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="81"/>
-      <c r="E67" s="82"/>
+      <c r="B67" s="86"/>
+      <c r="C67" s="89"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="93"/>
       <c r="F67" s="60" t="s">
         <v>31</v>
       </c>
@@ -10694,10 +10694,10 @@
     </row>
     <row r="68" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A68" s="51"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="79"/>
-      <c r="D68" s="83"/>
-      <c r="E68" s="84"/>
+      <c r="B68" s="86"/>
+      <c r="C68" s="90"/>
+      <c r="D68" s="94"/>
+      <c r="E68" s="95"/>
       <c r="F68" s="61"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -10830,10 +10830,10 @@
     </row>
     <row r="69" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A69" s="51"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="79"/>
-      <c r="D69" s="83"/>
-      <c r="E69" s="84"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="90"/>
+      <c r="D69" s="94"/>
+      <c r="E69" s="95"/>
       <c r="F69" s="62" t="s">
         <v>32</v>
       </c>
@@ -10968,10 +10968,10 @@
     </row>
     <row r="70" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A70" s="51"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="85"/>
-      <c r="E70" s="86"/>
+      <c r="B70" s="86"/>
+      <c r="C70" s="91"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="97"/>
       <c r="F70" s="61"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -11104,10 +11104,10 @@
     </row>
     <row r="71" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A71" s="51"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="87"/>
-      <c r="D71" s="97"/>
-      <c r="E71" s="91"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="79"/>
+      <c r="E71" s="80"/>
       <c r="F71" s="60" t="s">
         <v>31</v>
       </c>
@@ -11242,10 +11242,10 @@
     </row>
     <row r="72" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A72" s="51"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="88"/>
-      <c r="D72" s="98"/>
-      <c r="E72" s="93"/>
+      <c r="B72" s="86"/>
+      <c r="C72" s="77"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="82"/>
       <c r="F72" s="61"/>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
@@ -11378,10 +11378,10 @@
     </row>
     <row r="73" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="88"/>
-      <c r="D73" s="98"/>
-      <c r="E73" s="93"/>
+      <c r="B73" s="86"/>
+      <c r="C73" s="77"/>
+      <c r="D73" s="81"/>
+      <c r="E73" s="82"/>
       <c r="F73" s="62" t="s">
         <v>32</v>
       </c>
@@ -11516,10 +11516,10 @@
     </row>
     <row r="74" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A74" s="51"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="89"/>
-      <c r="D74" s="94"/>
-      <c r="E74" s="95"/>
+      <c r="B74" s="86"/>
+      <c r="C74" s="78"/>
+      <c r="D74" s="83"/>
+      <c r="E74" s="84"/>
       <c r="F74" s="61"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -11652,10 +11652,10 @@
     </row>
     <row r="75" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A75" s="51"/>
-      <c r="B75" s="96"/>
-      <c r="C75" s="78"/>
-      <c r="D75" s="81"/>
-      <c r="E75" s="82"/>
+      <c r="B75" s="86"/>
+      <c r="C75" s="89"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="93"/>
       <c r="F75" s="60" t="s">
         <v>31</v>
       </c>
@@ -11790,10 +11790,10 @@
     </row>
     <row r="76" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A76" s="51"/>
-      <c r="B76" s="96"/>
-      <c r="C76" s="79"/>
-      <c r="D76" s="83"/>
-      <c r="E76" s="84"/>
+      <c r="B76" s="86"/>
+      <c r="C76" s="90"/>
+      <c r="D76" s="94"/>
+      <c r="E76" s="95"/>
       <c r="F76" s="61"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -11926,10 +11926,10 @@
     </row>
     <row r="77" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A77" s="51"/>
-      <c r="B77" s="96"/>
-      <c r="C77" s="79"/>
-      <c r="D77" s="83"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="86"/>
+      <c r="C77" s="90"/>
+      <c r="D77" s="94"/>
+      <c r="E77" s="95"/>
       <c r="F77" s="62" t="s">
         <v>32</v>
       </c>
@@ -12064,10 +12064,10 @@
     </row>
     <row r="78" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
-      <c r="B78" s="96"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="85"/>
-      <c r="E78" s="86"/>
+      <c r="B78" s="86"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="96"/>
+      <c r="E78" s="97"/>
       <c r="F78" s="61"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -12199,19 +12199,19 @@
       <c r="ED78" s="18"/>
     </row>
     <row r="79" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A79" s="76">
+      <c r="A79" s="85">
         <v>11</v>
       </c>
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="87" t="s">
+      <c r="C79" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="97" t="s">
+      <c r="D79" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="91"/>
+      <c r="E79" s="80"/>
       <c r="F79" s="60" t="s">
         <v>31</v>
       </c>
@@ -12345,11 +12345,11 @@
       <c r="ED79" s="25"/>
     </row>
     <row r="80" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A80" s="76"/>
-      <c r="B80" s="77"/>
-      <c r="C80" s="88"/>
-      <c r="D80" s="98"/>
-      <c r="E80" s="93"/>
+      <c r="A80" s="85"/>
+      <c r="B80" s="98"/>
+      <c r="C80" s="77"/>
+      <c r="D80" s="81"/>
+      <c r="E80" s="82"/>
       <c r="F80" s="61"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12481,11 +12481,11 @@
       <c r="ED80" s="28"/>
     </row>
     <row r="81" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A81" s="76"/>
-      <c r="B81" s="77"/>
-      <c r="C81" s="88"/>
-      <c r="D81" s="98"/>
-      <c r="E81" s="93"/>
+      <c r="A81" s="85"/>
+      <c r="B81" s="98"/>
+      <c r="C81" s="77"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="82"/>
       <c r="F81" s="62" t="s">
         <v>32</v>
       </c>
@@ -12619,11 +12619,11 @@
       <c r="ED81" s="28"/>
     </row>
     <row r="82" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A82" s="76"/>
-      <c r="B82" s="77"/>
-      <c r="C82" s="89"/>
-      <c r="D82" s="94"/>
-      <c r="E82" s="95"/>
+      <c r="A82" s="85"/>
+      <c r="B82" s="98"/>
+      <c r="C82" s="78"/>
+      <c r="D82" s="83"/>
+      <c r="E82" s="84"/>
       <c r="F82" s="61"/>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
@@ -12756,14 +12756,14 @@
     </row>
     <row r="83" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A83" s="51"/>
-      <c r="B83" s="77"/>
-      <c r="C83" s="78" t="s">
+      <c r="B83" s="98"/>
+      <c r="C83" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="81" t="s">
+      <c r="D83" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="E83" s="82"/>
+      <c r="E83" s="93"/>
       <c r="F83" s="60" t="s">
         <v>31</v>
       </c>
@@ -12898,10 +12898,10 @@
     </row>
     <row r="84" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A84" s="51"/>
-      <c r="B84" s="77"/>
-      <c r="C84" s="79"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="84"/>
+      <c r="B84" s="98"/>
+      <c r="C84" s="90"/>
+      <c r="D84" s="94"/>
+      <c r="E84" s="95"/>
       <c r="F84" s="61"/>
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
@@ -13034,10 +13034,10 @@
     </row>
     <row r="85" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A85" s="51"/>
-      <c r="B85" s="77"/>
-      <c r="C85" s="79"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="84"/>
+      <c r="B85" s="98"/>
+      <c r="C85" s="90"/>
+      <c r="D85" s="94"/>
+      <c r="E85" s="95"/>
       <c r="F85" s="62" t="s">
         <v>32</v>
       </c>
@@ -13172,10 +13172,10 @@
     </row>
     <row r="86" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A86" s="51"/>
-      <c r="B86" s="77"/>
-      <c r="C86" s="80"/>
-      <c r="D86" s="85"/>
-      <c r="E86" s="86"/>
+      <c r="B86" s="98"/>
+      <c r="C86" s="91"/>
+      <c r="D86" s="96"/>
+      <c r="E86" s="97"/>
       <c r="F86" s="61"/>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -13308,14 +13308,14 @@
     </row>
     <row r="87" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A87" s="51"/>
-      <c r="B87" s="77"/>
-      <c r="C87" s="87" t="s">
+      <c r="B87" s="98"/>
+      <c r="C87" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="D87" s="97" t="s">
+      <c r="D87" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="91"/>
+      <c r="E87" s="80"/>
       <c r="F87" s="60" t="s">
         <v>31</v>
       </c>
@@ -13450,10 +13450,10 @@
     </row>
     <row r="88" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A88" s="51"/>
-      <c r="B88" s="77"/>
-      <c r="C88" s="88"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="93"/>
+      <c r="B88" s="98"/>
+      <c r="C88" s="77"/>
+      <c r="D88" s="81"/>
+      <c r="E88" s="82"/>
       <c r="F88" s="61"/>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -13586,10 +13586,10 @@
     </row>
     <row r="89" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A89" s="51"/>
-      <c r="B89" s="77"/>
-      <c r="C89" s="88"/>
-      <c r="D89" s="98"/>
-      <c r="E89" s="93"/>
+      <c r="B89" s="98"/>
+      <c r="C89" s="77"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="82"/>
       <c r="F89" s="62" t="s">
         <v>32</v>
       </c>
@@ -13724,10 +13724,10 @@
     </row>
     <row r="90" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
-      <c r="B90" s="77"/>
-      <c r="C90" s="89"/>
-      <c r="D90" s="94"/>
-      <c r="E90" s="95"/>
+      <c r="B90" s="98"/>
+      <c r="C90" s="78"/>
+      <c r="D90" s="83"/>
+      <c r="E90" s="84"/>
       <c r="F90" s="61"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -13859,17 +13859,17 @@
       <c r="ED90" s="28"/>
     </row>
     <row r="91" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A91" s="76">
+      <c r="A91" s="85">
         <v>13</v>
       </c>
-      <c r="B91" s="77"/>
-      <c r="C91" s="78" t="s">
+      <c r="B91" s="98"/>
+      <c r="C91" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="81" t="s">
+      <c r="D91" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E91" s="82"/>
+      <c r="E91" s="93"/>
       <c r="F91" s="60" t="s">
         <v>31</v>
       </c>
@@ -14003,11 +14003,11 @@
       <c r="ED91" s="12"/>
     </row>
     <row r="92" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A92" s="76"/>
-      <c r="B92" s="77"/>
-      <c r="C92" s="79"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="84"/>
+      <c r="A92" s="85"/>
+      <c r="B92" s="98"/>
+      <c r="C92" s="90"/>
+      <c r="D92" s="94"/>
+      <c r="E92" s="95"/>
       <c r="F92" s="61"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -14139,11 +14139,11 @@
       <c r="ED92" s="18"/>
     </row>
     <row r="93" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A93" s="76"/>
-      <c r="B93" s="77"/>
-      <c r="C93" s="79"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="84"/>
+      <c r="A93" s="85"/>
+      <c r="B93" s="98"/>
+      <c r="C93" s="90"/>
+      <c r="D93" s="94"/>
+      <c r="E93" s="95"/>
       <c r="F93" s="62" t="s">
         <v>32</v>
       </c>
@@ -14277,11 +14277,11 @@
       <c r="ED93" s="18"/>
     </row>
     <row r="94" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A94" s="76"/>
-      <c r="B94" s="77"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="85"/>
-      <c r="E94" s="86"/>
+      <c r="A94" s="85"/>
+      <c r="B94" s="98"/>
+      <c r="C94" s="91"/>
+      <c r="D94" s="96"/>
+      <c r="E94" s="97"/>
       <c r="F94" s="61"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17"/>
@@ -14413,19 +14413,19 @@
       <c r="ED94" s="18"/>
     </row>
     <row r="95" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A95" s="76">
+      <c r="A95" s="85">
         <v>14</v>
       </c>
-      <c r="B95" s="96" t="s">
+      <c r="B95" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="87" t="s">
+      <c r="C95" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="90" t="s">
+      <c r="D95" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="91"/>
+      <c r="E95" s="80"/>
       <c r="F95" s="60" t="s">
         <v>31</v>
       </c>
@@ -14559,11 +14559,11 @@
       <c r="ED95" s="25"/>
     </row>
     <row r="96" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A96" s="76"/>
-      <c r="B96" s="96"/>
-      <c r="C96" s="88"/>
-      <c r="D96" s="92"/>
-      <c r="E96" s="93"/>
+      <c r="A96" s="85"/>
+      <c r="B96" s="86"/>
+      <c r="C96" s="77"/>
+      <c r="D96" s="88"/>
+      <c r="E96" s="82"/>
       <c r="F96" s="61"/>
       <c r="G96" s="26"/>
       <c r="H96" s="27"/>
@@ -14695,11 +14695,11 @@
       <c r="ED96" s="28"/>
     </row>
     <row r="97" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A97" s="76"/>
-      <c r="B97" s="96"/>
-      <c r="C97" s="88"/>
-      <c r="D97" s="92"/>
-      <c r="E97" s="93"/>
+      <c r="A97" s="85"/>
+      <c r="B97" s="86"/>
+      <c r="C97" s="77"/>
+      <c r="D97" s="88"/>
+      <c r="E97" s="82"/>
       <c r="F97" s="62" t="s">
         <v>32</v>
       </c>
@@ -14833,11 +14833,11 @@
       <c r="ED97" s="28"/>
     </row>
     <row r="98" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A98" s="76"/>
-      <c r="B98" s="96"/>
-      <c r="C98" s="89"/>
-      <c r="D98" s="94"/>
-      <c r="E98" s="95"/>
+      <c r="A98" s="85"/>
+      <c r="B98" s="86"/>
+      <c r="C98" s="78"/>
+      <c r="D98" s="83"/>
+      <c r="E98" s="84"/>
       <c r="F98" s="61"/>
       <c r="G98" s="26"/>
       <c r="H98" s="27"/>
@@ -14969,17 +14969,17 @@
       <c r="ED98" s="28"/>
     </row>
     <row r="99" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A99" s="76">
+      <c r="A99" s="85">
         <v>15</v>
       </c>
-      <c r="B99" s="96"/>
-      <c r="C99" s="78" t="s">
+      <c r="B99" s="86"/>
+      <c r="C99" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="81" t="s">
+      <c r="D99" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="E99" s="82"/>
+      <c r="E99" s="93"/>
       <c r="F99" s="60" t="s">
         <v>31</v>
       </c>
@@ -15113,11 +15113,11 @@
       <c r="ED99" s="12"/>
     </row>
     <row r="100" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A100" s="76"/>
-      <c r="B100" s="96"/>
-      <c r="C100" s="79"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="84"/>
+      <c r="A100" s="85"/>
+      <c r="B100" s="86"/>
+      <c r="C100" s="90"/>
+      <c r="D100" s="94"/>
+      <c r="E100" s="95"/>
       <c r="F100" s="61"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -15249,11 +15249,11 @@
       <c r="ED100" s="18"/>
     </row>
     <row r="101" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A101" s="76"/>
-      <c r="B101" s="96"/>
-      <c r="C101" s="79"/>
-      <c r="D101" s="83"/>
-      <c r="E101" s="84"/>
+      <c r="A101" s="85"/>
+      <c r="B101" s="86"/>
+      <c r="C101" s="90"/>
+      <c r="D101" s="94"/>
+      <c r="E101" s="95"/>
       <c r="F101" s="62" t="s">
         <v>32</v>
       </c>
@@ -15387,11 +15387,11 @@
       <c r="ED101" s="18"/>
     </row>
     <row r="102" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A102" s="76"/>
-      <c r="B102" s="96"/>
-      <c r="C102" s="80"/>
-      <c r="D102" s="85"/>
-      <c r="E102" s="86"/>
+      <c r="A102" s="85"/>
+      <c r="B102" s="86"/>
+      <c r="C102" s="91"/>
+      <c r="D102" s="96"/>
+      <c r="E102" s="97"/>
       <c r="F102" s="61"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -15523,17 +15523,17 @@
       <c r="ED102" s="18"/>
     </row>
     <row r="103" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A103" s="76">
+      <c r="A103" s="85">
         <v>16</v>
       </c>
-      <c r="B103" s="96"/>
-      <c r="C103" s="87" t="s">
+      <c r="B103" s="86"/>
+      <c r="C103" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="90" t="s">
+      <c r="D103" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="91"/>
+      <c r="E103" s="80"/>
       <c r="F103" s="60" t="s">
         <v>31</v>
       </c>
@@ -15667,11 +15667,11 @@
       <c r="ED103" s="25"/>
     </row>
     <row r="104" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A104" s="76"/>
-      <c r="B104" s="96"/>
-      <c r="C104" s="88"/>
-      <c r="D104" s="92"/>
-      <c r="E104" s="93"/>
+      <c r="A104" s="85"/>
+      <c r="B104" s="86"/>
+      <c r="C104" s="77"/>
+      <c r="D104" s="88"/>
+      <c r="E104" s="82"/>
       <c r="F104" s="61"/>
       <c r="G104" s="26"/>
       <c r="H104" s="27"/>
@@ -15803,11 +15803,11 @@
       <c r="ED104" s="28"/>
     </row>
     <row r="105" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A105" s="76"/>
-      <c r="B105" s="96"/>
-      <c r="C105" s="88"/>
-      <c r="D105" s="92"/>
-      <c r="E105" s="93"/>
+      <c r="A105" s="85"/>
+      <c r="B105" s="86"/>
+      <c r="C105" s="77"/>
+      <c r="D105" s="88"/>
+      <c r="E105" s="82"/>
       <c r="F105" s="62" t="s">
         <v>32</v>
       </c>
@@ -15941,11 +15941,11 @@
       <c r="ED105" s="28"/>
     </row>
     <row r="106" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A106" s="76"/>
-      <c r="B106" s="96"/>
-      <c r="C106" s="89"/>
-      <c r="D106" s="94"/>
-      <c r="E106" s="95"/>
+      <c r="A106" s="85"/>
+      <c r="B106" s="86"/>
+      <c r="C106" s="78"/>
+      <c r="D106" s="83"/>
+      <c r="E106" s="84"/>
       <c r="F106" s="61"/>
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
@@ -16077,13 +16077,13 @@
       <c r="ED106" s="28"/>
     </row>
     <row r="107" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A107" s="99"/>
+      <c r="A107" s="69"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="100" t="s">
+      <c r="C107" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="102"/>
-      <c r="E107" s="103"/>
+      <c r="D107" s="72"/>
+      <c r="E107" s="73"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
       <c r="H107" s="44"/>
@@ -16217,11 +16217,11 @@
       <c r="ED107" s="45"/>
     </row>
     <row r="108" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A108" s="99"/>
+      <c r="A108" s="69"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="101"/>
-      <c r="D108" s="104"/>
-      <c r="E108" s="105"/>
+      <c r="C108" s="71"/>
+      <c r="D108" s="74"/>
+      <c r="E108" s="75"/>
       <c r="F108" s="46"/>
       <c r="G108" s="47"/>
       <c r="H108" s="48"/>
@@ -16354,44 +16354,40 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:E108"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:E90"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:E98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:E102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="D103:E106"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B94"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="D79:E82"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:E94"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="D83:E86"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:E74"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:E78"/>
-    <mergeCell ref="D59:E62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:E66"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:E70"/>
-    <mergeCell ref="D39:E42"/>
-    <mergeCell ref="D47:E50"/>
-    <mergeCell ref="D51:E54"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="AE1:AL1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="DW1:ED1"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="BC1:BJ1"/>
+    <mergeCell ref="BK1:BR1"/>
+    <mergeCell ref="BS1:BZ1"/>
+    <mergeCell ref="CA1:CH1"/>
+    <mergeCell ref="CI1:CP1"/>
+    <mergeCell ref="CQ1:CX1"/>
+    <mergeCell ref="CY1:DF1"/>
+    <mergeCell ref="DG1:DN1"/>
+    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:E6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:E22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="B23:B78"/>
     <mergeCell ref="C23:C26"/>
@@ -16408,40 +16404,44 @@
     <mergeCell ref="C47:C50"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:E6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:E14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:E22"/>
-    <mergeCell ref="DW1:ED1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="BC1:BJ1"/>
-    <mergeCell ref="BK1:BR1"/>
-    <mergeCell ref="BS1:BZ1"/>
-    <mergeCell ref="CA1:CH1"/>
-    <mergeCell ref="CI1:CP1"/>
-    <mergeCell ref="CQ1:CX1"/>
-    <mergeCell ref="CY1:DF1"/>
-    <mergeCell ref="DG1:DN1"/>
-    <mergeCell ref="DO1:DV1"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:V1"/>
-    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="D51:E54"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:E74"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:E78"/>
+    <mergeCell ref="D59:E62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:E66"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:E70"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B94"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:E82"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:E94"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:E86"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:E108"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:E90"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B106"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:E98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="D99:E102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:E106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started work on about and contact pages
</commit_message>
<xml_diff>
--- a/documentation/Gantt.xlsx
+++ b/documentation/Gantt.xlsx
@@ -564,7 +564,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -674,6 +674,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1132,7 +1133,7 @@
   <dimension ref="A1:ED108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BZ25" sqref="BZ25"/>
+      <selection activeCell="BT48" sqref="BT48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,10 +1150,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
@@ -1163,168 +1164,168 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="69">
+      <c r="G1" s="70">
         <v>42803</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="69">
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="70">
         <v>42804</v>
       </c>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="69">
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="70">
         <v>42809</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="71"/>
-      <c r="AE1" s="69">
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="70">
         <v>42810</v>
       </c>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="71"/>
-      <c r="AM1" s="69">
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="72"/>
+      <c r="AM1" s="70">
         <v>42811</v>
       </c>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="70"/>
-      <c r="AR1" s="70"/>
-      <c r="AS1" s="70"/>
-      <c r="AT1" s="71"/>
-      <c r="AU1" s="69">
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="71"/>
+      <c r="AP1" s="71"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="72"/>
+      <c r="AU1" s="70">
         <v>42816</v>
       </c>
-      <c r="AV1" s="70"/>
-      <c r="AW1" s="70"/>
-      <c r="AX1" s="70"/>
-      <c r="AY1" s="70"/>
-      <c r="AZ1" s="70"/>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="71"/>
-      <c r="BC1" s="69">
+      <c r="AV1" s="71"/>
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="71"/>
+      <c r="AY1" s="71"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="71"/>
+      <c r="BB1" s="72"/>
+      <c r="BC1" s="70">
         <v>42817</v>
       </c>
-      <c r="BD1" s="70"/>
-      <c r="BE1" s="70"/>
-      <c r="BF1" s="70"/>
-      <c r="BG1" s="70"/>
-      <c r="BH1" s="70"/>
-      <c r="BI1" s="70"/>
-      <c r="BJ1" s="71"/>
-      <c r="BK1" s="69">
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="71"/>
+      <c r="BH1" s="71"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="72"/>
+      <c r="BK1" s="70">
         <v>42818</v>
       </c>
-      <c r="BL1" s="70"/>
-      <c r="BM1" s="70"/>
-      <c r="BN1" s="70"/>
-      <c r="BO1" s="70"/>
-      <c r="BP1" s="70"/>
-      <c r="BQ1" s="70"/>
-      <c r="BR1" s="71"/>
-      <c r="BS1" s="69">
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="71"/>
+      <c r="BN1" s="71"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="71"/>
+      <c r="BQ1" s="71"/>
+      <c r="BR1" s="72"/>
+      <c r="BS1" s="70">
         <v>42823</v>
       </c>
-      <c r="BT1" s="70"/>
-      <c r="BU1" s="70"/>
-      <c r="BV1" s="70"/>
-      <c r="BW1" s="70"/>
-      <c r="BX1" s="70"/>
-      <c r="BY1" s="70"/>
-      <c r="BZ1" s="71"/>
-      <c r="CA1" s="69">
+      <c r="BT1" s="71"/>
+      <c r="BU1" s="71"/>
+      <c r="BV1" s="71"/>
+      <c r="BW1" s="71"/>
+      <c r="BX1" s="71"/>
+      <c r="BY1" s="71"/>
+      <c r="BZ1" s="72"/>
+      <c r="CA1" s="70">
         <v>42824</v>
       </c>
-      <c r="CB1" s="74"/>
-      <c r="CC1" s="74"/>
-      <c r="CD1" s="74"/>
-      <c r="CE1" s="74"/>
-      <c r="CF1" s="74"/>
-      <c r="CG1" s="74"/>
-      <c r="CH1" s="75"/>
-      <c r="CI1" s="69">
+      <c r="CB1" s="75"/>
+      <c r="CC1" s="75"/>
+      <c r="CD1" s="75"/>
+      <c r="CE1" s="75"/>
+      <c r="CF1" s="75"/>
+      <c r="CG1" s="75"/>
+      <c r="CH1" s="76"/>
+      <c r="CI1" s="70">
         <v>42825</v>
       </c>
-      <c r="CJ1" s="74"/>
-      <c r="CK1" s="74"/>
-      <c r="CL1" s="74"/>
-      <c r="CM1" s="74"/>
-      <c r="CN1" s="74"/>
-      <c r="CO1" s="74"/>
-      <c r="CP1" s="75"/>
-      <c r="CQ1" s="69">
+      <c r="CJ1" s="75"/>
+      <c r="CK1" s="75"/>
+      <c r="CL1" s="75"/>
+      <c r="CM1" s="75"/>
+      <c r="CN1" s="75"/>
+      <c r="CO1" s="75"/>
+      <c r="CP1" s="76"/>
+      <c r="CQ1" s="70">
         <v>42826</v>
       </c>
-      <c r="CR1" s="74"/>
-      <c r="CS1" s="74"/>
-      <c r="CT1" s="74"/>
-      <c r="CU1" s="74"/>
-      <c r="CV1" s="74"/>
-      <c r="CW1" s="74"/>
-      <c r="CX1" s="75"/>
-      <c r="CY1" s="69">
+      <c r="CR1" s="75"/>
+      <c r="CS1" s="75"/>
+      <c r="CT1" s="75"/>
+      <c r="CU1" s="75"/>
+      <c r="CV1" s="75"/>
+      <c r="CW1" s="75"/>
+      <c r="CX1" s="76"/>
+      <c r="CY1" s="70">
         <v>42830</v>
       </c>
-      <c r="CZ1" s="74"/>
-      <c r="DA1" s="74"/>
-      <c r="DB1" s="74"/>
-      <c r="DC1" s="74"/>
-      <c r="DD1" s="74"/>
-      <c r="DE1" s="74"/>
-      <c r="DF1" s="75"/>
-      <c r="DG1" s="69">
+      <c r="CZ1" s="75"/>
+      <c r="DA1" s="75"/>
+      <c r="DB1" s="75"/>
+      <c r="DC1" s="75"/>
+      <c r="DD1" s="75"/>
+      <c r="DE1" s="75"/>
+      <c r="DF1" s="76"/>
+      <c r="DG1" s="70">
         <v>42831</v>
       </c>
-      <c r="DH1" s="74"/>
-      <c r="DI1" s="74"/>
-      <c r="DJ1" s="74"/>
-      <c r="DK1" s="74"/>
-      <c r="DL1" s="74"/>
-      <c r="DM1" s="74"/>
-      <c r="DN1" s="75"/>
-      <c r="DO1" s="69">
+      <c r="DH1" s="75"/>
+      <c r="DI1" s="75"/>
+      <c r="DJ1" s="75"/>
+      <c r="DK1" s="75"/>
+      <c r="DL1" s="75"/>
+      <c r="DM1" s="75"/>
+      <c r="DN1" s="76"/>
+      <c r="DO1" s="70">
         <v>42832</v>
       </c>
-      <c r="DP1" s="74"/>
-      <c r="DQ1" s="74"/>
-      <c r="DR1" s="74"/>
-      <c r="DS1" s="74"/>
-      <c r="DT1" s="74"/>
-      <c r="DU1" s="74"/>
-      <c r="DV1" s="75"/>
-      <c r="DW1" s="69"/>
-      <c r="DX1" s="74"/>
-      <c r="DY1" s="74"/>
-      <c r="DZ1" s="74"/>
-      <c r="EA1" s="74"/>
-      <c r="EB1" s="74"/>
-      <c r="EC1" s="74"/>
-      <c r="ED1" s="75"/>
+      <c r="DP1" s="75"/>
+      <c r="DQ1" s="75"/>
+      <c r="DR1" s="75"/>
+      <c r="DS1" s="75"/>
+      <c r="DT1" s="75"/>
+      <c r="DU1" s="75"/>
+      <c r="DV1" s="76"/>
+      <c r="DW1" s="70"/>
+      <c r="DX1" s="75"/>
+      <c r="DY1" s="75"/>
+      <c r="DZ1" s="75"/>
+      <c r="EA1" s="75"/>
+      <c r="EB1" s="75"/>
+      <c r="EC1" s="75"/>
+      <c r="ED1" s="76"/>
     </row>
     <row r="2" spans="1:134" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="74"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1705,19 +1706,19 @@
       <c r="ED2" s="9"/>
     </row>
     <row r="3" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A3" s="76">
+      <c r="A3" s="77">
         <v>1</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="82"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="60" t="s">
         <v>31</v>
       </c>
@@ -1851,11 +1852,11 @@
       <c r="ED3" s="12"/>
     </row>
     <row r="4" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="61"/>
       <c r="G4" s="65"/>
       <c r="H4" s="16"/>
@@ -1987,11 +1988,11 @@
       <c r="ED4" s="18"/>
     </row>
     <row r="5" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="85"/>
       <c r="F5" s="62" t="s">
         <v>32</v>
       </c>
@@ -2125,11 +2126,11 @@
       <c r="ED5" s="18"/>
     </row>
     <row r="6" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="61"/>
       <c r="G6" s="67"/>
       <c r="H6" s="22"/>
@@ -2261,17 +2262,17 @@
       <c r="ED6" s="18"/>
     </row>
     <row r="7" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A7" s="76">
+      <c r="A7" s="77">
         <v>2</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="87" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="91"/>
+      <c r="E7" s="92"/>
       <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
@@ -2405,11 +2406,11 @@
       <c r="ED7" s="25"/>
     </row>
     <row r="8" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="94"/>
       <c r="F8" s="61"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -2541,11 +2542,11 @@
       <c r="ED8" s="28"/>
     </row>
     <row r="9" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="93"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="94"/>
       <c r="F9" s="62" t="s">
         <v>32</v>
       </c>
@@ -2679,11 +2680,11 @@
       <c r="ED9" s="28"/>
     </row>
     <row r="10" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="96"/>
       <c r="F10" s="61"/>
       <c r="G10" s="26"/>
       <c r="H10" s="27"/>
@@ -2815,17 +2816,17 @@
       <c r="ED10" s="28"/>
     </row>
     <row r="11" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A11" s="76">
+      <c r="A11" s="77">
         <v>3</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="81" t="s">
+      <c r="D11" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="82"/>
+      <c r="E11" s="83"/>
       <c r="F11" s="60" t="s">
         <v>31</v>
       </c>
@@ -2959,11 +2960,11 @@
       <c r="ED11" s="12"/>
     </row>
     <row r="12" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="84"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="61"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3095,11 +3096,11 @@
       <c r="ED12" s="18"/>
     </row>
     <row r="13" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="84"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="62" t="s">
         <v>32</v>
       </c>
@@ -3233,11 +3234,11 @@
       <c r="ED13" s="18"/>
     </row>
     <row r="14" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="86"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="61"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3369,17 +3370,17 @@
       <c r="ED14" s="18"/>
     </row>
     <row r="15" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A15" s="76">
+      <c r="A15" s="77">
         <v>4</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="87" t="s">
+      <c r="B15" s="78"/>
+      <c r="C15" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="91"/>
+      <c r="E15" s="92"/>
       <c r="F15" s="60" t="s">
         <v>31</v>
       </c>
@@ -3513,11 +3514,11 @@
       <c r="ED15" s="25"/>
     </row>
     <row r="16" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="94"/>
       <c r="F16" s="61"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -3649,11 +3650,11 @@
       <c r="ED16" s="28"/>
     </row>
     <row r="17" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A17" s="76"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="93"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="62" t="s">
         <v>32</v>
       </c>
@@ -3787,11 +3788,11 @@
       <c r="ED17" s="28"/>
     </row>
     <row r="18" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A18" s="76"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
       <c r="F18" s="61"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27"/>
@@ -3923,17 +3924,17 @@
       <c r="ED18" s="28"/>
     </row>
     <row r="19" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A19" s="76">
+      <c r="A19" s="77">
         <v>5</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="78" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="81" t="s">
+      <c r="D19" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="82"/>
+      <c r="E19" s="83"/>
       <c r="F19" s="60" t="s">
         <v>31</v>
       </c>
@@ -4067,11 +4068,11 @@
       <c r="ED19" s="12"/>
     </row>
     <row r="20" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A20" s="76"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
       <c r="F20" s="61"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -4203,11 +4204,11 @@
       <c r="ED20" s="18"/>
     </row>
     <row r="21" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="84"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="62" t="s">
         <v>32</v>
       </c>
@@ -4341,11 +4342,11 @@
       <c r="ED21" s="18"/>
     </row>
     <row r="22" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="86"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="61"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -4477,19 +4478,19 @@
       <c r="ED22" s="18"/>
     </row>
     <row r="23" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A23" s="76">
+      <c r="A23" s="77">
         <v>6</v>
       </c>
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="97" t="s">
+      <c r="D23" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="91"/>
+      <c r="E23" s="92"/>
       <c r="F23" s="60" t="s">
         <v>31</v>
       </c>
@@ -4623,11 +4624,11 @@
       <c r="ED23" s="25"/>
     </row>
     <row r="24" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A24" s="76"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="93"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="94"/>
       <c r="F24" s="61"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -4759,11 +4760,11 @@
       <c r="ED24" s="28"/>
     </row>
     <row r="25" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A25" s="76"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="93"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="94"/>
       <c r="F25" s="62" t="s">
         <v>32</v>
       </c>
@@ -4897,11 +4898,11 @@
       <c r="ED25" s="28"/>
     </row>
     <row r="26" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A26" s="76"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="95"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
       <c r="F26" s="61"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
@@ -5033,17 +5034,17 @@
       <c r="ED26" s="28"/>
     </row>
     <row r="27" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A27" s="76">
+      <c r="A27" s="77">
         <v>7</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="78" t="s">
+      <c r="B27" s="97"/>
+      <c r="C27" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="82"/>
+      <c r="E27" s="83"/>
       <c r="F27" s="60" t="s">
         <v>31</v>
       </c>
@@ -5177,11 +5178,11 @@
       <c r="ED27" s="12"/>
     </row>
     <row r="28" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A28" s="76"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="84"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="61"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -5313,11 +5314,11 @@
       <c r="ED28" s="18"/>
     </row>
     <row r="29" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A29" s="76"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="84"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="85"/>
       <c r="F29" s="62" t="s">
         <v>32</v>
       </c>
@@ -5451,11 +5452,11 @@
       <c r="ED29" s="18"/>
     </row>
     <row r="30" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A30" s="76"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="86"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="87"/>
       <c r="F30" s="61"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5587,17 +5588,17 @@
       <c r="ED30" s="18"/>
     </row>
     <row r="31" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A31" s="76">
+      <c r="A31" s="77">
         <v>8</v>
       </c>
-      <c r="B31" s="96"/>
-      <c r="C31" s="87" t="s">
+      <c r="B31" s="97"/>
+      <c r="C31" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="97" t="s">
+      <c r="D31" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="91"/>
+      <c r="E31" s="92"/>
       <c r="F31" s="60" t="s">
         <v>31</v>
       </c>
@@ -5731,11 +5732,11 @@
       <c r="ED31" s="25"/>
     </row>
     <row r="32" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="93"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="94"/>
       <c r="F32" s="61"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -5867,11 +5868,11 @@
       <c r="ED32" s="28"/>
     </row>
     <row r="33" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="93"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="94"/>
       <c r="F33" s="62" t="s">
         <v>32</v>
       </c>
@@ -5939,18 +5940,18 @@
       <c r="BP33" s="19"/>
       <c r="BQ33" s="19"/>
       <c r="BR33" s="30"/>
-      <c r="BS33" s="26"/>
-      <c r="BT33" s="27"/>
-      <c r="BU33" s="27"/>
-      <c r="BV33" s="27"/>
-      <c r="BW33" s="27"/>
-      <c r="BX33" s="27"/>
-      <c r="BY33" s="27"/>
-      <c r="BZ33" s="28"/>
-      <c r="CA33" s="26"/>
-      <c r="CB33" s="27"/>
-      <c r="CC33" s="27"/>
-      <c r="CD33" s="27"/>
+      <c r="BS33" s="68"/>
+      <c r="BT33" s="19"/>
+      <c r="BU33" s="19"/>
+      <c r="BV33" s="19"/>
+      <c r="BW33" s="19"/>
+      <c r="BX33" s="19"/>
+      <c r="BY33" s="19"/>
+      <c r="BZ33" s="30"/>
+      <c r="CA33" s="68"/>
+      <c r="CB33" s="19"/>
+      <c r="CC33" s="19"/>
+      <c r="CD33" s="19"/>
       <c r="CE33" s="27"/>
       <c r="CF33" s="27"/>
       <c r="CG33" s="27"/>
@@ -6005,11 +6006,11 @@
       <c r="ED33" s="28"/>
     </row>
     <row r="34" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="95"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
       <c r="F34" s="61"/>
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
@@ -6075,18 +6076,18 @@
       <c r="BP34" s="19"/>
       <c r="BQ34" s="19"/>
       <c r="BR34" s="30"/>
-      <c r="BS34" s="26"/>
-      <c r="BT34" s="27"/>
-      <c r="BU34" s="27"/>
-      <c r="BV34" s="27"/>
-      <c r="BW34" s="33"/>
-      <c r="BX34" s="33"/>
-      <c r="BY34" s="33"/>
-      <c r="BZ34" s="28"/>
-      <c r="CA34" s="26"/>
-      <c r="CB34" s="27"/>
-      <c r="CC34" s="27"/>
-      <c r="CD34" s="27"/>
+      <c r="BS34" s="68"/>
+      <c r="BT34" s="19"/>
+      <c r="BU34" s="19"/>
+      <c r="BV34" s="19"/>
+      <c r="BW34" s="69"/>
+      <c r="BX34" s="69"/>
+      <c r="BY34" s="69"/>
+      <c r="BZ34" s="30"/>
+      <c r="CA34" s="68"/>
+      <c r="CB34" s="19"/>
+      <c r="CC34" s="19"/>
+      <c r="CD34" s="19"/>
       <c r="CE34" s="27"/>
       <c r="CF34" s="27"/>
       <c r="CG34" s="27"/>
@@ -6141,17 +6142,17 @@
       <c r="ED34" s="28"/>
     </row>
     <row r="35" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A35" s="76">
+      <c r="A35" s="77">
         <v>9</v>
       </c>
-      <c r="B35" s="96"/>
-      <c r="C35" s="78" t="s">
+      <c r="B35" s="97"/>
+      <c r="C35" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="82"/>
+      <c r="E35" s="83"/>
       <c r="F35" s="60" t="s">
         <v>31</v>
       </c>
@@ -6285,11 +6286,11 @@
       <c r="ED35" s="12"/>
     </row>
     <row r="36" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85"/>
       <c r="F36" s="61"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -6421,11 +6422,11 @@
       <c r="ED36" s="18"/>
     </row>
     <row r="37" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="84"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="85"/>
       <c r="F37" s="62" t="s">
         <v>32</v>
       </c>
@@ -6505,10 +6506,10 @@
       <c r="CB37" s="17"/>
       <c r="CC37" s="17"/>
       <c r="CD37" s="17"/>
-      <c r="CE37" s="17"/>
-      <c r="CF37" s="17"/>
-      <c r="CG37" s="17"/>
-      <c r="CH37" s="18"/>
+      <c r="CE37" s="19"/>
+      <c r="CF37" s="19"/>
+      <c r="CG37" s="19"/>
+      <c r="CH37" s="30"/>
       <c r="CI37" s="17"/>
       <c r="CJ37" s="17"/>
       <c r="CK37" s="17"/>
@@ -6559,11 +6560,11 @@
       <c r="ED37" s="18"/>
     </row>
     <row r="38" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="86"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="87"/>
       <c r="F38" s="61"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -6641,10 +6642,10 @@
       <c r="CB38" s="17"/>
       <c r="CC38" s="17"/>
       <c r="CD38" s="17"/>
-      <c r="CE38" s="17"/>
-      <c r="CF38" s="17"/>
-      <c r="CG38" s="17"/>
-      <c r="CH38" s="18"/>
+      <c r="CE38" s="19"/>
+      <c r="CF38" s="19"/>
+      <c r="CG38" s="19"/>
+      <c r="CH38" s="30"/>
       <c r="CI38" s="17"/>
       <c r="CJ38" s="17"/>
       <c r="CK38" s="17"/>
@@ -6696,14 +6697,14 @@
     </row>
     <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
-      <c r="B39" s="96"/>
-      <c r="C39" s="87" t="s">
+      <c r="B39" s="97"/>
+      <c r="C39" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="97" t="s">
+      <c r="D39" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="91"/>
+      <c r="E39" s="92"/>
       <c r="F39" s="60" t="s">
         <v>31</v>
       </c>
@@ -6838,10 +6839,10 @@
     </row>
     <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="88"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="93"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="94"/>
       <c r="F40" s="61"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -6974,10 +6975,10 @@
     </row>
     <row r="41" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="88"/>
-      <c r="D41" s="98"/>
-      <c r="E41" s="93"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="99"/>
+      <c r="E41" s="94"/>
       <c r="F41" s="62" t="s">
         <v>32</v>
       </c>
@@ -7058,9 +7059,9 @@
       <c r="CC41" s="27"/>
       <c r="CD41" s="27"/>
       <c r="CE41" s="27"/>
-      <c r="CF41" s="27"/>
-      <c r="CG41" s="27"/>
-      <c r="CH41" s="28"/>
+      <c r="CF41" s="19"/>
+      <c r="CG41" s="19"/>
+      <c r="CH41" s="30"/>
       <c r="CI41" s="27"/>
       <c r="CJ41" s="27"/>
       <c r="CK41" s="27"/>
@@ -7112,10 +7113,10 @@
     </row>
     <row r="42" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="95"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
       <c r="F42" s="61"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -7194,9 +7195,9 @@
       <c r="CC42" s="27"/>
       <c r="CD42" s="27"/>
       <c r="CE42" s="27"/>
-      <c r="CF42" s="27"/>
-      <c r="CG42" s="27"/>
-      <c r="CH42" s="28"/>
+      <c r="CF42" s="19"/>
+      <c r="CG42" s="19"/>
+      <c r="CH42" s="30"/>
       <c r="CI42" s="27"/>
       <c r="CJ42" s="27"/>
       <c r="CK42" s="27"/>
@@ -7248,14 +7249,14 @@
     </row>
     <row r="43" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
-      <c r="B43" s="96"/>
-      <c r="C43" s="78" t="s">
+      <c r="B43" s="97"/>
+      <c r="C43" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="D43" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="82"/>
+      <c r="E43" s="83"/>
       <c r="F43" s="60" t="s">
         <v>31</v>
       </c>
@@ -7390,10 +7391,10 @@
     </row>
     <row r="44" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="83"/>
-      <c r="E44" s="84"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="85"/>
       <c r="F44" s="61"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -7526,10 +7527,10 @@
     </row>
     <row r="45" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="84"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="85"/>
       <c r="F45" s="62" t="s">
         <v>32</v>
       </c>
@@ -7664,10 +7665,10 @@
     </row>
     <row r="46" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
-      <c r="B46" s="96"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="85"/>
-      <c r="E46" s="86"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="87"/>
       <c r="F46" s="61"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -7800,14 +7801,14 @@
     </row>
     <row r="47" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="87" t="s">
+      <c r="B47" s="97"/>
+      <c r="C47" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="97" t="s">
+      <c r="D47" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="91"/>
+      <c r="E47" s="92"/>
       <c r="F47" s="60" t="s">
         <v>31</v>
       </c>
@@ -7942,10 +7943,10 @@
     </row>
     <row r="48" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="93"/>
+      <c r="B48" s="97"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="94"/>
       <c r="F48" s="61"/>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -8078,10 +8079,10 @@
     </row>
     <row r="49" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="93"/>
+      <c r="B49" s="97"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="94"/>
       <c r="F49" s="62" t="s">
         <v>32</v>
       </c>
@@ -8216,10 +8217,10 @@
     </row>
     <row r="50" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="94"/>
-      <c r="E50" s="95"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="96"/>
       <c r="F50" s="61"/>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -8352,14 +8353,14 @@
     </row>
     <row r="51" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
-      <c r="B51" s="96"/>
+      <c r="B51" s="97"/>
       <c r="C51" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="81" t="s">
+      <c r="D51" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="82"/>
+      <c r="E51" s="83"/>
       <c r="F51" s="60" t="s">
         <v>31</v>
       </c>
@@ -8494,10 +8495,10 @@
     </row>
     <row r="52" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
-      <c r="B52" s="96"/>
+      <c r="B52" s="97"/>
       <c r="C52" s="53"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="85"/>
       <c r="F52" s="61"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
@@ -8630,10 +8631,10 @@
     </row>
     <row r="53" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
-      <c r="B53" s="96"/>
+      <c r="B53" s="97"/>
       <c r="C53" s="53"/>
-      <c r="D53" s="83"/>
-      <c r="E53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="85"/>
       <c r="F53" s="62" t="s">
         <v>32</v>
       </c>
@@ -8768,10 +8769,10 @@
     </row>
     <row r="54" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
-      <c r="B54" s="96"/>
+      <c r="B54" s="97"/>
       <c r="C54" s="54"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="86"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="87"/>
       <c r="F54" s="61"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -8904,14 +8905,14 @@
     </row>
     <row r="55" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
-      <c r="B55" s="96"/>
+      <c r="B55" s="97"/>
       <c r="C55" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="97" t="s">
+      <c r="D55" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="91"/>
+      <c r="E55" s="92"/>
       <c r="F55" s="60" t="s">
         <v>31</v>
       </c>
@@ -9046,10 +9047,10 @@
     </row>
     <row r="56" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
-      <c r="B56" s="96"/>
+      <c r="B56" s="97"/>
       <c r="C56" s="56"/>
-      <c r="D56" s="98"/>
-      <c r="E56" s="93"/>
+      <c r="D56" s="99"/>
+      <c r="E56" s="94"/>
       <c r="F56" s="61"/>
       <c r="G56" s="26"/>
       <c r="H56" s="27"/>
@@ -9182,10 +9183,10 @@
     </row>
     <row r="57" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
-      <c r="B57" s="96"/>
+      <c r="B57" s="97"/>
       <c r="C57" s="56"/>
-      <c r="D57" s="98"/>
-      <c r="E57" s="93"/>
+      <c r="D57" s="99"/>
+      <c r="E57" s="94"/>
       <c r="F57" s="62" t="s">
         <v>32</v>
       </c>
@@ -9320,10 +9321,10 @@
     </row>
     <row r="58" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
-      <c r="B58" s="96"/>
+      <c r="B58" s="97"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="94"/>
-      <c r="E58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="96"/>
       <c r="F58" s="61"/>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -9456,14 +9457,14 @@
     </row>
     <row r="59" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A59" s="51"/>
-      <c r="B59" s="96"/>
+      <c r="B59" s="97"/>
       <c r="C59" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="81" t="s">
+      <c r="D59" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="82"/>
+      <c r="E59" s="83"/>
       <c r="F59" s="60" t="s">
         <v>31</v>
       </c>
@@ -9598,10 +9599,10 @@
     </row>
     <row r="60" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A60" s="51"/>
-      <c r="B60" s="96"/>
+      <c r="B60" s="97"/>
       <c r="C60" s="53"/>
-      <c r="D60" s="83"/>
-      <c r="E60" s="84"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="85"/>
       <c r="F60" s="61"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -9734,10 +9735,10 @@
     </row>
     <row r="61" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
-      <c r="B61" s="96"/>
+      <c r="B61" s="97"/>
       <c r="C61" s="53"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="85"/>
       <c r="F61" s="62" t="s">
         <v>32</v>
       </c>
@@ -9872,10 +9873,10 @@
     </row>
     <row r="62" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
-      <c r="B62" s="96"/>
+      <c r="B62" s="97"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="87"/>
       <c r="F62" s="61"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -10008,10 +10009,10 @@
     </row>
     <row r="63" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="87"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="91"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="88"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="92"/>
       <c r="F63" s="60" t="s">
         <v>31</v>
       </c>
@@ -10146,10 +10147,10 @@
     </row>
     <row r="64" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="93"/>
+      <c r="B64" s="97"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="94"/>
       <c r="F64" s="61"/>
       <c r="G64" s="26"/>
       <c r="H64" s="27"/>
@@ -10282,10 +10283,10 @@
     </row>
     <row r="65" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="88"/>
-      <c r="D65" s="98"/>
-      <c r="E65" s="93"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="99"/>
+      <c r="E65" s="94"/>
       <c r="F65" s="62" t="s">
         <v>32</v>
       </c>
@@ -10420,10 +10421,10 @@
     </row>
     <row r="66" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="89"/>
-      <c r="D66" s="94"/>
-      <c r="E66" s="95"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="90"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="96"/>
       <c r="F66" s="61"/>
       <c r="G66" s="26"/>
       <c r="H66" s="27"/>
@@ -10556,10 +10557,10 @@
     </row>
     <row r="67" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A67" s="51"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="81"/>
-      <c r="E67" s="82"/>
+      <c r="B67" s="97"/>
+      <c r="C67" s="79"/>
+      <c r="D67" s="82"/>
+      <c r="E67" s="83"/>
       <c r="F67" s="60" t="s">
         <v>31</v>
       </c>
@@ -10694,10 +10695,10 @@
     </row>
     <row r="68" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A68" s="51"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="79"/>
-      <c r="D68" s="83"/>
-      <c r="E68" s="84"/>
+      <c r="B68" s="97"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="85"/>
       <c r="F68" s="61"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -10830,10 +10831,10 @@
     </row>
     <row r="69" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A69" s="51"/>
-      <c r="B69" s="96"/>
-      <c r="C69" s="79"/>
-      <c r="D69" s="83"/>
-      <c r="E69" s="84"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="85"/>
       <c r="F69" s="62" t="s">
         <v>32</v>
       </c>
@@ -10968,10 +10969,10 @@
     </row>
     <row r="70" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A70" s="51"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="85"/>
-      <c r="E70" s="86"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="86"/>
+      <c r="E70" s="87"/>
       <c r="F70" s="61"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -11104,10 +11105,10 @@
     </row>
     <row r="71" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A71" s="51"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="87"/>
-      <c r="D71" s="97"/>
-      <c r="E71" s="91"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="88"/>
+      <c r="D71" s="98"/>
+      <c r="E71" s="92"/>
       <c r="F71" s="60" t="s">
         <v>31</v>
       </c>
@@ -11242,10 +11243,10 @@
     </row>
     <row r="72" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A72" s="51"/>
-      <c r="B72" s="96"/>
-      <c r="C72" s="88"/>
-      <c r="D72" s="98"/>
-      <c r="E72" s="93"/>
+      <c r="B72" s="97"/>
+      <c r="C72" s="89"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="94"/>
       <c r="F72" s="61"/>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
@@ -11378,10 +11379,10 @@
     </row>
     <row r="73" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
-      <c r="B73" s="96"/>
-      <c r="C73" s="88"/>
-      <c r="D73" s="98"/>
-      <c r="E73" s="93"/>
+      <c r="B73" s="97"/>
+      <c r="C73" s="89"/>
+      <c r="D73" s="99"/>
+      <c r="E73" s="94"/>
       <c r="F73" s="62" t="s">
         <v>32</v>
       </c>
@@ -11516,10 +11517,10 @@
     </row>
     <row r="74" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A74" s="51"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="89"/>
-      <c r="D74" s="94"/>
-      <c r="E74" s="95"/>
+      <c r="B74" s="97"/>
+      <c r="C74" s="90"/>
+      <c r="D74" s="95"/>
+      <c r="E74" s="96"/>
       <c r="F74" s="61"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -11652,10 +11653,10 @@
     </row>
     <row r="75" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A75" s="51"/>
-      <c r="B75" s="96"/>
-      <c r="C75" s="78"/>
-      <c r="D75" s="81"/>
-      <c r="E75" s="82"/>
+      <c r="B75" s="97"/>
+      <c r="C75" s="79"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="83"/>
       <c r="F75" s="60" t="s">
         <v>31</v>
       </c>
@@ -11790,10 +11791,10 @@
     </row>
     <row r="76" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A76" s="51"/>
-      <c r="B76" s="96"/>
-      <c r="C76" s="79"/>
-      <c r="D76" s="83"/>
-      <c r="E76" s="84"/>
+      <c r="B76" s="97"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="85"/>
       <c r="F76" s="61"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -11926,10 +11927,10 @@
     </row>
     <row r="77" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A77" s="51"/>
-      <c r="B77" s="96"/>
-      <c r="C77" s="79"/>
-      <c r="D77" s="83"/>
-      <c r="E77" s="84"/>
+      <c r="B77" s="97"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="85"/>
       <c r="F77" s="62" t="s">
         <v>32</v>
       </c>
@@ -12064,10 +12065,10 @@
     </row>
     <row r="78" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
-      <c r="B78" s="96"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="85"/>
-      <c r="E78" s="86"/>
+      <c r="B78" s="97"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="87"/>
       <c r="F78" s="61"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -12199,19 +12200,19 @@
       <c r="ED78" s="18"/>
     </row>
     <row r="79" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A79" s="76">
+      <c r="A79" s="77">
         <v>11</v>
       </c>
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="87" t="s">
+      <c r="C79" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="97" t="s">
+      <c r="D79" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="91"/>
+      <c r="E79" s="92"/>
       <c r="F79" s="60" t="s">
         <v>31</v>
       </c>
@@ -12345,11 +12346,11 @@
       <c r="ED79" s="25"/>
     </row>
     <row r="80" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A80" s="76"/>
-      <c r="B80" s="77"/>
-      <c r="C80" s="88"/>
-      <c r="D80" s="98"/>
-      <c r="E80" s="93"/>
+      <c r="A80" s="77"/>
+      <c r="B80" s="78"/>
+      <c r="C80" s="89"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="94"/>
       <c r="F80" s="61"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12481,11 +12482,11 @@
       <c r="ED80" s="28"/>
     </row>
     <row r="81" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A81" s="76"/>
-      <c r="B81" s="77"/>
-      <c r="C81" s="88"/>
-      <c r="D81" s="98"/>
-      <c r="E81" s="93"/>
+      <c r="A81" s="77"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="89"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="94"/>
       <c r="F81" s="62" t="s">
         <v>32</v>
       </c>
@@ -12619,11 +12620,11 @@
       <c r="ED81" s="28"/>
     </row>
     <row r="82" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A82" s="76"/>
-      <c r="B82" s="77"/>
-      <c r="C82" s="89"/>
-      <c r="D82" s="94"/>
-      <c r="E82" s="95"/>
+      <c r="A82" s="77"/>
+      <c r="B82" s="78"/>
+      <c r="C82" s="90"/>
+      <c r="D82" s="95"/>
+      <c r="E82" s="96"/>
       <c r="F82" s="61"/>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
@@ -12756,14 +12757,14 @@
     </row>
     <row r="83" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A83" s="51"/>
-      <c r="B83" s="77"/>
-      <c r="C83" s="78" t="s">
+      <c r="B83" s="78"/>
+      <c r="C83" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="81" t="s">
+      <c r="D83" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E83" s="82"/>
+      <c r="E83" s="83"/>
       <c r="F83" s="60" t="s">
         <v>31</v>
       </c>
@@ -12898,10 +12899,10 @@
     </row>
     <row r="84" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A84" s="51"/>
-      <c r="B84" s="77"/>
-      <c r="C84" s="79"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="84"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="85"/>
       <c r="F84" s="61"/>
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
@@ -13034,10 +13035,10 @@
     </row>
     <row r="85" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A85" s="51"/>
-      <c r="B85" s="77"/>
-      <c r="C85" s="79"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="84"/>
+      <c r="B85" s="78"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="85"/>
       <c r="F85" s="62" t="s">
         <v>32</v>
       </c>
@@ -13172,10 +13173,10 @@
     </row>
     <row r="86" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A86" s="51"/>
-      <c r="B86" s="77"/>
-      <c r="C86" s="80"/>
-      <c r="D86" s="85"/>
-      <c r="E86" s="86"/>
+      <c r="B86" s="78"/>
+      <c r="C86" s="81"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="87"/>
       <c r="F86" s="61"/>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -13308,14 +13309,14 @@
     </row>
     <row r="87" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A87" s="51"/>
-      <c r="B87" s="77"/>
-      <c r="C87" s="87" t="s">
+      <c r="B87" s="78"/>
+      <c r="C87" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D87" s="97" t="s">
+      <c r="D87" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="91"/>
+      <c r="E87" s="92"/>
       <c r="F87" s="60" t="s">
         <v>31</v>
       </c>
@@ -13450,10 +13451,10 @@
     </row>
     <row r="88" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A88" s="51"/>
-      <c r="B88" s="77"/>
-      <c r="C88" s="88"/>
-      <c r="D88" s="98"/>
-      <c r="E88" s="93"/>
+      <c r="B88" s="78"/>
+      <c r="C88" s="89"/>
+      <c r="D88" s="99"/>
+      <c r="E88" s="94"/>
       <c r="F88" s="61"/>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -13586,10 +13587,10 @@
     </row>
     <row r="89" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A89" s="51"/>
-      <c r="B89" s="77"/>
-      <c r="C89" s="88"/>
-      <c r="D89" s="98"/>
-      <c r="E89" s="93"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="89"/>
+      <c r="D89" s="99"/>
+      <c r="E89" s="94"/>
       <c r="F89" s="62" t="s">
         <v>32</v>
       </c>
@@ -13724,10 +13725,10 @@
     </row>
     <row r="90" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
-      <c r="B90" s="77"/>
-      <c r="C90" s="89"/>
-      <c r="D90" s="94"/>
-      <c r="E90" s="95"/>
+      <c r="B90" s="78"/>
+      <c r="C90" s="90"/>
+      <c r="D90" s="95"/>
+      <c r="E90" s="96"/>
       <c r="F90" s="61"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -13859,17 +13860,17 @@
       <c r="ED90" s="28"/>
     </row>
     <row r="91" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A91" s="76">
+      <c r="A91" s="77">
         <v>13</v>
       </c>
-      <c r="B91" s="77"/>
-      <c r="C91" s="78" t="s">
+      <c r="B91" s="78"/>
+      <c r="C91" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="81" t="s">
+      <c r="D91" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E91" s="82"/>
+      <c r="E91" s="83"/>
       <c r="F91" s="60" t="s">
         <v>31</v>
       </c>
@@ -14003,11 +14004,11 @@
       <c r="ED91" s="12"/>
     </row>
     <row r="92" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A92" s="76"/>
-      <c r="B92" s="77"/>
-      <c r="C92" s="79"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="84"/>
+      <c r="A92" s="77"/>
+      <c r="B92" s="78"/>
+      <c r="C92" s="80"/>
+      <c r="D92" s="84"/>
+      <c r="E92" s="85"/>
       <c r="F92" s="61"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -14139,11 +14140,11 @@
       <c r="ED92" s="18"/>
     </row>
     <row r="93" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A93" s="76"/>
-      <c r="B93" s="77"/>
-      <c r="C93" s="79"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="84"/>
+      <c r="A93" s="77"/>
+      <c r="B93" s="78"/>
+      <c r="C93" s="80"/>
+      <c r="D93" s="84"/>
+      <c r="E93" s="85"/>
       <c r="F93" s="62" t="s">
         <v>32</v>
       </c>
@@ -14277,11 +14278,11 @@
       <c r="ED93" s="18"/>
     </row>
     <row r="94" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A94" s="76"/>
-      <c r="B94" s="77"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="85"/>
-      <c r="E94" s="86"/>
+      <c r="A94" s="77"/>
+      <c r="B94" s="78"/>
+      <c r="C94" s="81"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="87"/>
       <c r="F94" s="61"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17"/>
@@ -14413,19 +14414,19 @@
       <c r="ED94" s="18"/>
     </row>
     <row r="95" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A95" s="76">
+      <c r="A95" s="77">
         <v>14</v>
       </c>
-      <c r="B95" s="96" t="s">
+      <c r="B95" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="87" t="s">
+      <c r="C95" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="90" t="s">
+      <c r="D95" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="91"/>
+      <c r="E95" s="92"/>
       <c r="F95" s="60" t="s">
         <v>31</v>
       </c>
@@ -14559,11 +14560,11 @@
       <c r="ED95" s="25"/>
     </row>
     <row r="96" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A96" s="76"/>
-      <c r="B96" s="96"/>
-      <c r="C96" s="88"/>
-      <c r="D96" s="92"/>
-      <c r="E96" s="93"/>
+      <c r="A96" s="77"/>
+      <c r="B96" s="97"/>
+      <c r="C96" s="89"/>
+      <c r="D96" s="93"/>
+      <c r="E96" s="94"/>
       <c r="F96" s="61"/>
       <c r="G96" s="26"/>
       <c r="H96" s="27"/>
@@ -14695,11 +14696,11 @@
       <c r="ED96" s="28"/>
     </row>
     <row r="97" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A97" s="76"/>
-      <c r="B97" s="96"/>
-      <c r="C97" s="88"/>
-      <c r="D97" s="92"/>
-      <c r="E97" s="93"/>
+      <c r="A97" s="77"/>
+      <c r="B97" s="97"/>
+      <c r="C97" s="89"/>
+      <c r="D97" s="93"/>
+      <c r="E97" s="94"/>
       <c r="F97" s="62" t="s">
         <v>32</v>
       </c>
@@ -14833,11 +14834,11 @@
       <c r="ED97" s="28"/>
     </row>
     <row r="98" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A98" s="76"/>
-      <c r="B98" s="96"/>
-      <c r="C98" s="89"/>
-      <c r="D98" s="94"/>
-      <c r="E98" s="95"/>
+      <c r="A98" s="77"/>
+      <c r="B98" s="97"/>
+      <c r="C98" s="90"/>
+      <c r="D98" s="95"/>
+      <c r="E98" s="96"/>
       <c r="F98" s="61"/>
       <c r="G98" s="26"/>
       <c r="H98" s="27"/>
@@ -14969,17 +14970,17 @@
       <c r="ED98" s="28"/>
     </row>
     <row r="99" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A99" s="76">
+      <c r="A99" s="77">
         <v>15</v>
       </c>
-      <c r="B99" s="96"/>
-      <c r="C99" s="78" t="s">
+      <c r="B99" s="97"/>
+      <c r="C99" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="81" t="s">
+      <c r="D99" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E99" s="82"/>
+      <c r="E99" s="83"/>
       <c r="F99" s="60" t="s">
         <v>31</v>
       </c>
@@ -15113,11 +15114,11 @@
       <c r="ED99" s="12"/>
     </row>
     <row r="100" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A100" s="76"/>
-      <c r="B100" s="96"/>
-      <c r="C100" s="79"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="84"/>
+      <c r="A100" s="77"/>
+      <c r="B100" s="97"/>
+      <c r="C100" s="80"/>
+      <c r="D100" s="84"/>
+      <c r="E100" s="85"/>
       <c r="F100" s="61"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -15249,11 +15250,11 @@
       <c r="ED100" s="18"/>
     </row>
     <row r="101" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A101" s="76"/>
-      <c r="B101" s="96"/>
-      <c r="C101" s="79"/>
-      <c r="D101" s="83"/>
-      <c r="E101" s="84"/>
+      <c r="A101" s="77"/>
+      <c r="B101" s="97"/>
+      <c r="C101" s="80"/>
+      <c r="D101" s="84"/>
+      <c r="E101" s="85"/>
       <c r="F101" s="62" t="s">
         <v>32</v>
       </c>
@@ -15387,11 +15388,11 @@
       <c r="ED101" s="18"/>
     </row>
     <row r="102" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A102" s="76"/>
-      <c r="B102" s="96"/>
-      <c r="C102" s="80"/>
-      <c r="D102" s="85"/>
-      <c r="E102" s="86"/>
+      <c r="A102" s="77"/>
+      <c r="B102" s="97"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="86"/>
+      <c r="E102" s="87"/>
       <c r="F102" s="61"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -15523,17 +15524,17 @@
       <c r="ED102" s="18"/>
     </row>
     <row r="103" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A103" s="76">
+      <c r="A103" s="77">
         <v>16</v>
       </c>
-      <c r="B103" s="96"/>
-      <c r="C103" s="87" t="s">
+      <c r="B103" s="97"/>
+      <c r="C103" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="90" t="s">
+      <c r="D103" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="91"/>
+      <c r="E103" s="92"/>
       <c r="F103" s="60" t="s">
         <v>31</v>
       </c>
@@ -15667,11 +15668,11 @@
       <c r="ED103" s="25"/>
     </row>
     <row r="104" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A104" s="76"/>
-      <c r="B104" s="96"/>
-      <c r="C104" s="88"/>
-      <c r="D104" s="92"/>
-      <c r="E104" s="93"/>
+      <c r="A104" s="77"/>
+      <c r="B104" s="97"/>
+      <c r="C104" s="89"/>
+      <c r="D104" s="93"/>
+      <c r="E104" s="94"/>
       <c r="F104" s="61"/>
       <c r="G104" s="26"/>
       <c r="H104" s="27"/>
@@ -15803,11 +15804,11 @@
       <c r="ED104" s="28"/>
     </row>
     <row r="105" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A105" s="76"/>
-      <c r="B105" s="96"/>
-      <c r="C105" s="88"/>
-      <c r="D105" s="92"/>
-      <c r="E105" s="93"/>
+      <c r="A105" s="77"/>
+      <c r="B105" s="97"/>
+      <c r="C105" s="89"/>
+      <c r="D105" s="93"/>
+      <c r="E105" s="94"/>
       <c r="F105" s="62" t="s">
         <v>32</v>
       </c>
@@ -15941,11 +15942,11 @@
       <c r="ED105" s="28"/>
     </row>
     <row r="106" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A106" s="76"/>
-      <c r="B106" s="96"/>
-      <c r="C106" s="89"/>
-      <c r="D106" s="94"/>
-      <c r="E106" s="95"/>
+      <c r="A106" s="77"/>
+      <c r="B106" s="97"/>
+      <c r="C106" s="90"/>
+      <c r="D106" s="95"/>
+      <c r="E106" s="96"/>
       <c r="F106" s="61"/>
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
@@ -16077,13 +16078,13 @@
       <c r="ED106" s="28"/>
     </row>
     <row r="107" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A107" s="99"/>
+      <c r="A107" s="100"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="100" t="s">
+      <c r="C107" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="102"/>
-      <c r="E107" s="103"/>
+      <c r="D107" s="103"/>
+      <c r="E107" s="104"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
       <c r="H107" s="44"/>
@@ -16217,11 +16218,11 @@
       <c r="ED107" s="45"/>
     </row>
     <row r="108" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A108" s="99"/>
+      <c r="A108" s="100"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="101"/>
-      <c r="D108" s="104"/>
-      <c r="E108" s="105"/>
+      <c r="C108" s="102"/>
+      <c r="D108" s="105"/>
+      <c r="E108" s="106"/>
       <c r="F108" s="46"/>
       <c r="G108" s="47"/>
       <c r="H108" s="48"/>

</xml_diff>

<commit_message>
Text is now required. Added theme colour
</commit_message>
<xml_diff>
--- a/documentation/Gantt.xlsx
+++ b/documentation/Gantt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\zraisb\WebstormProjects\Resonance-Web\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\WebstormProjects\Resonance-Web\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12888"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -675,32 +675,65 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -729,68 +762,35 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
-    <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1132,28 +1132,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ED108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BT48" sqref="BT48"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="CI105" sqref="CI105:CL106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="126" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="126" width="2.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="106" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
@@ -1164,168 +1164,168 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="70">
+      <c r="G1" s="100">
         <v>42803</v>
       </c>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="70">
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="100">
         <v>42804</v>
       </c>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="70">
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="100">
         <v>42809</v>
       </c>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
-      <c r="AB1" s="71"/>
-      <c r="AC1" s="71"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="70">
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="103"/>
+      <c r="AD1" s="104"/>
+      <c r="AE1" s="100">
         <v>42810</v>
       </c>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="71"/>
-      <c r="AH1" s="71"/>
-      <c r="AI1" s="71"/>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="70">
+      <c r="AF1" s="103"/>
+      <c r="AG1" s="103"/>
+      <c r="AH1" s="103"/>
+      <c r="AI1" s="103"/>
+      <c r="AJ1" s="103"/>
+      <c r="AK1" s="103"/>
+      <c r="AL1" s="104"/>
+      <c r="AM1" s="100">
         <v>42811</v>
       </c>
-      <c r="AN1" s="71"/>
-      <c r="AO1" s="71"/>
-      <c r="AP1" s="71"/>
-      <c r="AQ1" s="71"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="71"/>
-      <c r="AT1" s="72"/>
-      <c r="AU1" s="70">
+      <c r="AN1" s="103"/>
+      <c r="AO1" s="103"/>
+      <c r="AP1" s="103"/>
+      <c r="AQ1" s="103"/>
+      <c r="AR1" s="103"/>
+      <c r="AS1" s="103"/>
+      <c r="AT1" s="104"/>
+      <c r="AU1" s="100">
         <v>42816</v>
       </c>
-      <c r="AV1" s="71"/>
-      <c r="AW1" s="71"/>
-      <c r="AX1" s="71"/>
-      <c r="AY1" s="71"/>
-      <c r="AZ1" s="71"/>
-      <c r="BA1" s="71"/>
-      <c r="BB1" s="72"/>
-      <c r="BC1" s="70">
+      <c r="AV1" s="103"/>
+      <c r="AW1" s="103"/>
+      <c r="AX1" s="103"/>
+      <c r="AY1" s="103"/>
+      <c r="AZ1" s="103"/>
+      <c r="BA1" s="103"/>
+      <c r="BB1" s="104"/>
+      <c r="BC1" s="100">
         <v>42817</v>
       </c>
-      <c r="BD1" s="71"/>
-      <c r="BE1" s="71"/>
-      <c r="BF1" s="71"/>
-      <c r="BG1" s="71"/>
-      <c r="BH1" s="71"/>
-      <c r="BI1" s="71"/>
-      <c r="BJ1" s="72"/>
-      <c r="BK1" s="70">
+      <c r="BD1" s="103"/>
+      <c r="BE1" s="103"/>
+      <c r="BF1" s="103"/>
+      <c r="BG1" s="103"/>
+      <c r="BH1" s="103"/>
+      <c r="BI1" s="103"/>
+      <c r="BJ1" s="104"/>
+      <c r="BK1" s="100">
         <v>42818</v>
       </c>
-      <c r="BL1" s="71"/>
-      <c r="BM1" s="71"/>
-      <c r="BN1" s="71"/>
-      <c r="BO1" s="71"/>
-      <c r="BP1" s="71"/>
-      <c r="BQ1" s="71"/>
-      <c r="BR1" s="72"/>
-      <c r="BS1" s="70">
+      <c r="BL1" s="103"/>
+      <c r="BM1" s="103"/>
+      <c r="BN1" s="103"/>
+      <c r="BO1" s="103"/>
+      <c r="BP1" s="103"/>
+      <c r="BQ1" s="103"/>
+      <c r="BR1" s="104"/>
+      <c r="BS1" s="100">
         <v>42823</v>
       </c>
-      <c r="BT1" s="71"/>
-      <c r="BU1" s="71"/>
-      <c r="BV1" s="71"/>
-      <c r="BW1" s="71"/>
-      <c r="BX1" s="71"/>
-      <c r="BY1" s="71"/>
-      <c r="BZ1" s="72"/>
-      <c r="CA1" s="70">
+      <c r="BT1" s="103"/>
+      <c r="BU1" s="103"/>
+      <c r="BV1" s="103"/>
+      <c r="BW1" s="103"/>
+      <c r="BX1" s="103"/>
+      <c r="BY1" s="103"/>
+      <c r="BZ1" s="104"/>
+      <c r="CA1" s="100">
         <v>42824</v>
       </c>
-      <c r="CB1" s="75"/>
-      <c r="CC1" s="75"/>
-      <c r="CD1" s="75"/>
-      <c r="CE1" s="75"/>
-      <c r="CF1" s="75"/>
-      <c r="CG1" s="75"/>
-      <c r="CH1" s="76"/>
-      <c r="CI1" s="70">
+      <c r="CB1" s="101"/>
+      <c r="CC1" s="101"/>
+      <c r="CD1" s="101"/>
+      <c r="CE1" s="101"/>
+      <c r="CF1" s="101"/>
+      <c r="CG1" s="101"/>
+      <c r="CH1" s="102"/>
+      <c r="CI1" s="100">
         <v>42825</v>
       </c>
-      <c r="CJ1" s="75"/>
-      <c r="CK1" s="75"/>
-      <c r="CL1" s="75"/>
-      <c r="CM1" s="75"/>
-      <c r="CN1" s="75"/>
-      <c r="CO1" s="75"/>
-      <c r="CP1" s="76"/>
-      <c r="CQ1" s="70">
+      <c r="CJ1" s="101"/>
+      <c r="CK1" s="101"/>
+      <c r="CL1" s="101"/>
+      <c r="CM1" s="101"/>
+      <c r="CN1" s="101"/>
+      <c r="CO1" s="101"/>
+      <c r="CP1" s="102"/>
+      <c r="CQ1" s="100">
         <v>42826</v>
       </c>
-      <c r="CR1" s="75"/>
-      <c r="CS1" s="75"/>
-      <c r="CT1" s="75"/>
-      <c r="CU1" s="75"/>
-      <c r="CV1" s="75"/>
-      <c r="CW1" s="75"/>
-      <c r="CX1" s="76"/>
-      <c r="CY1" s="70">
+      <c r="CR1" s="101"/>
+      <c r="CS1" s="101"/>
+      <c r="CT1" s="101"/>
+      <c r="CU1" s="101"/>
+      <c r="CV1" s="101"/>
+      <c r="CW1" s="101"/>
+      <c r="CX1" s="102"/>
+      <c r="CY1" s="100">
         <v>42830</v>
       </c>
-      <c r="CZ1" s="75"/>
-      <c r="DA1" s="75"/>
-      <c r="DB1" s="75"/>
-      <c r="DC1" s="75"/>
-      <c r="DD1" s="75"/>
-      <c r="DE1" s="75"/>
-      <c r="DF1" s="76"/>
-      <c r="DG1" s="70">
+      <c r="CZ1" s="101"/>
+      <c r="DA1" s="101"/>
+      <c r="DB1" s="101"/>
+      <c r="DC1" s="101"/>
+      <c r="DD1" s="101"/>
+      <c r="DE1" s="101"/>
+      <c r="DF1" s="102"/>
+      <c r="DG1" s="100">
         <v>42831</v>
       </c>
-      <c r="DH1" s="75"/>
-      <c r="DI1" s="75"/>
-      <c r="DJ1" s="75"/>
-      <c r="DK1" s="75"/>
-      <c r="DL1" s="75"/>
-      <c r="DM1" s="75"/>
-      <c r="DN1" s="76"/>
-      <c r="DO1" s="70">
+      <c r="DH1" s="101"/>
+      <c r="DI1" s="101"/>
+      <c r="DJ1" s="101"/>
+      <c r="DK1" s="101"/>
+      <c r="DL1" s="101"/>
+      <c r="DM1" s="101"/>
+      <c r="DN1" s="102"/>
+      <c r="DO1" s="100">
         <v>42832</v>
       </c>
-      <c r="DP1" s="75"/>
-      <c r="DQ1" s="75"/>
-      <c r="DR1" s="75"/>
-      <c r="DS1" s="75"/>
-      <c r="DT1" s="75"/>
-      <c r="DU1" s="75"/>
-      <c r="DV1" s="76"/>
-      <c r="DW1" s="70"/>
-      <c r="DX1" s="75"/>
-      <c r="DY1" s="75"/>
-      <c r="DZ1" s="75"/>
-      <c r="EA1" s="75"/>
-      <c r="EB1" s="75"/>
-      <c r="EC1" s="75"/>
-      <c r="ED1" s="76"/>
+      <c r="DP1" s="101"/>
+      <c r="DQ1" s="101"/>
+      <c r="DR1" s="101"/>
+      <c r="DS1" s="101"/>
+      <c r="DT1" s="101"/>
+      <c r="DU1" s="101"/>
+      <c r="DV1" s="102"/>
+      <c r="DW1" s="100"/>
+      <c r="DX1" s="101"/>
+      <c r="DY1" s="101"/>
+      <c r="DZ1" s="101"/>
+      <c r="EA1" s="101"/>
+      <c r="EB1" s="101"/>
+      <c r="EC1" s="101"/>
+      <c r="ED1" s="102"/>
     </row>
-    <row r="2" spans="1:134" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74"/>
+    <row r="2" spans="1:134" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="105"/>
+      <c r="B2" s="106"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1705,20 +1705,20 @@
       <c r="EC2" s="8"/>
       <c r="ED2" s="9"/>
     </row>
-    <row r="3" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A3" s="77">
+    <row r="3" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A3" s="86">
         <v>1</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="83"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="60" t="s">
         <v>31</v>
       </c>
@@ -1851,12 +1851,12 @@
       <c r="EC3" s="11"/>
       <c r="ED3" s="12"/>
     </row>
-    <row r="4" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A4" s="77"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
+    <row r="4" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A4" s="86"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
       <c r="F4" s="61"/>
       <c r="G4" s="65"/>
       <c r="H4" s="16"/>
@@ -1987,12 +1987,12 @@
       <c r="EC4" s="17"/>
       <c r="ED4" s="18"/>
     </row>
-    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
+    <row r="5" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A5" s="86"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="96"/>
       <c r="F5" s="62" t="s">
         <v>32</v>
       </c>
@@ -2125,12 +2125,12 @@
       <c r="EC5" s="17"/>
       <c r="ED5" s="18"/>
     </row>
-    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A6" s="77"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="87"/>
+    <row r="6" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A6" s="86"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
       <c r="F6" s="61"/>
       <c r="G6" s="67"/>
       <c r="H6" s="22"/>
@@ -2261,18 +2261,18 @@
       <c r="EC6" s="17"/>
       <c r="ED6" s="18"/>
     </row>
-    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A7" s="77">
+    <row r="7" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A7" s="86">
         <v>2</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="88" t="s">
+      <c r="B7" s="99"/>
+      <c r="C7" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="92"/>
+      <c r="E7" s="81"/>
       <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
@@ -2405,12 +2405,12 @@
       <c r="EC7" s="24"/>
       <c r="ED7" s="25"/>
     </row>
-    <row r="8" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
+    <row r="8" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A8" s="86"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="83"/>
       <c r="F8" s="61"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -2541,12 +2541,12 @@
       <c r="EC8" s="27"/>
       <c r="ED8" s="28"/>
     </row>
-    <row r="9" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
+    <row r="9" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A9" s="86"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="83"/>
       <c r="F9" s="62" t="s">
         <v>32</v>
       </c>
@@ -2679,12 +2679,12 @@
       <c r="EC9" s="27"/>
       <c r="ED9" s="28"/>
     </row>
-    <row r="10" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A10" s="77"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="96"/>
+    <row r="10" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A10" s="86"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="61"/>
       <c r="G10" s="26"/>
       <c r="H10" s="27"/>
@@ -2815,18 +2815,18 @@
       <c r="EC10" s="27"/>
       <c r="ED10" s="28"/>
     </row>
-    <row r="11" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A11" s="77">
+    <row r="11" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A11" s="86">
         <v>3</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79" t="s">
+      <c r="B11" s="99"/>
+      <c r="C11" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="83"/>
+      <c r="E11" s="94"/>
       <c r="F11" s="60" t="s">
         <v>31</v>
       </c>
@@ -2959,12 +2959,12 @@
       <c r="EC11" s="11"/>
       <c r="ED11" s="12"/>
     </row>
-    <row r="12" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="85"/>
+    <row r="12" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A12" s="86"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="61"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3095,12 +3095,12 @@
       <c r="EC12" s="17"/>
       <c r="ED12" s="18"/>
     </row>
-    <row r="13" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="85"/>
+    <row r="13" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A13" s="86"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="62" t="s">
         <v>32</v>
       </c>
@@ -3233,12 +3233,12 @@
       <c r="EC13" s="17"/>
       <c r="ED13" s="18"/>
     </row>
-    <row r="14" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="87"/>
+    <row r="14" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A14" s="86"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="61"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3369,18 +3369,18 @@
       <c r="EC14" s="17"/>
       <c r="ED14" s="18"/>
     </row>
-    <row r="15" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A15" s="77">
+    <row r="15" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A15" s="86">
         <v>4</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="88" t="s">
+      <c r="B15" s="99"/>
+      <c r="C15" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="91" t="s">
+      <c r="D15" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="92"/>
+      <c r="E15" s="81"/>
       <c r="F15" s="60" t="s">
         <v>31</v>
       </c>
@@ -3513,12 +3513,12 @@
       <c r="EC15" s="24"/>
       <c r="ED15" s="25"/>
     </row>
-    <row r="16" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A16" s="77"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="94"/>
+    <row r="16" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="61"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -3649,12 +3649,12 @@
       <c r="EC16" s="27"/>
       <c r="ED16" s="28"/>
     </row>
-    <row r="17" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="94"/>
+    <row r="17" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A17" s="86"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="83"/>
       <c r="F17" s="62" t="s">
         <v>32</v>
       </c>
@@ -3787,12 +3787,12 @@
       <c r="EC17" s="27"/>
       <c r="ED17" s="28"/>
     </row>
-    <row r="18" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A18" s="77"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="95"/>
-      <c r="E18" s="96"/>
+    <row r="18" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A18" s="86"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="61"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27"/>
@@ -3923,18 +3923,18 @@
       <c r="EC18" s="27"/>
       <c r="ED18" s="28"/>
     </row>
-    <row r="19" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A19" s="77">
+    <row r="19" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A19" s="86">
         <v>5</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79" t="s">
+      <c r="B19" s="99"/>
+      <c r="C19" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="D19" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="83"/>
+      <c r="E19" s="94"/>
       <c r="F19" s="60" t="s">
         <v>31</v>
       </c>
@@ -4067,12 +4067,12 @@
       <c r="EC19" s="11"/>
       <c r="ED19" s="12"/>
     </row>
-    <row r="20" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A20" s="77"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="85"/>
+    <row r="20" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A20" s="86"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
       <c r="F20" s="61"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -4203,12 +4203,12 @@
       <c r="EC20" s="17"/>
       <c r="ED20" s="18"/>
     </row>
-    <row r="21" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="85"/>
+    <row r="21" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A21" s="86"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
       <c r="F21" s="62" t="s">
         <v>32</v>
       </c>
@@ -4341,12 +4341,12 @@
       <c r="EC21" s="17"/>
       <c r="ED21" s="18"/>
     </row>
-    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A22" s="77"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="87"/>
+    <row r="22" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A22" s="86"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="98"/>
       <c r="F22" s="61"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -4477,20 +4477,20 @@
       <c r="EC22" s="17"/>
       <c r="ED22" s="18"/>
     </row>
-    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A23" s="77">
+    <row r="23" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A23" s="86">
         <v>6</v>
       </c>
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="92"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="60" t="s">
         <v>31</v>
       </c>
@@ -4623,12 +4623,12 @@
       <c r="EC23" s="24"/>
       <c r="ED23" s="25"/>
     </row>
-    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="94"/>
+    <row r="24" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A24" s="86"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="83"/>
       <c r="F24" s="61"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -4759,12 +4759,12 @@
       <c r="EC24" s="27"/>
       <c r="ED24" s="28"/>
     </row>
-    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="94"/>
+    <row r="25" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A25" s="86"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="83"/>
       <c r="F25" s="62" t="s">
         <v>32</v>
       </c>
@@ -4897,12 +4897,12 @@
       <c r="EC25" s="27"/>
       <c r="ED25" s="28"/>
     </row>
-    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="96"/>
+    <row r="26" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A26" s="86"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="85"/>
       <c r="F26" s="61"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
@@ -5033,18 +5033,18 @@
       <c r="EC26" s="27"/>
       <c r="ED26" s="28"/>
     </row>
-    <row r="27" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A27" s="77">
+    <row r="27" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A27" s="86">
         <v>7</v>
       </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="79" t="s">
+      <c r="B27" s="87"/>
+      <c r="C27" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="82" t="s">
+      <c r="D27" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="83"/>
+      <c r="E27" s="94"/>
       <c r="F27" s="60" t="s">
         <v>31</v>
       </c>
@@ -5177,12 +5177,12 @@
       <c r="EC27" s="11"/>
       <c r="ED27" s="12"/>
     </row>
-    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="85"/>
+    <row r="28" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A28" s="86"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="95"/>
+      <c r="E28" s="96"/>
       <c r="F28" s="61"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -5313,12 +5313,12 @@
       <c r="EC28" s="17"/>
       <c r="ED28" s="18"/>
     </row>
-    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
-      <c r="B29" s="97"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="85"/>
+    <row r="29" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A29" s="86"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
       <c r="F29" s="62" t="s">
         <v>32</v>
       </c>
@@ -5451,12 +5451,12 @@
       <c r="EC29" s="17"/>
       <c r="ED29" s="18"/>
     </row>
-    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A30" s="77"/>
-      <c r="B30" s="97"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="87"/>
+    <row r="30" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A30" s="86"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="98"/>
       <c r="F30" s="61"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5587,18 +5587,18 @@
       <c r="EC30" s="17"/>
       <c r="ED30" s="18"/>
     </row>
-    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A31" s="77">
+    <row r="31" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A31" s="86">
         <v>8</v>
       </c>
-      <c r="B31" s="97"/>
-      <c r="C31" s="88" t="s">
+      <c r="B31" s="87"/>
+      <c r="C31" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="92"/>
+      <c r="E31" s="81"/>
       <c r="F31" s="60" t="s">
         <v>31</v>
       </c>
@@ -5731,12 +5731,12 @@
       <c r="EC31" s="24"/>
       <c r="ED31" s="25"/>
     </row>
-    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
-      <c r="B32" s="97"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="94"/>
+    <row r="32" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A32" s="86"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="83"/>
       <c r="F32" s="61"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -5867,12 +5867,12 @@
       <c r="EC32" s="27"/>
       <c r="ED32" s="28"/>
     </row>
-    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
-      <c r="B33" s="97"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="94"/>
+    <row r="33" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A33" s="86"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="83"/>
       <c r="F33" s="62" t="s">
         <v>32</v>
       </c>
@@ -6005,12 +6005,12 @@
       <c r="EC33" s="27"/>
       <c r="ED33" s="28"/>
     </row>
-    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A34" s="77"/>
-      <c r="B34" s="97"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="96"/>
+    <row r="34" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A34" s="86"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="85"/>
       <c r="F34" s="61"/>
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
@@ -6141,18 +6141,18 @@
       <c r="EC34" s="27"/>
       <c r="ED34" s="28"/>
     </row>
-    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A35" s="77">
+    <row r="35" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A35" s="86">
         <v>9</v>
       </c>
-      <c r="B35" s="97"/>
-      <c r="C35" s="79" t="s">
+      <c r="B35" s="87"/>
+      <c r="C35" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="83"/>
+      <c r="E35" s="94"/>
       <c r="F35" s="60" t="s">
         <v>31</v>
       </c>
@@ -6285,12 +6285,12 @@
       <c r="EC35" s="11"/>
       <c r="ED35" s="12"/>
     </row>
-    <row r="36" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A36" s="77"/>
-      <c r="B36" s="97"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="85"/>
+    <row r="36" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A36" s="86"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="96"/>
       <c r="F36" s="61"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -6421,12 +6421,12 @@
       <c r="EC36" s="17"/>
       <c r="ED36" s="18"/>
     </row>
-    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="97"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="85"/>
+    <row r="37" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A37" s="86"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="96"/>
       <c r="F37" s="62" t="s">
         <v>32</v>
       </c>
@@ -6559,12 +6559,12 @@
       <c r="EC37" s="17"/>
       <c r="ED37" s="18"/>
     </row>
-    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="97"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="87"/>
+    <row r="38" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A38" s="86"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="97"/>
+      <c r="E38" s="98"/>
       <c r="F38" s="61"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -6695,16 +6695,16 @@
       <c r="EC38" s="17"/>
       <c r="ED38" s="18"/>
     </row>
-    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A39" s="51"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="88" t="s">
+      <c r="B39" s="87"/>
+      <c r="C39" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="98" t="s">
+      <c r="D39" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="92"/>
+      <c r="E39" s="81"/>
       <c r="F39" s="60" t="s">
         <v>31</v>
       </c>
@@ -6837,12 +6837,12 @@
       <c r="EC39" s="24"/>
       <c r="ED39" s="25"/>
     </row>
-    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A40" s="51"/>
-      <c r="B40" s="97"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="94"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="78"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="83"/>
       <c r="F40" s="61"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -6973,12 +6973,12 @@
       <c r="EC40" s="27"/>
       <c r="ED40" s="28"/>
     </row>
-    <row r="41" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A41" s="51"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="94"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="83"/>
       <c r="F41" s="62" t="s">
         <v>32</v>
       </c>
@@ -7111,12 +7111,12 @@
       <c r="EC41" s="27"/>
       <c r="ED41" s="28"/>
     </row>
-    <row r="42" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A42" s="51"/>
-      <c r="B42" s="97"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="96"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="85"/>
       <c r="F42" s="61"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -7247,16 +7247,16 @@
       <c r="EC42" s="27"/>
       <c r="ED42" s="28"/>
     </row>
-    <row r="43" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A43" s="51"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="79" t="s">
+      <c r="B43" s="87"/>
+      <c r="C43" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="83"/>
+      <c r="E43" s="94"/>
       <c r="F43" s="60" t="s">
         <v>31</v>
       </c>
@@ -7389,12 +7389,12 @@
       <c r="EC43" s="11"/>
       <c r="ED43" s="12"/>
     </row>
-    <row r="44" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A44" s="51"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="85"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="96"/>
       <c r="F44" s="61"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -7525,12 +7525,12 @@
       <c r="EC44" s="17"/>
       <c r="ED44" s="18"/>
     </row>
-    <row r="45" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A45" s="51"/>
-      <c r="B45" s="97"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="85"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="96"/>
       <c r="F45" s="62" t="s">
         <v>32</v>
       </c>
@@ -7663,12 +7663,12 @@
       <c r="EC45" s="17"/>
       <c r="ED45" s="18"/>
     </row>
-    <row r="46" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A46" s="51"/>
-      <c r="B46" s="97"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="87"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="98"/>
       <c r="F46" s="61"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -7799,16 +7799,16 @@
       <c r="EC46" s="17"/>
       <c r="ED46" s="18"/>
     </row>
-    <row r="47" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A47" s="51"/>
-      <c r="B47" s="97"/>
-      <c r="C47" s="88" t="s">
+      <c r="B47" s="87"/>
+      <c r="C47" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="98" t="s">
+      <c r="D47" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="92"/>
+      <c r="E47" s="81"/>
       <c r="F47" s="60" t="s">
         <v>31</v>
       </c>
@@ -7941,12 +7941,12 @@
       <c r="EC47" s="24"/>
       <c r="ED47" s="25"/>
     </row>
-    <row r="48" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A48" s="51"/>
-      <c r="B48" s="97"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="94"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="78"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="83"/>
       <c r="F48" s="61"/>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -8077,12 +8077,12 @@
       <c r="EC48" s="27"/>
       <c r="ED48" s="28"/>
     </row>
-    <row r="49" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A49" s="51"/>
-      <c r="B49" s="97"/>
-      <c r="C49" s="89"/>
-      <c r="D49" s="99"/>
-      <c r="E49" s="94"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="78"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
       <c r="F49" s="62" t="s">
         <v>32</v>
       </c>
@@ -8215,12 +8215,12 @@
       <c r="EC49" s="27"/>
       <c r="ED49" s="28"/>
     </row>
-    <row r="50" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A50" s="51"/>
-      <c r="B50" s="97"/>
-      <c r="C50" s="90"/>
-      <c r="D50" s="95"/>
-      <c r="E50" s="96"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="85"/>
       <c r="F50" s="61"/>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -8351,16 +8351,16 @@
       <c r="EC50" s="27"/>
       <c r="ED50" s="28"/>
     </row>
-    <row r="51" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A51" s="51"/>
-      <c r="B51" s="97"/>
+      <c r="B51" s="87"/>
       <c r="C51" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="82" t="s">
+      <c r="D51" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="83"/>
+      <c r="E51" s="94"/>
       <c r="F51" s="60" t="s">
         <v>31</v>
       </c>
@@ -8493,12 +8493,12 @@
       <c r="EC51" s="11"/>
       <c r="ED51" s="12"/>
     </row>
-    <row r="52" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A52" s="51"/>
-      <c r="B52" s="97"/>
+      <c r="B52" s="87"/>
       <c r="C52" s="53"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="85"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="96"/>
       <c r="F52" s="61"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
@@ -8629,12 +8629,12 @@
       <c r="EC52" s="17"/>
       <c r="ED52" s="18"/>
     </row>
-    <row r="53" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A53" s="51"/>
-      <c r="B53" s="97"/>
+      <c r="B53" s="87"/>
       <c r="C53" s="53"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="85"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="96"/>
       <c r="F53" s="62" t="s">
         <v>32</v>
       </c>
@@ -8767,12 +8767,12 @@
       <c r="EC53" s="17"/>
       <c r="ED53" s="18"/>
     </row>
-    <row r="54" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A54" s="51"/>
-      <c r="B54" s="97"/>
+      <c r="B54" s="87"/>
       <c r="C54" s="54"/>
-      <c r="D54" s="86"/>
-      <c r="E54" s="87"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="98"/>
       <c r="F54" s="61"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -8903,16 +8903,16 @@
       <c r="EC54" s="17"/>
       <c r="ED54" s="18"/>
     </row>
-    <row r="55" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A55" s="51"/>
-      <c r="B55" s="97"/>
+      <c r="B55" s="87"/>
       <c r="C55" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="98" t="s">
+      <c r="D55" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="92"/>
+      <c r="E55" s="81"/>
       <c r="F55" s="60" t="s">
         <v>31</v>
       </c>
@@ -9045,12 +9045,12 @@
       <c r="EC55" s="24"/>
       <c r="ED55" s="25"/>
     </row>
-    <row r="56" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A56" s="51"/>
-      <c r="B56" s="97"/>
+      <c r="B56" s="87"/>
       <c r="C56" s="56"/>
-      <c r="D56" s="99"/>
-      <c r="E56" s="94"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="83"/>
       <c r="F56" s="61"/>
       <c r="G56" s="26"/>
       <c r="H56" s="27"/>
@@ -9181,12 +9181,12 @@
       <c r="EC56" s="27"/>
       <c r="ED56" s="28"/>
     </row>
-    <row r="57" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A57" s="51"/>
-      <c r="B57" s="97"/>
+      <c r="B57" s="87"/>
       <c r="C57" s="56"/>
-      <c r="D57" s="99"/>
-      <c r="E57" s="94"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="83"/>
       <c r="F57" s="62" t="s">
         <v>32</v>
       </c>
@@ -9319,12 +9319,12 @@
       <c r="EC57" s="27"/>
       <c r="ED57" s="28"/>
     </row>
-    <row r="58" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A58" s="51"/>
-      <c r="B58" s="97"/>
+      <c r="B58" s="87"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="95"/>
-      <c r="E58" s="96"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="85"/>
       <c r="F58" s="61"/>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -9455,16 +9455,16 @@
       <c r="EC58" s="27"/>
       <c r="ED58" s="28"/>
     </row>
-    <row r="59" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A59" s="51"/>
-      <c r="B59" s="97"/>
+      <c r="B59" s="87"/>
       <c r="C59" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="82" t="s">
+      <c r="D59" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="83"/>
+      <c r="E59" s="94"/>
       <c r="F59" s="60" t="s">
         <v>31</v>
       </c>
@@ -9597,12 +9597,12 @@
       <c r="EC59" s="11"/>
       <c r="ED59" s="12"/>
     </row>
-    <row r="60" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A60" s="51"/>
-      <c r="B60" s="97"/>
+      <c r="B60" s="87"/>
       <c r="C60" s="53"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="85"/>
+      <c r="D60" s="95"/>
+      <c r="E60" s="96"/>
       <c r="F60" s="61"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -9733,12 +9733,12 @@
       <c r="EC60" s="17"/>
       <c r="ED60" s="18"/>
     </row>
-    <row r="61" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A61" s="51"/>
-      <c r="B61" s="97"/>
+      <c r="B61" s="87"/>
       <c r="C61" s="53"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="85"/>
+      <c r="D61" s="95"/>
+      <c r="E61" s="96"/>
       <c r="F61" s="62" t="s">
         <v>32</v>
       </c>
@@ -9871,12 +9871,12 @@
       <c r="EC61" s="17"/>
       <c r="ED61" s="18"/>
     </row>
-    <row r="62" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A62" s="51"/>
-      <c r="B62" s="97"/>
+      <c r="B62" s="87"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="86"/>
-      <c r="E62" s="87"/>
+      <c r="D62" s="97"/>
+      <c r="E62" s="98"/>
       <c r="F62" s="61"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -10007,12 +10007,12 @@
       <c r="EC62" s="17"/>
       <c r="ED62" s="18"/>
     </row>
-    <row r="63" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
-      <c r="B63" s="97"/>
-      <c r="C63" s="88"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="92"/>
+      <c r="B63" s="87"/>
+      <c r="C63" s="77"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="81"/>
       <c r="F63" s="60" t="s">
         <v>31</v>
       </c>
@@ -10145,12 +10145,12 @@
       <c r="EC63" s="24"/>
       <c r="ED63" s="25"/>
     </row>
-    <row r="64" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A64" s="51"/>
-      <c r="B64" s="97"/>
-      <c r="C64" s="89"/>
-      <c r="D64" s="99"/>
-      <c r="E64" s="94"/>
+      <c r="B64" s="87"/>
+      <c r="C64" s="78"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="83"/>
       <c r="F64" s="61"/>
       <c r="G64" s="26"/>
       <c r="H64" s="27"/>
@@ -10281,12 +10281,12 @@
       <c r="EC64" s="27"/>
       <c r="ED64" s="28"/>
     </row>
-    <row r="65" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A65" s="51"/>
-      <c r="B65" s="97"/>
-      <c r="C65" s="89"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="94"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="78"/>
+      <c r="D65" s="82"/>
+      <c r="E65" s="83"/>
       <c r="F65" s="62" t="s">
         <v>32</v>
       </c>
@@ -10419,12 +10419,12 @@
       <c r="EC65" s="27"/>
       <c r="ED65" s="28"/>
     </row>
-    <row r="66" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A66" s="51"/>
-      <c r="B66" s="97"/>
-      <c r="C66" s="90"/>
-      <c r="D66" s="95"/>
-      <c r="E66" s="96"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="79"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="85"/>
       <c r="F66" s="61"/>
       <c r="G66" s="26"/>
       <c r="H66" s="27"/>
@@ -10555,12 +10555,12 @@
       <c r="EC66" s="27"/>
       <c r="ED66" s="28"/>
     </row>
-    <row r="67" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A67" s="51"/>
-      <c r="B67" s="97"/>
-      <c r="C67" s="79"/>
-      <c r="D67" s="82"/>
-      <c r="E67" s="83"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="90"/>
+      <c r="D67" s="93"/>
+      <c r="E67" s="94"/>
       <c r="F67" s="60" t="s">
         <v>31</v>
       </c>
@@ -10693,12 +10693,12 @@
       <c r="EC67" s="11"/>
       <c r="ED67" s="12"/>
     </row>
-    <row r="68" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A68" s="51"/>
-      <c r="B68" s="97"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="84"/>
-      <c r="E68" s="85"/>
+      <c r="B68" s="87"/>
+      <c r="C68" s="91"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="96"/>
       <c r="F68" s="61"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -10829,12 +10829,12 @@
       <c r="EC68" s="17"/>
       <c r="ED68" s="18"/>
     </row>
-    <row r="69" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A69" s="51"/>
-      <c r="B69" s="97"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="84"/>
-      <c r="E69" s="85"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="91"/>
+      <c r="D69" s="95"/>
+      <c r="E69" s="96"/>
       <c r="F69" s="62" t="s">
         <v>32</v>
       </c>
@@ -10967,12 +10967,12 @@
       <c r="EC69" s="17"/>
       <c r="ED69" s="18"/>
     </row>
-    <row r="70" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A70" s="51"/>
-      <c r="B70" s="97"/>
-      <c r="C70" s="81"/>
-      <c r="D70" s="86"/>
-      <c r="E70" s="87"/>
+      <c r="B70" s="87"/>
+      <c r="C70" s="92"/>
+      <c r="D70" s="97"/>
+      <c r="E70" s="98"/>
       <c r="F70" s="61"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -11103,12 +11103,12 @@
       <c r="EC70" s="17"/>
       <c r="ED70" s="18"/>
     </row>
-    <row r="71" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A71" s="51"/>
-      <c r="B71" s="97"/>
-      <c r="C71" s="88"/>
-      <c r="D71" s="98"/>
-      <c r="E71" s="92"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="77"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="81"/>
       <c r="F71" s="60" t="s">
         <v>31</v>
       </c>
@@ -11241,12 +11241,12 @@
       <c r="EC71" s="24"/>
       <c r="ED71" s="25"/>
     </row>
-    <row r="72" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A72" s="51"/>
-      <c r="B72" s="97"/>
-      <c r="C72" s="89"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="94"/>
+      <c r="B72" s="87"/>
+      <c r="C72" s="78"/>
+      <c r="D72" s="82"/>
+      <c r="E72" s="83"/>
       <c r="F72" s="61"/>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
@@ -11377,12 +11377,12 @@
       <c r="EC72" s="27"/>
       <c r="ED72" s="28"/>
     </row>
-    <row r="73" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A73" s="51"/>
-      <c r="B73" s="97"/>
-      <c r="C73" s="89"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="94"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="78"/>
+      <c r="D73" s="82"/>
+      <c r="E73" s="83"/>
       <c r="F73" s="62" t="s">
         <v>32</v>
       </c>
@@ -11515,12 +11515,12 @@
       <c r="EC73" s="27"/>
       <c r="ED73" s="28"/>
     </row>
-    <row r="74" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A74" s="51"/>
-      <c r="B74" s="97"/>
-      <c r="C74" s="90"/>
-      <c r="D74" s="95"/>
-      <c r="E74" s="96"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="79"/>
+      <c r="D74" s="84"/>
+      <c r="E74" s="85"/>
       <c r="F74" s="61"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -11651,12 +11651,12 @@
       <c r="EC74" s="27"/>
       <c r="ED74" s="28"/>
     </row>
-    <row r="75" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A75" s="51"/>
-      <c r="B75" s="97"/>
-      <c r="C75" s="79"/>
-      <c r="D75" s="82"/>
-      <c r="E75" s="83"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="90"/>
+      <c r="D75" s="93"/>
+      <c r="E75" s="94"/>
       <c r="F75" s="60" t="s">
         <v>31</v>
       </c>
@@ -11789,12 +11789,12 @@
       <c r="EC75" s="11"/>
       <c r="ED75" s="12"/>
     </row>
-    <row r="76" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A76" s="51"/>
-      <c r="B76" s="97"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="84"/>
-      <c r="E76" s="85"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="91"/>
+      <c r="D76" s="95"/>
+      <c r="E76" s="96"/>
       <c r="F76" s="61"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -11925,12 +11925,12 @@
       <c r="EC76" s="17"/>
       <c r="ED76" s="18"/>
     </row>
-    <row r="77" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A77" s="51"/>
-      <c r="B77" s="97"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="85"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="95"/>
+      <c r="E77" s="96"/>
       <c r="F77" s="62" t="s">
         <v>32</v>
       </c>
@@ -12063,12 +12063,12 @@
       <c r="EC77" s="17"/>
       <c r="ED77" s="18"/>
     </row>
-    <row r="78" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A78" s="51"/>
-      <c r="B78" s="97"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="86"/>
-      <c r="E78" s="87"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="97"/>
+      <c r="E78" s="98"/>
       <c r="F78" s="61"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -12199,20 +12199,20 @@
       <c r="EC78" s="17"/>
       <c r="ED78" s="18"/>
     </row>
-    <row r="79" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A79" s="77">
+    <row r="79" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A79" s="86">
         <v>11</v>
       </c>
-      <c r="B79" s="78" t="s">
+      <c r="B79" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="88" t="s">
+      <c r="C79" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="98" t="s">
+      <c r="D79" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="92"/>
+      <c r="E79" s="81"/>
       <c r="F79" s="60" t="s">
         <v>31</v>
       </c>
@@ -12345,12 +12345,12 @@
       <c r="EC79" s="24"/>
       <c r="ED79" s="25"/>
     </row>
-    <row r="80" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A80" s="77"/>
-      <c r="B80" s="78"/>
-      <c r="C80" s="89"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="94"/>
+    <row r="80" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A80" s="86"/>
+      <c r="B80" s="99"/>
+      <c r="C80" s="78"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="83"/>
       <c r="F80" s="61"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12481,12 +12481,12 @@
       <c r="EC80" s="27"/>
       <c r="ED80" s="28"/>
     </row>
-    <row r="81" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A81" s="77"/>
-      <c r="B81" s="78"/>
-      <c r="C81" s="89"/>
-      <c r="D81" s="99"/>
-      <c r="E81" s="94"/>
+    <row r="81" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A81" s="86"/>
+      <c r="B81" s="99"/>
+      <c r="C81" s="78"/>
+      <c r="D81" s="82"/>
+      <c r="E81" s="83"/>
       <c r="F81" s="62" t="s">
         <v>32</v>
       </c>
@@ -12574,10 +12574,10 @@
       <c r="CJ81" s="27"/>
       <c r="CK81" s="27"/>
       <c r="CL81" s="27"/>
-      <c r="CM81" s="27"/>
-      <c r="CN81" s="27"/>
-      <c r="CO81" s="27"/>
-      <c r="CP81" s="28"/>
+      <c r="CM81" s="19"/>
+      <c r="CN81" s="19"/>
+      <c r="CO81" s="19"/>
+      <c r="CP81" s="30"/>
       <c r="CQ81" s="27"/>
       <c r="CR81" s="27"/>
       <c r="CS81" s="27"/>
@@ -12619,12 +12619,12 @@
       <c r="EC81" s="27"/>
       <c r="ED81" s="28"/>
     </row>
-    <row r="82" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A82" s="77"/>
-      <c r="B82" s="78"/>
-      <c r="C82" s="90"/>
-      <c r="D82" s="95"/>
-      <c r="E82" s="96"/>
+    <row r="82" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A82" s="86"/>
+      <c r="B82" s="99"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="84"/>
+      <c r="E82" s="85"/>
       <c r="F82" s="61"/>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
@@ -12710,10 +12710,10 @@
       <c r="CJ82" s="27"/>
       <c r="CK82" s="27"/>
       <c r="CL82" s="27"/>
-      <c r="CM82" s="27"/>
-      <c r="CN82" s="27"/>
-      <c r="CO82" s="27"/>
-      <c r="CP82" s="28"/>
+      <c r="CM82" s="19"/>
+      <c r="CN82" s="19"/>
+      <c r="CO82" s="19"/>
+      <c r="CP82" s="30"/>
       <c r="CQ82" s="27"/>
       <c r="CR82" s="27"/>
       <c r="CS82" s="27"/>
@@ -12755,16 +12755,16 @@
       <c r="EC82" s="27"/>
       <c r="ED82" s="28"/>
     </row>
-    <row r="83" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A83" s="51"/>
-      <c r="B83" s="78"/>
-      <c r="C83" s="79" t="s">
+      <c r="B83" s="99"/>
+      <c r="C83" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="82" t="s">
+      <c r="D83" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="E83" s="83"/>
+      <c r="E83" s="94"/>
       <c r="F83" s="60" t="s">
         <v>31</v>
       </c>
@@ -12897,12 +12897,12 @@
       <c r="EC83" s="11"/>
       <c r="ED83" s="12"/>
     </row>
-    <row r="84" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A84" s="51"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="84"/>
-      <c r="E84" s="85"/>
+      <c r="B84" s="99"/>
+      <c r="C84" s="91"/>
+      <c r="D84" s="95"/>
+      <c r="E84" s="96"/>
       <c r="F84" s="61"/>
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
@@ -13033,12 +13033,12 @@
       <c r="EC84" s="17"/>
       <c r="ED84" s="18"/>
     </row>
-    <row r="85" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A85" s="51"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="80"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="85"/>
+      <c r="B85" s="99"/>
+      <c r="C85" s="91"/>
+      <c r="D85" s="95"/>
+      <c r="E85" s="96"/>
       <c r="F85" s="62" t="s">
         <v>32</v>
       </c>
@@ -13171,12 +13171,12 @@
       <c r="EC85" s="17"/>
       <c r="ED85" s="18"/>
     </row>
-    <row r="86" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A86" s="51"/>
-      <c r="B86" s="78"/>
-      <c r="C86" s="81"/>
-      <c r="D86" s="86"/>
-      <c r="E86" s="87"/>
+      <c r="B86" s="99"/>
+      <c r="C86" s="92"/>
+      <c r="D86" s="97"/>
+      <c r="E86" s="98"/>
       <c r="F86" s="61"/>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -13307,16 +13307,16 @@
       <c r="EC86" s="17"/>
       <c r="ED86" s="18"/>
     </row>
-    <row r="87" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A87" s="51"/>
-      <c r="B87" s="78"/>
-      <c r="C87" s="88" t="s">
+      <c r="B87" s="99"/>
+      <c r="C87" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="D87" s="98" t="s">
+      <c r="D87" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="92"/>
+      <c r="E87" s="81"/>
       <c r="F87" s="60" t="s">
         <v>31</v>
       </c>
@@ -13449,12 +13449,12 @@
       <c r="EC87" s="24"/>
       <c r="ED87" s="25"/>
     </row>
-    <row r="88" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A88" s="51"/>
-      <c r="B88" s="78"/>
-      <c r="C88" s="89"/>
-      <c r="D88" s="99"/>
-      <c r="E88" s="94"/>
+      <c r="B88" s="99"/>
+      <c r="C88" s="78"/>
+      <c r="D88" s="82"/>
+      <c r="E88" s="83"/>
       <c r="F88" s="61"/>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -13585,12 +13585,12 @@
       <c r="EC88" s="27"/>
       <c r="ED88" s="28"/>
     </row>
-    <row r="89" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A89" s="51"/>
-      <c r="B89" s="78"/>
-      <c r="C89" s="89"/>
-      <c r="D89" s="99"/>
-      <c r="E89" s="94"/>
+      <c r="B89" s="99"/>
+      <c r="C89" s="78"/>
+      <c r="D89" s="82"/>
+      <c r="E89" s="83"/>
       <c r="F89" s="62" t="s">
         <v>32</v>
       </c>
@@ -13678,10 +13678,10 @@
       <c r="CJ89" s="27"/>
       <c r="CK89" s="27"/>
       <c r="CL89" s="27"/>
-      <c r="CM89" s="27"/>
-      <c r="CN89" s="27"/>
-      <c r="CO89" s="27"/>
-      <c r="CP89" s="28"/>
+      <c r="CM89" s="19"/>
+      <c r="CN89" s="19"/>
+      <c r="CO89" s="19"/>
+      <c r="CP89" s="30"/>
       <c r="CQ89" s="27"/>
       <c r="CR89" s="27"/>
       <c r="CS89" s="27"/>
@@ -13723,12 +13723,12 @@
       <c r="EC89" s="27"/>
       <c r="ED89" s="28"/>
     </row>
-    <row r="90" spans="1:134" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:134" x14ac:dyDescent="0.3">
       <c r="A90" s="51"/>
-      <c r="B90" s="78"/>
-      <c r="C90" s="90"/>
-      <c r="D90" s="95"/>
-      <c r="E90" s="96"/>
+      <c r="B90" s="99"/>
+      <c r="C90" s="79"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="85"/>
       <c r="F90" s="61"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -13814,10 +13814,10 @@
       <c r="CJ90" s="27"/>
       <c r="CK90" s="27"/>
       <c r="CL90" s="27"/>
-      <c r="CM90" s="27"/>
-      <c r="CN90" s="27"/>
-      <c r="CO90" s="27"/>
-      <c r="CP90" s="28"/>
+      <c r="CM90" s="19"/>
+      <c r="CN90" s="19"/>
+      <c r="CO90" s="19"/>
+      <c r="CP90" s="30"/>
       <c r="CQ90" s="27"/>
       <c r="CR90" s="27"/>
       <c r="CS90" s="27"/>
@@ -13859,18 +13859,18 @@
       <c r="EC90" s="27"/>
       <c r="ED90" s="28"/>
     </row>
-    <row r="91" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A91" s="77">
+    <row r="91" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A91" s="86">
         <v>13</v>
       </c>
-      <c r="B91" s="78"/>
-      <c r="C91" s="79" t="s">
+      <c r="B91" s="99"/>
+      <c r="C91" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="82" t="s">
+      <c r="D91" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="E91" s="83"/>
+      <c r="E91" s="94"/>
       <c r="F91" s="60" t="s">
         <v>31</v>
       </c>
@@ -14003,12 +14003,12 @@
       <c r="EC91" s="11"/>
       <c r="ED91" s="12"/>
     </row>
-    <row r="92" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A92" s="77"/>
-      <c r="B92" s="78"/>
-      <c r="C92" s="80"/>
-      <c r="D92" s="84"/>
-      <c r="E92" s="85"/>
+    <row r="92" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A92" s="86"/>
+      <c r="B92" s="99"/>
+      <c r="C92" s="91"/>
+      <c r="D92" s="95"/>
+      <c r="E92" s="96"/>
       <c r="F92" s="61"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -14139,12 +14139,12 @@
       <c r="EC92" s="17"/>
       <c r="ED92" s="18"/>
     </row>
-    <row r="93" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A93" s="77"/>
-      <c r="B93" s="78"/>
-      <c r="C93" s="80"/>
-      <c r="D93" s="84"/>
-      <c r="E93" s="85"/>
+    <row r="93" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A93" s="86"/>
+      <c r="B93" s="99"/>
+      <c r="C93" s="91"/>
+      <c r="D93" s="95"/>
+      <c r="E93" s="96"/>
       <c r="F93" s="62" t="s">
         <v>32</v>
       </c>
@@ -14277,12 +14277,12 @@
       <c r="EC93" s="17"/>
       <c r="ED93" s="18"/>
     </row>
-    <row r="94" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A94" s="77"/>
-      <c r="B94" s="78"/>
-      <c r="C94" s="81"/>
-      <c r="D94" s="86"/>
-      <c r="E94" s="87"/>
+    <row r="94" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A94" s="86"/>
+      <c r="B94" s="99"/>
+      <c r="C94" s="92"/>
+      <c r="D94" s="97"/>
+      <c r="E94" s="98"/>
       <c r="F94" s="61"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17"/>
@@ -14413,20 +14413,20 @@
       <c r="EC94" s="17"/>
       <c r="ED94" s="18"/>
     </row>
-    <row r="95" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A95" s="77">
+    <row r="95" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A95" s="86">
         <v>14</v>
       </c>
-      <c r="B95" s="97" t="s">
+      <c r="B95" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="88" t="s">
+      <c r="C95" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="91" t="s">
+      <c r="D95" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="92"/>
+      <c r="E95" s="81"/>
       <c r="F95" s="60" t="s">
         <v>31</v>
       </c>
@@ -14559,12 +14559,12 @@
       <c r="EC95" s="24"/>
       <c r="ED95" s="25"/>
     </row>
-    <row r="96" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A96" s="77"/>
-      <c r="B96" s="97"/>
-      <c r="C96" s="89"/>
-      <c r="D96" s="93"/>
-      <c r="E96" s="94"/>
+    <row r="96" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A96" s="86"/>
+      <c r="B96" s="87"/>
+      <c r="C96" s="78"/>
+      <c r="D96" s="89"/>
+      <c r="E96" s="83"/>
       <c r="F96" s="61"/>
       <c r="G96" s="26"/>
       <c r="H96" s="27"/>
@@ -14695,12 +14695,12 @@
       <c r="EC96" s="27"/>
       <c r="ED96" s="28"/>
     </row>
-    <row r="97" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A97" s="77"/>
-      <c r="B97" s="97"/>
-      <c r="C97" s="89"/>
-      <c r="D97" s="93"/>
-      <c r="E97" s="94"/>
+    <row r="97" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A97" s="86"/>
+      <c r="B97" s="87"/>
+      <c r="C97" s="78"/>
+      <c r="D97" s="89"/>
+      <c r="E97" s="83"/>
       <c r="F97" s="62" t="s">
         <v>32</v>
       </c>
@@ -14833,12 +14833,12 @@
       <c r="EC97" s="27"/>
       <c r="ED97" s="28"/>
     </row>
-    <row r="98" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A98" s="77"/>
-      <c r="B98" s="97"/>
-      <c r="C98" s="90"/>
-      <c r="D98" s="95"/>
-      <c r="E98" s="96"/>
+    <row r="98" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A98" s="86"/>
+      <c r="B98" s="87"/>
+      <c r="C98" s="79"/>
+      <c r="D98" s="84"/>
+      <c r="E98" s="85"/>
       <c r="F98" s="61"/>
       <c r="G98" s="26"/>
       <c r="H98" s="27"/>
@@ -14969,18 +14969,18 @@
       <c r="EC98" s="27"/>
       <c r="ED98" s="28"/>
     </row>
-    <row r="99" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A99" s="77">
+    <row r="99" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A99" s="86">
         <v>15</v>
       </c>
-      <c r="B99" s="97"/>
-      <c r="C99" s="79" t="s">
+      <c r="B99" s="87"/>
+      <c r="C99" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="82" t="s">
+      <c r="D99" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="E99" s="83"/>
+      <c r="E99" s="94"/>
       <c r="F99" s="60" t="s">
         <v>31</v>
       </c>
@@ -15113,12 +15113,12 @@
       <c r="EC99" s="11"/>
       <c r="ED99" s="12"/>
     </row>
-    <row r="100" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A100" s="77"/>
-      <c r="B100" s="97"/>
-      <c r="C100" s="80"/>
-      <c r="D100" s="84"/>
-      <c r="E100" s="85"/>
+    <row r="100" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A100" s="86"/>
+      <c r="B100" s="87"/>
+      <c r="C100" s="91"/>
+      <c r="D100" s="95"/>
+      <c r="E100" s="96"/>
       <c r="F100" s="61"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -15249,12 +15249,12 @@
       <c r="EC100" s="17"/>
       <c r="ED100" s="18"/>
     </row>
-    <row r="101" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A101" s="77"/>
-      <c r="B101" s="97"/>
-      <c r="C101" s="80"/>
-      <c r="D101" s="84"/>
-      <c r="E101" s="85"/>
+    <row r="101" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A101" s="86"/>
+      <c r="B101" s="87"/>
+      <c r="C101" s="91"/>
+      <c r="D101" s="95"/>
+      <c r="E101" s="96"/>
       <c r="F101" s="62" t="s">
         <v>32</v>
       </c>
@@ -15387,12 +15387,12 @@
       <c r="EC101" s="17"/>
       <c r="ED101" s="18"/>
     </row>
-    <row r="102" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A102" s="77"/>
-      <c r="B102" s="97"/>
-      <c r="C102" s="81"/>
-      <c r="D102" s="86"/>
-      <c r="E102" s="87"/>
+    <row r="102" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A102" s="86"/>
+      <c r="B102" s="87"/>
+      <c r="C102" s="92"/>
+      <c r="D102" s="97"/>
+      <c r="E102" s="98"/>
       <c r="F102" s="61"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -15523,18 +15523,18 @@
       <c r="EC102" s="17"/>
       <c r="ED102" s="18"/>
     </row>
-    <row r="103" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A103" s="77">
+    <row r="103" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A103" s="86">
         <v>16</v>
       </c>
-      <c r="B103" s="97"/>
-      <c r="C103" s="88" t="s">
+      <c r="B103" s="87"/>
+      <c r="C103" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="91" t="s">
+      <c r="D103" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="92"/>
+      <c r="E103" s="81"/>
       <c r="F103" s="60" t="s">
         <v>31</v>
       </c>
@@ -15667,12 +15667,12 @@
       <c r="EC103" s="24"/>
       <c r="ED103" s="25"/>
     </row>
-    <row r="104" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A104" s="77"/>
-      <c r="B104" s="97"/>
-      <c r="C104" s="89"/>
-      <c r="D104" s="93"/>
-      <c r="E104" s="94"/>
+    <row r="104" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A104" s="86"/>
+      <c r="B104" s="87"/>
+      <c r="C104" s="78"/>
+      <c r="D104" s="89"/>
+      <c r="E104" s="83"/>
       <c r="F104" s="61"/>
       <c r="G104" s="26"/>
       <c r="H104" s="27"/>
@@ -15803,12 +15803,12 @@
       <c r="EC104" s="27"/>
       <c r="ED104" s="28"/>
     </row>
-    <row r="105" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A105" s="77"/>
-      <c r="B105" s="97"/>
-      <c r="C105" s="89"/>
-      <c r="D105" s="93"/>
-      <c r="E105" s="94"/>
+    <row r="105" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A105" s="86"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="78"/>
+      <c r="D105" s="89"/>
+      <c r="E105" s="83"/>
       <c r="F105" s="62" t="s">
         <v>32</v>
       </c>
@@ -15892,10 +15892,10 @@
       <c r="CF105" s="27"/>
       <c r="CG105" s="27"/>
       <c r="CH105" s="28"/>
-      <c r="CI105" s="26"/>
-      <c r="CJ105" s="27"/>
-      <c r="CK105" s="27"/>
-      <c r="CL105" s="27"/>
+      <c r="CI105" s="68"/>
+      <c r="CJ105" s="19"/>
+      <c r="CK105" s="19"/>
+      <c r="CL105" s="19"/>
       <c r="CM105" s="27"/>
       <c r="CN105" s="27"/>
       <c r="CO105" s="27"/>
@@ -15941,12 +15941,12 @@
       <c r="EC105" s="27"/>
       <c r="ED105" s="28"/>
     </row>
-    <row r="106" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A106" s="77"/>
-      <c r="B106" s="97"/>
-      <c r="C106" s="90"/>
-      <c r="D106" s="95"/>
-      <c r="E106" s="96"/>
+    <row r="106" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A106" s="86"/>
+      <c r="B106" s="87"/>
+      <c r="C106" s="79"/>
+      <c r="D106" s="84"/>
+      <c r="E106" s="85"/>
       <c r="F106" s="61"/>
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
@@ -16028,10 +16028,10 @@
       <c r="CF106" s="27"/>
       <c r="CG106" s="27"/>
       <c r="CH106" s="28"/>
-      <c r="CI106" s="26"/>
-      <c r="CJ106" s="27"/>
-      <c r="CK106" s="27"/>
-      <c r="CL106" s="27"/>
+      <c r="CI106" s="68"/>
+      <c r="CJ106" s="19"/>
+      <c r="CK106" s="19"/>
+      <c r="CL106" s="19"/>
       <c r="CM106" s="27"/>
       <c r="CN106" s="27"/>
       <c r="CO106" s="27"/>
@@ -16077,14 +16077,14 @@
       <c r="EC106" s="27"/>
       <c r="ED106" s="28"/>
     </row>
-    <row r="107" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A107" s="100"/>
+    <row r="107" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A107" s="70"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="101" t="s">
+      <c r="C107" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="103"/>
-      <c r="E107" s="104"/>
+      <c r="D107" s="73"/>
+      <c r="E107" s="74"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
       <c r="H107" s="44"/>
@@ -16217,12 +16217,12 @@
       <c r="EC107" s="44"/>
       <c r="ED107" s="45"/>
     </row>
-    <row r="108" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A108" s="100"/>
+    <row r="108" spans="1:134" x14ac:dyDescent="0.3">
+      <c r="A108" s="70"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="102"/>
-      <c r="D108" s="105"/>
-      <c r="E108" s="106"/>
+      <c r="C108" s="72"/>
+      <c r="D108" s="75"/>
+      <c r="E108" s="76"/>
       <c r="F108" s="46"/>
       <c r="G108" s="47"/>
       <c r="H108" s="48"/>
@@ -16355,44 +16355,40 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:E108"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:E90"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:E98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:E102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="D103:E106"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B94"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="D79:E82"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:E94"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="D83:E86"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:E74"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:E78"/>
-    <mergeCell ref="D59:E62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:E66"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:E70"/>
-    <mergeCell ref="D39:E42"/>
-    <mergeCell ref="D47:E50"/>
-    <mergeCell ref="D51:E54"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="AE1:AL1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="DW1:ED1"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="BC1:BJ1"/>
+    <mergeCell ref="BK1:BR1"/>
+    <mergeCell ref="BS1:BZ1"/>
+    <mergeCell ref="CA1:CH1"/>
+    <mergeCell ref="CI1:CP1"/>
+    <mergeCell ref="CQ1:CX1"/>
+    <mergeCell ref="CY1:DF1"/>
+    <mergeCell ref="DG1:DN1"/>
+    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:E6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:E22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="B23:B78"/>
     <mergeCell ref="C23:C26"/>
@@ -16409,40 +16405,44 @@
     <mergeCell ref="C47:C50"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="C35:C38"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:E6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:E14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:E22"/>
-    <mergeCell ref="DW1:ED1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="BC1:BJ1"/>
-    <mergeCell ref="BK1:BR1"/>
-    <mergeCell ref="BS1:BZ1"/>
-    <mergeCell ref="CA1:CH1"/>
-    <mergeCell ref="CI1:CP1"/>
-    <mergeCell ref="CQ1:CX1"/>
-    <mergeCell ref="CY1:DF1"/>
-    <mergeCell ref="DG1:DN1"/>
-    <mergeCell ref="DO1:DV1"/>
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:V1"/>
-    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="D51:E54"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:E74"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:E78"/>
+    <mergeCell ref="D59:E62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:E66"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:E70"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B94"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:E82"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:E94"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:E86"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:E108"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:E90"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B106"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:E98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="D99:E102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:E106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed TODO and added delay to tooltips
</commit_message>
<xml_diff>
--- a/documentation/Gantt.xlsx
+++ b/documentation/Gantt.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\WebstormProjects\Resonance-Web\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\zraisb\WebstormProjects\Resonance-Web\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12888"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>Nr.</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>3h/</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -675,65 +678,32 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -762,35 +732,74 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
+    <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1132,28 +1141,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ED108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CI105" sqref="CI105:CL106"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AN67" sqref="AN67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="126" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="126" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
@@ -1164,168 +1173,168 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="100">
+      <c r="G1" s="70">
         <v>42803</v>
       </c>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="100">
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="70">
         <v>42804</v>
       </c>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="100">
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="70">
         <v>42809</v>
       </c>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="103"/>
-      <c r="AC1" s="103"/>
-      <c r="AD1" s="104"/>
-      <c r="AE1" s="100">
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="70">
         <v>42810</v>
       </c>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="103"/>
-      <c r="AI1" s="103"/>
-      <c r="AJ1" s="103"/>
-      <c r="AK1" s="103"/>
-      <c r="AL1" s="104"/>
-      <c r="AM1" s="100">
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="72"/>
+      <c r="AM1" s="70">
         <v>42811</v>
       </c>
-      <c r="AN1" s="103"/>
-      <c r="AO1" s="103"/>
-      <c r="AP1" s="103"/>
-      <c r="AQ1" s="103"/>
-      <c r="AR1" s="103"/>
-      <c r="AS1" s="103"/>
-      <c r="AT1" s="104"/>
-      <c r="AU1" s="100">
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="71"/>
+      <c r="AP1" s="71"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="72"/>
+      <c r="AU1" s="70">
         <v>42816</v>
       </c>
-      <c r="AV1" s="103"/>
-      <c r="AW1" s="103"/>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="103"/>
-      <c r="BA1" s="103"/>
-      <c r="BB1" s="104"/>
-      <c r="BC1" s="100">
+      <c r="AV1" s="71"/>
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="71"/>
+      <c r="AY1" s="71"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="71"/>
+      <c r="BB1" s="72"/>
+      <c r="BC1" s="70">
         <v>42817</v>
       </c>
-      <c r="BD1" s="103"/>
-      <c r="BE1" s="103"/>
-      <c r="BF1" s="103"/>
-      <c r="BG1" s="103"/>
-      <c r="BH1" s="103"/>
-      <c r="BI1" s="103"/>
-      <c r="BJ1" s="104"/>
-      <c r="BK1" s="100">
+      <c r="BD1" s="71"/>
+      <c r="BE1" s="71"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="71"/>
+      <c r="BH1" s="71"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="72"/>
+      <c r="BK1" s="70">
         <v>42818</v>
       </c>
-      <c r="BL1" s="103"/>
-      <c r="BM1" s="103"/>
-      <c r="BN1" s="103"/>
-      <c r="BO1" s="103"/>
-      <c r="BP1" s="103"/>
-      <c r="BQ1" s="103"/>
-      <c r="BR1" s="104"/>
-      <c r="BS1" s="100">
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="71"/>
+      <c r="BN1" s="71"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="71"/>
+      <c r="BQ1" s="71"/>
+      <c r="BR1" s="72"/>
+      <c r="BS1" s="70">
         <v>42823</v>
       </c>
-      <c r="BT1" s="103"/>
-      <c r="BU1" s="103"/>
-      <c r="BV1" s="103"/>
-      <c r="BW1" s="103"/>
-      <c r="BX1" s="103"/>
-      <c r="BY1" s="103"/>
-      <c r="BZ1" s="104"/>
-      <c r="CA1" s="100">
+      <c r="BT1" s="71"/>
+      <c r="BU1" s="71"/>
+      <c r="BV1" s="71"/>
+      <c r="BW1" s="71"/>
+      <c r="BX1" s="71"/>
+      <c r="BY1" s="71"/>
+      <c r="BZ1" s="72"/>
+      <c r="CA1" s="70">
         <v>42824</v>
       </c>
-      <c r="CB1" s="101"/>
-      <c r="CC1" s="101"/>
-      <c r="CD1" s="101"/>
-      <c r="CE1" s="101"/>
-      <c r="CF1" s="101"/>
-      <c r="CG1" s="101"/>
-      <c r="CH1" s="102"/>
-      <c r="CI1" s="100">
+      <c r="CB1" s="75"/>
+      <c r="CC1" s="75"/>
+      <c r="CD1" s="75"/>
+      <c r="CE1" s="75"/>
+      <c r="CF1" s="75"/>
+      <c r="CG1" s="75"/>
+      <c r="CH1" s="76"/>
+      <c r="CI1" s="70">
         <v>42825</v>
       </c>
-      <c r="CJ1" s="101"/>
-      <c r="CK1" s="101"/>
-      <c r="CL1" s="101"/>
-      <c r="CM1" s="101"/>
-      <c r="CN1" s="101"/>
-      <c r="CO1" s="101"/>
-      <c r="CP1" s="102"/>
-      <c r="CQ1" s="100">
+      <c r="CJ1" s="75"/>
+      <c r="CK1" s="75"/>
+      <c r="CL1" s="75"/>
+      <c r="CM1" s="75"/>
+      <c r="CN1" s="75"/>
+      <c r="CO1" s="75"/>
+      <c r="CP1" s="76"/>
+      <c r="CQ1" s="70">
         <v>42826</v>
       </c>
-      <c r="CR1" s="101"/>
-      <c r="CS1" s="101"/>
-      <c r="CT1" s="101"/>
-      <c r="CU1" s="101"/>
-      <c r="CV1" s="101"/>
-      <c r="CW1" s="101"/>
-      <c r="CX1" s="102"/>
-      <c r="CY1" s="100">
+      <c r="CR1" s="75"/>
+      <c r="CS1" s="75"/>
+      <c r="CT1" s="75"/>
+      <c r="CU1" s="75"/>
+      <c r="CV1" s="75"/>
+      <c r="CW1" s="75"/>
+      <c r="CX1" s="76"/>
+      <c r="CY1" s="70">
         <v>42830</v>
       </c>
-      <c r="CZ1" s="101"/>
-      <c r="DA1" s="101"/>
-      <c r="DB1" s="101"/>
-      <c r="DC1" s="101"/>
-      <c r="DD1" s="101"/>
-      <c r="DE1" s="101"/>
-      <c r="DF1" s="102"/>
-      <c r="DG1" s="100">
+      <c r="CZ1" s="75"/>
+      <c r="DA1" s="75"/>
+      <c r="DB1" s="75"/>
+      <c r="DC1" s="75"/>
+      <c r="DD1" s="75"/>
+      <c r="DE1" s="75"/>
+      <c r="DF1" s="76"/>
+      <c r="DG1" s="70">
         <v>42831</v>
       </c>
-      <c r="DH1" s="101"/>
-      <c r="DI1" s="101"/>
-      <c r="DJ1" s="101"/>
-      <c r="DK1" s="101"/>
-      <c r="DL1" s="101"/>
-      <c r="DM1" s="101"/>
-      <c r="DN1" s="102"/>
-      <c r="DO1" s="100">
+      <c r="DH1" s="75"/>
+      <c r="DI1" s="75"/>
+      <c r="DJ1" s="75"/>
+      <c r="DK1" s="75"/>
+      <c r="DL1" s="75"/>
+      <c r="DM1" s="75"/>
+      <c r="DN1" s="76"/>
+      <c r="DO1" s="70">
         <v>42832</v>
       </c>
-      <c r="DP1" s="101"/>
-      <c r="DQ1" s="101"/>
-      <c r="DR1" s="101"/>
-      <c r="DS1" s="101"/>
-      <c r="DT1" s="101"/>
-      <c r="DU1" s="101"/>
-      <c r="DV1" s="102"/>
-      <c r="DW1" s="100"/>
-      <c r="DX1" s="101"/>
-      <c r="DY1" s="101"/>
-      <c r="DZ1" s="101"/>
-      <c r="EA1" s="101"/>
-      <c r="EB1" s="101"/>
-      <c r="EC1" s="101"/>
-      <c r="ED1" s="102"/>
+      <c r="DP1" s="75"/>
+      <c r="DQ1" s="75"/>
+      <c r="DR1" s="75"/>
+      <c r="DS1" s="75"/>
+      <c r="DT1" s="75"/>
+      <c r="DU1" s="75"/>
+      <c r="DV1" s="76"/>
+      <c r="DW1" s="70"/>
+      <c r="DX1" s="75"/>
+      <c r="DY1" s="75"/>
+      <c r="DZ1" s="75"/>
+      <c r="EA1" s="75"/>
+      <c r="EB1" s="75"/>
+      <c r="EC1" s="75"/>
+      <c r="ED1" s="76"/>
     </row>
-    <row r="2" spans="1:134" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="105"/>
-      <c r="B2" s="106"/>
+    <row r="2" spans="1:134" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="73"/>
+      <c r="B2" s="74"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1705,20 +1714,20 @@
       <c r="EC2" s="8"/>
       <c r="ED2" s="9"/>
     </row>
-    <row r="3" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A3" s="86">
+    <row r="3" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A3" s="77">
         <v>1</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="94"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="60" t="s">
         <v>31</v>
       </c>
@@ -1851,12 +1860,12 @@
       <c r="EC3" s="11"/>
       <c r="ED3" s="12"/>
     </row>
-    <row r="4" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
+    <row r="4" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="61"/>
       <c r="G4" s="65"/>
       <c r="H4" s="16"/>
@@ -1987,12 +1996,12 @@
       <c r="EC4" s="17"/>
       <c r="ED4" s="18"/>
     </row>
-    <row r="5" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
+    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="85"/>
       <c r="F5" s="62" t="s">
         <v>32</v>
       </c>
@@ -2125,12 +2134,12 @@
       <c r="EC5" s="17"/>
       <c r="ED5" s="18"/>
     </row>
-    <row r="6" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
+    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="61"/>
       <c r="G6" s="67"/>
       <c r="H6" s="22"/>
@@ -2261,18 +2270,18 @@
       <c r="EC6" s="17"/>
       <c r="ED6" s="18"/>
     </row>
-    <row r="7" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A7" s="86">
+    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A7" s="77">
         <v>2</v>
       </c>
-      <c r="B7" s="99"/>
-      <c r="C7" s="77" t="s">
+      <c r="B7" s="78"/>
+      <c r="C7" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="88" t="s">
+      <c r="D7" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="92"/>
       <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
@@ -2405,12 +2414,12 @@
       <c r="EC7" s="24"/>
       <c r="ED7" s="25"/>
     </row>
-    <row r="8" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="83"/>
+    <row r="8" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="94"/>
       <c r="F8" s="61"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -2541,12 +2550,12 @@
       <c r="EC8" s="27"/>
       <c r="ED8" s="28"/>
     </row>
-    <row r="9" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A9" s="86"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="83"/>
+    <row r="9" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="94"/>
       <c r="F9" s="62" t="s">
         <v>32</v>
       </c>
@@ -2679,12 +2688,12 @@
       <c r="EC9" s="27"/>
       <c r="ED9" s="28"/>
     </row>
-    <row r="10" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="85"/>
+    <row r="10" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="96"/>
       <c r="F10" s="61"/>
       <c r="G10" s="26"/>
       <c r="H10" s="27"/>
@@ -2815,18 +2824,18 @@
       <c r="EC10" s="27"/>
       <c r="ED10" s="28"/>
     </row>
-    <row r="11" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A11" s="86">
+    <row r="11" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A11" s="77">
         <v>3</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="90" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="D11" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="94"/>
+      <c r="E11" s="83"/>
       <c r="F11" s="60" t="s">
         <v>31</v>
       </c>
@@ -2959,12 +2968,12 @@
       <c r="EC11" s="11"/>
       <c r="ED11" s="12"/>
     </row>
-    <row r="12" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="96"/>
+    <row r="12" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A12" s="77"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="61"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3095,12 +3104,12 @@
       <c r="EC12" s="17"/>
       <c r="ED12" s="18"/>
     </row>
-    <row r="13" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="96"/>
+    <row r="13" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="62" t="s">
         <v>32</v>
       </c>
@@ -3233,12 +3242,12 @@
       <c r="EC13" s="17"/>
       <c r="ED13" s="18"/>
     </row>
-    <row r="14" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="98"/>
+    <row r="14" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A14" s="77"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="61"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3369,18 +3378,18 @@
       <c r="EC14" s="17"/>
       <c r="ED14" s="18"/>
     </row>
-    <row r="15" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A15" s="86">
+    <row r="15" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A15" s="77">
         <v>4</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="77" t="s">
+      <c r="B15" s="78"/>
+      <c r="C15" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="92"/>
       <c r="F15" s="60" t="s">
         <v>31</v>
       </c>
@@ -3513,12 +3522,12 @@
       <c r="EC15" s="24"/>
       <c r="ED15" s="25"/>
     </row>
-    <row r="16" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="83"/>
+    <row r="16" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A16" s="77"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="94"/>
       <c r="F16" s="61"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -3649,12 +3658,12 @@
       <c r="EC16" s="27"/>
       <c r="ED16" s="28"/>
     </row>
-    <row r="17" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A17" s="86"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="83"/>
+    <row r="17" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="94"/>
       <c r="F17" s="62" t="s">
         <v>32</v>
       </c>
@@ -3787,12 +3796,12 @@
       <c r="EC17" s="27"/>
       <c r="ED17" s="28"/>
     </row>
-    <row r="18" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A18" s="86"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="85"/>
+    <row r="18" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A18" s="77"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="96"/>
       <c r="F18" s="61"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27"/>
@@ -3923,18 +3932,18 @@
       <c r="EC18" s="27"/>
       <c r="ED18" s="28"/>
     </row>
-    <row r="19" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A19" s="86">
+    <row r="19" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A19" s="77">
         <v>5</v>
       </c>
-      <c r="B19" s="99"/>
-      <c r="C19" s="90" t="s">
+      <c r="B19" s="78"/>
+      <c r="C19" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="94"/>
+      <c r="E19" s="83"/>
       <c r="F19" s="60" t="s">
         <v>31</v>
       </c>
@@ -4067,12 +4076,12 @@
       <c r="EC19" s="11"/>
       <c r="ED19" s="12"/>
     </row>
-    <row r="20" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="96"/>
+    <row r="20" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A20" s="77"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
       <c r="F20" s="61"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -4203,12 +4212,12 @@
       <c r="EC20" s="17"/>
       <c r="ED20" s="18"/>
     </row>
-    <row r="21" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A21" s="86"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="96"/>
+    <row r="21" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A21" s="77"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="62" t="s">
         <v>32</v>
       </c>
@@ -4341,12 +4350,12 @@
       <c r="EC21" s="17"/>
       <c r="ED21" s="18"/>
     </row>
-    <row r="22" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A22" s="86"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="98"/>
+    <row r="22" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="61"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -4477,20 +4486,20 @@
       <c r="EC22" s="17"/>
       <c r="ED22" s="18"/>
     </row>
-    <row r="23" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A23" s="86">
+    <row r="23" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A23" s="77">
         <v>6</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="81"/>
+      <c r="E23" s="92"/>
       <c r="F23" s="60" t="s">
         <v>31</v>
       </c>
@@ -4623,12 +4632,12 @@
       <c r="EC23" s="24"/>
       <c r="ED23" s="25"/>
     </row>
-    <row r="24" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="83"/>
+    <row r="24" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A24" s="77"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="94"/>
       <c r="F24" s="61"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -4759,12 +4768,12 @@
       <c r="EC24" s="27"/>
       <c r="ED24" s="28"/>
     </row>
-    <row r="25" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="83"/>
+    <row r="25" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A25" s="77"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="94"/>
       <c r="F25" s="62" t="s">
         <v>32</v>
       </c>
@@ -4897,12 +4906,12 @@
       <c r="EC25" s="27"/>
       <c r="ED25" s="28"/>
     </row>
-    <row r="26" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A26" s="86"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
+    <row r="26" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A26" s="77"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="96"/>
       <c r="F26" s="61"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
@@ -5033,18 +5042,18 @@
       <c r="EC26" s="27"/>
       <c r="ED26" s="28"/>
     </row>
-    <row r="27" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A27" s="86">
+    <row r="27" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A27" s="77">
         <v>7</v>
       </c>
-      <c r="B27" s="87"/>
-      <c r="C27" s="90" t="s">
+      <c r="B27" s="97"/>
+      <c r="C27" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="93" t="s">
+      <c r="D27" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="94"/>
+      <c r="E27" s="83"/>
       <c r="F27" s="60" t="s">
         <v>31</v>
       </c>
@@ -5177,12 +5186,12 @@
       <c r="EC27" s="11"/>
       <c r="ED27" s="12"/>
     </row>
-    <row r="28" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A28" s="86"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="96"/>
+    <row r="28" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A28" s="77"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="61"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -5313,12 +5322,12 @@
       <c r="EC28" s="17"/>
       <c r="ED28" s="18"/>
     </row>
-    <row r="29" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A29" s="86"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="96"/>
+    <row r="29" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A29" s="77"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="85"/>
       <c r="F29" s="62" t="s">
         <v>32</v>
       </c>
@@ -5451,12 +5460,12 @@
       <c r="EC29" s="17"/>
       <c r="ED29" s="18"/>
     </row>
-    <row r="30" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A30" s="86"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="98"/>
+    <row r="30" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A30" s="77"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="87"/>
       <c r="F30" s="61"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5587,18 +5596,18 @@
       <c r="EC30" s="17"/>
       <c r="ED30" s="18"/>
     </row>
-    <row r="31" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A31" s="86">
+    <row r="31" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A31" s="77">
         <v>8</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="77" t="s">
+      <c r="B31" s="97"/>
+      <c r="C31" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="80" t="s">
+      <c r="D31" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="81"/>
+      <c r="E31" s="92"/>
       <c r="F31" s="60" t="s">
         <v>31</v>
       </c>
@@ -5731,12 +5740,12 @@
       <c r="EC31" s="24"/>
       <c r="ED31" s="25"/>
     </row>
-    <row r="32" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="83"/>
+    <row r="32" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A32" s="77"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="94"/>
       <c r="F32" s="61"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -5867,12 +5876,12 @@
       <c r="EC32" s="27"/>
       <c r="ED32" s="28"/>
     </row>
-    <row r="33" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="83"/>
+    <row r="33" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A33" s="77"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="94"/>
       <c r="F33" s="62" t="s">
         <v>32</v>
       </c>
@@ -5960,10 +5969,10 @@
       <c r="CJ33" s="27"/>
       <c r="CK33" s="27"/>
       <c r="CL33" s="27"/>
-      <c r="CM33" s="27"/>
-      <c r="CN33" s="27"/>
-      <c r="CO33" s="27"/>
-      <c r="CP33" s="28"/>
+      <c r="CM33" s="19"/>
+      <c r="CN33" s="19"/>
+      <c r="CO33" s="19"/>
+      <c r="CP33" s="30"/>
       <c r="CQ33" s="26"/>
       <c r="CR33" s="27"/>
       <c r="CS33" s="27"/>
@@ -6005,12 +6014,12 @@
       <c r="EC33" s="27"/>
       <c r="ED33" s="28"/>
     </row>
-    <row r="34" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A34" s="86"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="85"/>
+    <row r="34" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A34" s="77"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="96"/>
       <c r="F34" s="61"/>
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
@@ -6096,10 +6105,10 @@
       <c r="CJ34" s="27"/>
       <c r="CK34" s="27"/>
       <c r="CL34" s="27"/>
-      <c r="CM34" s="27"/>
-      <c r="CN34" s="27"/>
-      <c r="CO34" s="27"/>
-      <c r="CP34" s="28"/>
+      <c r="CM34" s="19"/>
+      <c r="CN34" s="19"/>
+      <c r="CO34" s="19"/>
+      <c r="CP34" s="30"/>
       <c r="CQ34" s="26"/>
       <c r="CR34" s="27"/>
       <c r="CS34" s="27"/>
@@ -6141,18 +6150,18 @@
       <c r="EC34" s="27"/>
       <c r="ED34" s="28"/>
     </row>
-    <row r="35" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A35" s="86">
+    <row r="35" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A35" s="77">
         <v>9</v>
       </c>
-      <c r="B35" s="87"/>
-      <c r="C35" s="90" t="s">
+      <c r="B35" s="97"/>
+      <c r="C35" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="93" t="s">
+      <c r="D35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="94"/>
+      <c r="E35" s="83"/>
       <c r="F35" s="60" t="s">
         <v>31</v>
       </c>
@@ -6285,12 +6294,12 @@
       <c r="EC35" s="11"/>
       <c r="ED35" s="12"/>
     </row>
-    <row r="36" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="96"/>
+    <row r="36" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A36" s="77"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85"/>
       <c r="F36" s="61"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -6421,12 +6430,12 @@
       <c r="EC36" s="17"/>
       <c r="ED36" s="18"/>
     </row>
-    <row r="37" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
-      <c r="B37" s="87"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="96"/>
+    <row r="37" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A37" s="77"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="85"/>
       <c r="F37" s="62" t="s">
         <v>32</v>
       </c>
@@ -6523,9 +6532,9 @@
       <c r="CS37" s="17"/>
       <c r="CT37" s="17"/>
       <c r="CU37" s="17"/>
-      <c r="CV37" s="17"/>
-      <c r="CW37" s="17"/>
-      <c r="CX37" s="18"/>
+      <c r="CV37" s="19"/>
+      <c r="CW37" s="19"/>
+      <c r="CX37" s="30"/>
       <c r="CY37" s="17"/>
       <c r="CZ37" s="17"/>
       <c r="DA37" s="17"/>
@@ -6559,12 +6568,12 @@
       <c r="EC37" s="17"/>
       <c r="ED37" s="18"/>
     </row>
-    <row r="38" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="97"/>
-      <c r="E38" s="98"/>
+    <row r="38" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A38" s="77"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="87"/>
       <c r="F38" s="61"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -6659,9 +6668,9 @@
       <c r="CS38" s="17"/>
       <c r="CT38" s="17"/>
       <c r="CU38" s="17"/>
-      <c r="CV38" s="17"/>
-      <c r="CW38" s="17"/>
-      <c r="CX38" s="18"/>
+      <c r="CV38" s="19"/>
+      <c r="CW38" s="19"/>
+      <c r="CX38" s="30"/>
       <c r="CY38" s="17"/>
       <c r="CZ38" s="17"/>
       <c r="DA38" s="17"/>
@@ -6695,16 +6704,16 @@
       <c r="EC38" s="17"/>
       <c r="ED38" s="18"/>
     </row>
-    <row r="39" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="77" t="s">
+      <c r="B39" s="97"/>
+      <c r="C39" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="80" t="s">
+      <c r="D39" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="81"/>
+      <c r="E39" s="92"/>
       <c r="F39" s="60" t="s">
         <v>31</v>
       </c>
@@ -6837,12 +6846,12 @@
       <c r="EC39" s="24"/>
       <c r="ED39" s="25"/>
     </row>
-    <row r="40" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
-      <c r="B40" s="87"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="94"/>
       <c r="F40" s="61"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -6973,12 +6982,12 @@
       <c r="EC40" s="27"/>
       <c r="ED40" s="28"/>
     </row>
-    <row r="41" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="87"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="83"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="99"/>
+      <c r="E41" s="94"/>
       <c r="F41" s="62" t="s">
         <v>32</v>
       </c>
@@ -7111,12 +7120,12 @@
       <c r="EC41" s="27"/>
       <c r="ED41" s="28"/>
     </row>
-    <row r="42" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
-      <c r="B42" s="87"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="85"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
       <c r="F42" s="61"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -7247,16 +7256,16 @@
       <c r="EC42" s="27"/>
       <c r="ED42" s="28"/>
     </row>
-    <row r="43" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
-      <c r="B43" s="87"/>
-      <c r="C43" s="90" t="s">
+      <c r="B43" s="97"/>
+      <c r="C43" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="93" t="s">
+      <c r="D43" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="94"/>
+      <c r="E43" s="83"/>
       <c r="F43" s="60" t="s">
         <v>31</v>
       </c>
@@ -7389,12 +7398,12 @@
       <c r="EC43" s="11"/>
       <c r="ED43" s="12"/>
     </row>
-    <row r="44" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
-      <c r="B44" s="87"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="96"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="85"/>
       <c r="F44" s="61"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -7525,12 +7534,12 @@
       <c r="EC44" s="17"/>
       <c r="ED44" s="18"/>
     </row>
-    <row r="45" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
-      <c r="B45" s="87"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="95"/>
-      <c r="E45" s="96"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="85"/>
       <c r="F45" s="62" t="s">
         <v>32</v>
       </c>
@@ -7643,9 +7652,9 @@
       <c r="DI45" s="17"/>
       <c r="DJ45" s="17"/>
       <c r="DK45" s="17"/>
-      <c r="DL45" s="17"/>
-      <c r="DM45" s="17"/>
-      <c r="DN45" s="18"/>
+      <c r="DL45" s="19"/>
+      <c r="DM45" s="19"/>
+      <c r="DN45" s="30"/>
       <c r="DO45" s="17"/>
       <c r="DP45" s="17"/>
       <c r="DQ45" s="17"/>
@@ -7663,12 +7672,12 @@
       <c r="EC45" s="17"/>
       <c r="ED45" s="18"/>
     </row>
-    <row r="46" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
-      <c r="B46" s="87"/>
-      <c r="C46" s="92"/>
-      <c r="D46" s="97"/>
-      <c r="E46" s="98"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="87"/>
       <c r="F46" s="61"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -7779,9 +7788,9 @@
       <c r="DI46" s="17"/>
       <c r="DJ46" s="17"/>
       <c r="DK46" s="17"/>
-      <c r="DL46" s="17"/>
-      <c r="DM46" s="17"/>
-      <c r="DN46" s="18"/>
+      <c r="DL46" s="19"/>
+      <c r="DM46" s="19"/>
+      <c r="DN46" s="30"/>
       <c r="DO46" s="17"/>
       <c r="DP46" s="17"/>
       <c r="DQ46" s="17"/>
@@ -7799,16 +7808,16 @@
       <c r="EC46" s="17"/>
       <c r="ED46" s="18"/>
     </row>
-    <row r="47" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
-      <c r="B47" s="87"/>
-      <c r="C47" s="77" t="s">
+      <c r="B47" s="97"/>
+      <c r="C47" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="80" t="s">
+      <c r="D47" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="81"/>
+      <c r="E47" s="92"/>
       <c r="F47" s="60" t="s">
         <v>31</v>
       </c>
@@ -7941,12 +7950,12 @@
       <c r="EC47" s="24"/>
       <c r="ED47" s="25"/>
     </row>
-    <row r="48" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
-      <c r="B48" s="87"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
+      <c r="B48" s="97"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="94"/>
       <c r="F48" s="61"/>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -8077,12 +8086,12 @@
       <c r="EC48" s="27"/>
       <c r="ED48" s="28"/>
     </row>
-    <row r="49" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
-      <c r="B49" s="87"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="83"/>
+      <c r="B49" s="97"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="94"/>
       <c r="F49" s="62" t="s">
         <v>32</v>
       </c>
@@ -8215,12 +8224,12 @@
       <c r="EC49" s="27"/>
       <c r="ED49" s="28"/>
     </row>
-    <row r="50" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
-      <c r="B50" s="87"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="85"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="96"/>
       <c r="F50" s="61"/>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -8351,16 +8360,16 @@
       <c r="EC50" s="27"/>
       <c r="ED50" s="28"/>
     </row>
-    <row r="51" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
-      <c r="B51" s="87"/>
+      <c r="B51" s="97"/>
       <c r="C51" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="93" t="s">
+      <c r="D51" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="94"/>
+      <c r="E51" s="83"/>
       <c r="F51" s="60" t="s">
         <v>31</v>
       </c>
@@ -8493,12 +8502,12 @@
       <c r="EC51" s="11"/>
       <c r="ED51" s="12"/>
     </row>
-    <row r="52" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
-      <c r="B52" s="87"/>
+      <c r="B52" s="97"/>
       <c r="C52" s="53"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="96"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="85"/>
       <c r="F52" s="61"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
@@ -8629,12 +8638,12 @@
       <c r="EC52" s="17"/>
       <c r="ED52" s="18"/>
     </row>
-    <row r="53" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
-      <c r="B53" s="87"/>
+      <c r="B53" s="97"/>
       <c r="C53" s="53"/>
-      <c r="D53" s="95"/>
-      <c r="E53" s="96"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="85"/>
       <c r="F53" s="62" t="s">
         <v>32</v>
       </c>
@@ -8767,12 +8776,12 @@
       <c r="EC53" s="17"/>
       <c r="ED53" s="18"/>
     </row>
-    <row r="54" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
-      <c r="B54" s="87"/>
+      <c r="B54" s="97"/>
       <c r="C54" s="54"/>
-      <c r="D54" s="97"/>
-      <c r="E54" s="98"/>
+      <c r="D54" s="86"/>
+      <c r="E54" s="87"/>
       <c r="F54" s="61"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -8903,16 +8912,16 @@
       <c r="EC54" s="17"/>
       <c r="ED54" s="18"/>
     </row>
-    <row r="55" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
-      <c r="B55" s="87"/>
+      <c r="B55" s="97"/>
       <c r="C55" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="80" t="s">
+      <c r="D55" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="81"/>
+      <c r="E55" s="92"/>
       <c r="F55" s="60" t="s">
         <v>31</v>
       </c>
@@ -9045,12 +9054,12 @@
       <c r="EC55" s="24"/>
       <c r="ED55" s="25"/>
     </row>
-    <row r="56" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
-      <c r="B56" s="87"/>
+      <c r="B56" s="97"/>
       <c r="C56" s="56"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="83"/>
+      <c r="D56" s="99"/>
+      <c r="E56" s="94"/>
       <c r="F56" s="61"/>
       <c r="G56" s="26"/>
       <c r="H56" s="27"/>
@@ -9181,12 +9190,12 @@
       <c r="EC56" s="27"/>
       <c r="ED56" s="28"/>
     </row>
-    <row r="57" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
-      <c r="B57" s="87"/>
+      <c r="B57" s="97"/>
       <c r="C57" s="56"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="83"/>
+      <c r="D57" s="99"/>
+      <c r="E57" s="94"/>
       <c r="F57" s="62" t="s">
         <v>32</v>
       </c>
@@ -9319,12 +9328,12 @@
       <c r="EC57" s="27"/>
       <c r="ED57" s="28"/>
     </row>
-    <row r="58" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
-      <c r="B58" s="87"/>
+      <c r="B58" s="97"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="85"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="96"/>
       <c r="F58" s="61"/>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -9455,16 +9464,16 @@
       <c r="EC58" s="27"/>
       <c r="ED58" s="28"/>
     </row>
-    <row r="59" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A59" s="51"/>
-      <c r="B59" s="87"/>
+      <c r="B59" s="97"/>
       <c r="C59" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="93" t="s">
+      <c r="D59" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="94"/>
+      <c r="E59" s="83"/>
       <c r="F59" s="60" t="s">
         <v>31</v>
       </c>
@@ -9597,12 +9606,12 @@
       <c r="EC59" s="11"/>
       <c r="ED59" s="12"/>
     </row>
-    <row r="60" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A60" s="51"/>
-      <c r="B60" s="87"/>
+      <c r="B60" s="97"/>
       <c r="C60" s="53"/>
-      <c r="D60" s="95"/>
-      <c r="E60" s="96"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="85"/>
       <c r="F60" s="61"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -9733,12 +9742,12 @@
       <c r="EC60" s="17"/>
       <c r="ED60" s="18"/>
     </row>
-    <row r="61" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
-      <c r="B61" s="87"/>
+      <c r="B61" s="97"/>
       <c r="C61" s="53"/>
-      <c r="D61" s="95"/>
-      <c r="E61" s="96"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="85"/>
       <c r="F61" s="62" t="s">
         <v>32</v>
       </c>
@@ -9871,12 +9880,12 @@
       <c r="EC61" s="17"/>
       <c r="ED61" s="18"/>
     </row>
-    <row r="62" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
-      <c r="B62" s="87"/>
+      <c r="B62" s="97"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="98"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="87"/>
       <c r="F62" s="61"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -10007,12 +10016,14 @@
       <c r="EC62" s="17"/>
       <c r="ED62" s="18"/>
     </row>
-    <row r="63" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
-      <c r="B63" s="87"/>
-      <c r="C63" s="77"/>
-      <c r="D63" s="80"/>
-      <c r="E63" s="81"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="98"/>
+      <c r="E63" s="92"/>
       <c r="F63" s="60" t="s">
         <v>31</v>
       </c>
@@ -10125,14 +10136,14 @@
       <c r="DI63" s="24"/>
       <c r="DJ63" s="24"/>
       <c r="DK63" s="24"/>
-      <c r="DL63" s="14"/>
-      <c r="DM63" s="14"/>
-      <c r="DN63" s="50"/>
-      <c r="DO63" s="13"/>
-      <c r="DP63" s="14"/>
-      <c r="DQ63" s="14"/>
-      <c r="DR63" s="14"/>
-      <c r="DS63" s="14"/>
+      <c r="DL63" s="109"/>
+      <c r="DM63" s="109"/>
+      <c r="DN63" s="110"/>
+      <c r="DO63" s="111"/>
+      <c r="DP63" s="109"/>
+      <c r="DQ63" s="109"/>
+      <c r="DR63" s="109"/>
+      <c r="DS63" s="109"/>
       <c r="DT63" s="24"/>
       <c r="DU63" s="24"/>
       <c r="DV63" s="25"/>
@@ -10145,12 +10156,12 @@
       <c r="EC63" s="24"/>
       <c r="ED63" s="25"/>
     </row>
-    <row r="64" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
-      <c r="B64" s="87"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="83"/>
+      <c r="B64" s="97"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="94"/>
       <c r="F64" s="61"/>
       <c r="G64" s="26"/>
       <c r="H64" s="27"/>
@@ -10261,14 +10272,14 @@
       <c r="DI64" s="27"/>
       <c r="DJ64" s="27"/>
       <c r="DK64" s="27"/>
-      <c r="DL64" s="21"/>
-      <c r="DM64" s="21"/>
-      <c r="DN64" s="31"/>
-      <c r="DO64" s="29"/>
-      <c r="DP64" s="21"/>
-      <c r="DQ64" s="21"/>
-      <c r="DR64" s="21"/>
-      <c r="DS64" s="21"/>
+      <c r="DL64" s="107"/>
+      <c r="DM64" s="107"/>
+      <c r="DN64" s="108"/>
+      <c r="DO64" s="112"/>
+      <c r="DP64" s="107"/>
+      <c r="DQ64" s="107"/>
+      <c r="DR64" s="107"/>
+      <c r="DS64" s="107"/>
       <c r="DT64" s="27"/>
       <c r="DU64" s="27"/>
       <c r="DV64" s="28"/>
@@ -10281,12 +10292,12 @@
       <c r="EC64" s="27"/>
       <c r="ED64" s="28"/>
     </row>
-    <row r="65" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
-      <c r="B65" s="87"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="82"/>
-      <c r="E65" s="83"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="99"/>
+      <c r="E65" s="94"/>
       <c r="F65" s="62" t="s">
         <v>32</v>
       </c>
@@ -10386,19 +10397,19 @@
       <c r="CV65" s="27"/>
       <c r="CW65" s="27"/>
       <c r="CX65" s="28"/>
-      <c r="CY65" s="26"/>
-      <c r="CZ65" s="27"/>
-      <c r="DA65" s="27"/>
-      <c r="DB65" s="27"/>
-      <c r="DC65" s="27"/>
-      <c r="DD65" s="27"/>
-      <c r="DE65" s="27"/>
-      <c r="DF65" s="28"/>
-      <c r="DG65" s="26"/>
-      <c r="DH65" s="27"/>
-      <c r="DI65" s="27"/>
-      <c r="DJ65" s="27"/>
-      <c r="DK65" s="27"/>
+      <c r="CY65" s="68"/>
+      <c r="CZ65" s="19"/>
+      <c r="DA65" s="19"/>
+      <c r="DB65" s="19"/>
+      <c r="DC65" s="19"/>
+      <c r="DD65" s="19"/>
+      <c r="DE65" s="19"/>
+      <c r="DF65" s="30"/>
+      <c r="DG65" s="68"/>
+      <c r="DH65" s="19"/>
+      <c r="DI65" s="19"/>
+      <c r="DJ65" s="19"/>
+      <c r="DK65" s="19"/>
       <c r="DL65" s="27"/>
       <c r="DM65" s="27"/>
       <c r="DN65" s="28"/>
@@ -10419,12 +10430,12 @@
       <c r="EC65" s="27"/>
       <c r="ED65" s="28"/>
     </row>
-    <row r="66" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
-      <c r="B66" s="87"/>
-      <c r="C66" s="79"/>
-      <c r="D66" s="84"/>
-      <c r="E66" s="85"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="90"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="96"/>
       <c r="F66" s="61"/>
       <c r="G66" s="26"/>
       <c r="H66" s="27"/>
@@ -10522,19 +10533,19 @@
       <c r="CV66" s="27"/>
       <c r="CW66" s="27"/>
       <c r="CX66" s="28"/>
-      <c r="CY66" s="26"/>
-      <c r="CZ66" s="27"/>
-      <c r="DA66" s="27"/>
-      <c r="DB66" s="27"/>
-      <c r="DC66" s="27"/>
-      <c r="DD66" s="27"/>
-      <c r="DE66" s="27"/>
-      <c r="DF66" s="28"/>
-      <c r="DG66" s="26"/>
-      <c r="DH66" s="27"/>
-      <c r="DI66" s="27"/>
-      <c r="DJ66" s="27"/>
-      <c r="DK66" s="27"/>
+      <c r="CY66" s="68"/>
+      <c r="CZ66" s="19"/>
+      <c r="DA66" s="19"/>
+      <c r="DB66" s="19"/>
+      <c r="DC66" s="19"/>
+      <c r="DD66" s="19"/>
+      <c r="DE66" s="19"/>
+      <c r="DF66" s="30"/>
+      <c r="DG66" s="68"/>
+      <c r="DH66" s="19"/>
+      <c r="DI66" s="19"/>
+      <c r="DJ66" s="19"/>
+      <c r="DK66" s="19"/>
       <c r="DL66" s="27"/>
       <c r="DM66" s="27"/>
       <c r="DN66" s="28"/>
@@ -10555,12 +10566,12 @@
       <c r="EC66" s="27"/>
       <c r="ED66" s="28"/>
     </row>
-    <row r="67" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A67" s="51"/>
-      <c r="B67" s="87"/>
-      <c r="C67" s="90"/>
-      <c r="D67" s="93"/>
-      <c r="E67" s="94"/>
+      <c r="B67" s="97"/>
+      <c r="C67" s="79"/>
+      <c r="D67" s="82"/>
+      <c r="E67" s="83"/>
       <c r="F67" s="60" t="s">
         <v>31</v>
       </c>
@@ -10693,12 +10704,12 @@
       <c r="EC67" s="11"/>
       <c r="ED67" s="12"/>
     </row>
-    <row r="68" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A68" s="51"/>
-      <c r="B68" s="87"/>
-      <c r="C68" s="91"/>
-      <c r="D68" s="95"/>
-      <c r="E68" s="96"/>
+      <c r="B68" s="97"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="85"/>
       <c r="F68" s="61"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -10829,12 +10840,12 @@
       <c r="EC68" s="17"/>
       <c r="ED68" s="18"/>
     </row>
-    <row r="69" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A69" s="51"/>
-      <c r="B69" s="87"/>
-      <c r="C69" s="91"/>
-      <c r="D69" s="95"/>
-      <c r="E69" s="96"/>
+      <c r="B69" s="97"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="85"/>
       <c r="F69" s="62" t="s">
         <v>32</v>
       </c>
@@ -10967,12 +10978,12 @@
       <c r="EC69" s="17"/>
       <c r="ED69" s="18"/>
     </row>
-    <row r="70" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A70" s="51"/>
-      <c r="B70" s="87"/>
-      <c r="C70" s="92"/>
-      <c r="D70" s="97"/>
-      <c r="E70" s="98"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="86"/>
+      <c r="E70" s="87"/>
       <c r="F70" s="61"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -11103,12 +11114,12 @@
       <c r="EC70" s="17"/>
       <c r="ED70" s="18"/>
     </row>
-    <row r="71" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A71" s="51"/>
-      <c r="B71" s="87"/>
-      <c r="C71" s="77"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="81"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="88"/>
+      <c r="D71" s="98"/>
+      <c r="E71" s="92"/>
       <c r="F71" s="60" t="s">
         <v>31</v>
       </c>
@@ -11241,12 +11252,12 @@
       <c r="EC71" s="24"/>
       <c r="ED71" s="25"/>
     </row>
-    <row r="72" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A72" s="51"/>
-      <c r="B72" s="87"/>
-      <c r="C72" s="78"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="83"/>
+      <c r="B72" s="97"/>
+      <c r="C72" s="89"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="94"/>
       <c r="F72" s="61"/>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
@@ -11377,12 +11388,12 @@
       <c r="EC72" s="27"/>
       <c r="ED72" s="28"/>
     </row>
-    <row r="73" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
-      <c r="B73" s="87"/>
-      <c r="C73" s="78"/>
-      <c r="D73" s="82"/>
-      <c r="E73" s="83"/>
+      <c r="B73" s="97"/>
+      <c r="C73" s="89"/>
+      <c r="D73" s="99"/>
+      <c r="E73" s="94"/>
       <c r="F73" s="62" t="s">
         <v>32</v>
       </c>
@@ -11515,12 +11526,12 @@
       <c r="EC73" s="27"/>
       <c r="ED73" s="28"/>
     </row>
-    <row r="74" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A74" s="51"/>
-      <c r="B74" s="87"/>
-      <c r="C74" s="79"/>
-      <c r="D74" s="84"/>
-      <c r="E74" s="85"/>
+      <c r="B74" s="97"/>
+      <c r="C74" s="90"/>
+      <c r="D74" s="95"/>
+      <c r="E74" s="96"/>
       <c r="F74" s="61"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -11651,12 +11662,12 @@
       <c r="EC74" s="27"/>
       <c r="ED74" s="28"/>
     </row>
-    <row r="75" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A75" s="51"/>
-      <c r="B75" s="87"/>
-      <c r="C75" s="90"/>
-      <c r="D75" s="93"/>
-      <c r="E75" s="94"/>
+      <c r="B75" s="97"/>
+      <c r="C75" s="79"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="83"/>
       <c r="F75" s="60" t="s">
         <v>31</v>
       </c>
@@ -11789,12 +11800,12 @@
       <c r="EC75" s="11"/>
       <c r="ED75" s="12"/>
     </row>
-    <row r="76" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A76" s="51"/>
-      <c r="B76" s="87"/>
-      <c r="C76" s="91"/>
-      <c r="D76" s="95"/>
-      <c r="E76" s="96"/>
+      <c r="B76" s="97"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="85"/>
       <c r="F76" s="61"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -11925,12 +11936,12 @@
       <c r="EC76" s="17"/>
       <c r="ED76" s="18"/>
     </row>
-    <row r="77" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A77" s="51"/>
-      <c r="B77" s="87"/>
-      <c r="C77" s="91"/>
-      <c r="D77" s="95"/>
-      <c r="E77" s="96"/>
+      <c r="B77" s="97"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="85"/>
       <c r="F77" s="62" t="s">
         <v>32</v>
       </c>
@@ -12063,12 +12074,12 @@
       <c r="EC77" s="17"/>
       <c r="ED77" s="18"/>
     </row>
-    <row r="78" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
-      <c r="B78" s="87"/>
-      <c r="C78" s="92"/>
-      <c r="D78" s="97"/>
-      <c r="E78" s="98"/>
+      <c r="B78" s="97"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="87"/>
       <c r="F78" s="61"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -12199,20 +12210,20 @@
       <c r="EC78" s="17"/>
       <c r="ED78" s="18"/>
     </row>
-    <row r="79" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A79" s="86">
+    <row r="79" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A79" s="77">
         <v>11</v>
       </c>
-      <c r="B79" s="99" t="s">
+      <c r="B79" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="77" t="s">
+      <c r="C79" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="80" t="s">
+      <c r="D79" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E79" s="81"/>
+      <c r="E79" s="92"/>
       <c r="F79" s="60" t="s">
         <v>31</v>
       </c>
@@ -12345,12 +12356,12 @@
       <c r="EC79" s="24"/>
       <c r="ED79" s="25"/>
     </row>
-    <row r="80" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A80" s="86"/>
-      <c r="B80" s="99"/>
-      <c r="C80" s="78"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="83"/>
+    <row r="80" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A80" s="77"/>
+      <c r="B80" s="78"/>
+      <c r="C80" s="89"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="94"/>
       <c r="F80" s="61"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12481,12 +12492,12 @@
       <c r="EC80" s="27"/>
       <c r="ED80" s="28"/>
     </row>
-    <row r="81" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A81" s="86"/>
-      <c r="B81" s="99"/>
-      <c r="C81" s="78"/>
-      <c r="D81" s="82"/>
-      <c r="E81" s="83"/>
+    <row r="81" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A81" s="77"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="89"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="94"/>
       <c r="F81" s="62" t="s">
         <v>32</v>
       </c>
@@ -12574,10 +12585,10 @@
       <c r="CJ81" s="27"/>
       <c r="CK81" s="27"/>
       <c r="CL81" s="27"/>
-      <c r="CM81" s="19"/>
-      <c r="CN81" s="19"/>
-      <c r="CO81" s="19"/>
-      <c r="CP81" s="30"/>
+      <c r="CM81" s="107"/>
+      <c r="CN81" s="107"/>
+      <c r="CO81" s="107"/>
+      <c r="CP81" s="108"/>
       <c r="CQ81" s="27"/>
       <c r="CR81" s="27"/>
       <c r="CS81" s="27"/>
@@ -12619,12 +12630,12 @@
       <c r="EC81" s="27"/>
       <c r="ED81" s="28"/>
     </row>
-    <row r="82" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A82" s="86"/>
-      <c r="B82" s="99"/>
-      <c r="C82" s="79"/>
-      <c r="D82" s="84"/>
-      <c r="E82" s="85"/>
+    <row r="82" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A82" s="77"/>
+      <c r="B82" s="78"/>
+      <c r="C82" s="90"/>
+      <c r="D82" s="95"/>
+      <c r="E82" s="96"/>
       <c r="F82" s="61"/>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
@@ -12710,10 +12721,10 @@
       <c r="CJ82" s="27"/>
       <c r="CK82" s="27"/>
       <c r="CL82" s="27"/>
-      <c r="CM82" s="19"/>
-      <c r="CN82" s="19"/>
-      <c r="CO82" s="19"/>
-      <c r="CP82" s="30"/>
+      <c r="CM82" s="107"/>
+      <c r="CN82" s="107"/>
+      <c r="CO82" s="107"/>
+      <c r="CP82" s="108"/>
       <c r="CQ82" s="27"/>
       <c r="CR82" s="27"/>
       <c r="CS82" s="27"/>
@@ -12755,16 +12766,16 @@
       <c r="EC82" s="27"/>
       <c r="ED82" s="28"/>
     </row>
-    <row r="83" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A83" s="51"/>
-      <c r="B83" s="99"/>
-      <c r="C83" s="90" t="s">
+      <c r="B83" s="78"/>
+      <c r="C83" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="93" t="s">
+      <c r="D83" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E83" s="94"/>
+      <c r="E83" s="83"/>
       <c r="F83" s="60" t="s">
         <v>31</v>
       </c>
@@ -12897,12 +12908,12 @@
       <c r="EC83" s="11"/>
       <c r="ED83" s="12"/>
     </row>
-    <row r="84" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A84" s="51"/>
-      <c r="B84" s="99"/>
-      <c r="C84" s="91"/>
-      <c r="D84" s="95"/>
-      <c r="E84" s="96"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="85"/>
       <c r="F84" s="61"/>
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
@@ -13033,12 +13044,12 @@
       <c r="EC84" s="17"/>
       <c r="ED84" s="18"/>
     </row>
-    <row r="85" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A85" s="51"/>
-      <c r="B85" s="99"/>
-      <c r="C85" s="91"/>
-      <c r="D85" s="95"/>
-      <c r="E85" s="96"/>
+      <c r="B85" s="78"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="85"/>
       <c r="F85" s="62" t="s">
         <v>32</v>
       </c>
@@ -13171,12 +13182,12 @@
       <c r="EC85" s="17"/>
       <c r="ED85" s="18"/>
     </row>
-    <row r="86" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A86" s="51"/>
-      <c r="B86" s="99"/>
-      <c r="C86" s="92"/>
-      <c r="D86" s="97"/>
-      <c r="E86" s="98"/>
+      <c r="B86" s="78"/>
+      <c r="C86" s="81"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="87"/>
       <c r="F86" s="61"/>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -13307,16 +13318,16 @@
       <c r="EC86" s="17"/>
       <c r="ED86" s="18"/>
     </row>
-    <row r="87" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A87" s="51"/>
-      <c r="B87" s="99"/>
-      <c r="C87" s="77" t="s">
+      <c r="B87" s="78"/>
+      <c r="C87" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D87" s="80" t="s">
+      <c r="D87" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="81"/>
+      <c r="E87" s="92"/>
       <c r="F87" s="60" t="s">
         <v>31</v>
       </c>
@@ -13449,12 +13460,12 @@
       <c r="EC87" s="24"/>
       <c r="ED87" s="25"/>
     </row>
-    <row r="88" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A88" s="51"/>
-      <c r="B88" s="99"/>
-      <c r="C88" s="78"/>
-      <c r="D88" s="82"/>
-      <c r="E88" s="83"/>
+      <c r="B88" s="78"/>
+      <c r="C88" s="89"/>
+      <c r="D88" s="99"/>
+      <c r="E88" s="94"/>
       <c r="F88" s="61"/>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -13585,12 +13596,12 @@
       <c r="EC88" s="27"/>
       <c r="ED88" s="28"/>
     </row>
-    <row r="89" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A89" s="51"/>
-      <c r="B89" s="99"/>
-      <c r="C89" s="78"/>
-      <c r="D89" s="82"/>
-      <c r="E89" s="83"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="89"/>
+      <c r="D89" s="99"/>
+      <c r="E89" s="94"/>
       <c r="F89" s="62" t="s">
         <v>32</v>
       </c>
@@ -13678,8 +13689,8 @@
       <c r="CJ89" s="27"/>
       <c r="CK89" s="27"/>
       <c r="CL89" s="27"/>
-      <c r="CM89" s="19"/>
-      <c r="CN89" s="19"/>
+      <c r="CM89" s="27"/>
+      <c r="CN89" s="27"/>
       <c r="CO89" s="19"/>
       <c r="CP89" s="30"/>
       <c r="CQ89" s="27"/>
@@ -13696,8 +13707,8 @@
       <c r="DB89" s="27"/>
       <c r="DC89" s="27"/>
       <c r="DD89" s="27"/>
-      <c r="DE89" s="27"/>
-      <c r="DF89" s="28"/>
+      <c r="DE89" s="19"/>
+      <c r="DF89" s="30"/>
       <c r="DG89" s="27"/>
       <c r="DH89" s="27"/>
       <c r="DI89" s="27"/>
@@ -13723,12 +13734,12 @@
       <c r="EC89" s="27"/>
       <c r="ED89" s="28"/>
     </row>
-    <row r="90" spans="1:134" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
-      <c r="B90" s="99"/>
-      <c r="C90" s="79"/>
-      <c r="D90" s="84"/>
-      <c r="E90" s="85"/>
+      <c r="B90" s="78"/>
+      <c r="C90" s="90"/>
+      <c r="D90" s="95"/>
+      <c r="E90" s="96"/>
       <c r="F90" s="61"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -13814,8 +13825,8 @@
       <c r="CJ90" s="27"/>
       <c r="CK90" s="27"/>
       <c r="CL90" s="27"/>
-      <c r="CM90" s="19"/>
-      <c r="CN90" s="19"/>
+      <c r="CM90" s="27"/>
+      <c r="CN90" s="27"/>
       <c r="CO90" s="19"/>
       <c r="CP90" s="30"/>
       <c r="CQ90" s="27"/>
@@ -13832,8 +13843,8 @@
       <c r="DB90" s="27"/>
       <c r="DC90" s="27"/>
       <c r="DD90" s="27"/>
-      <c r="DE90" s="27"/>
-      <c r="DF90" s="28"/>
+      <c r="DE90" s="19"/>
+      <c r="DF90" s="30"/>
       <c r="DG90" s="27"/>
       <c r="DH90" s="27"/>
       <c r="DI90" s="27"/>
@@ -13859,18 +13870,18 @@
       <c r="EC90" s="27"/>
       <c r="ED90" s="28"/>
     </row>
-    <row r="91" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A91" s="86">
+    <row r="91" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A91" s="77">
         <v>13</v>
       </c>
-      <c r="B91" s="99"/>
-      <c r="C91" s="90" t="s">
+      <c r="B91" s="78"/>
+      <c r="C91" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="93" t="s">
+      <c r="D91" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E91" s="94"/>
+      <c r="E91" s="83"/>
       <c r="F91" s="60" t="s">
         <v>31</v>
       </c>
@@ -14003,12 +14014,12 @@
       <c r="EC91" s="11"/>
       <c r="ED91" s="12"/>
     </row>
-    <row r="92" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A92" s="86"/>
-      <c r="B92" s="99"/>
-      <c r="C92" s="91"/>
-      <c r="D92" s="95"/>
-      <c r="E92" s="96"/>
+    <row r="92" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A92" s="77"/>
+      <c r="B92" s="78"/>
+      <c r="C92" s="80"/>
+      <c r="D92" s="84"/>
+      <c r="E92" s="85"/>
       <c r="F92" s="61"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -14139,12 +14150,12 @@
       <c r="EC92" s="17"/>
       <c r="ED92" s="18"/>
     </row>
-    <row r="93" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A93" s="86"/>
-      <c r="B93" s="99"/>
-      <c r="C93" s="91"/>
-      <c r="D93" s="95"/>
-      <c r="E93" s="96"/>
+    <row r="93" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A93" s="77"/>
+      <c r="B93" s="78"/>
+      <c r="C93" s="80"/>
+      <c r="D93" s="84"/>
+      <c r="E93" s="85"/>
       <c r="F93" s="62" t="s">
         <v>32</v>
       </c>
@@ -14277,12 +14288,12 @@
       <c r="EC93" s="17"/>
       <c r="ED93" s="18"/>
     </row>
-    <row r="94" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A94" s="86"/>
-      <c r="B94" s="99"/>
-      <c r="C94" s="92"/>
-      <c r="D94" s="97"/>
-      <c r="E94" s="98"/>
+    <row r="94" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A94" s="77"/>
+      <c r="B94" s="78"/>
+      <c r="C94" s="81"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="87"/>
       <c r="F94" s="61"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17"/>
@@ -14413,20 +14424,20 @@
       <c r="EC94" s="17"/>
       <c r="ED94" s="18"/>
     </row>
-    <row r="95" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A95" s="86">
+    <row r="95" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A95" s="77">
         <v>14</v>
       </c>
-      <c r="B95" s="87" t="s">
+      <c r="B95" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="77" t="s">
+      <c r="C95" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="88" t="s">
+      <c r="D95" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="81"/>
+      <c r="E95" s="92"/>
       <c r="F95" s="60" t="s">
         <v>31</v>
       </c>
@@ -14559,12 +14570,12 @@
       <c r="EC95" s="24"/>
       <c r="ED95" s="25"/>
     </row>
-    <row r="96" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A96" s="86"/>
-      <c r="B96" s="87"/>
-      <c r="C96" s="78"/>
-      <c r="D96" s="89"/>
-      <c r="E96" s="83"/>
+    <row r="96" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A96" s="77"/>
+      <c r="B96" s="97"/>
+      <c r="C96" s="89"/>
+      <c r="D96" s="93"/>
+      <c r="E96" s="94"/>
       <c r="F96" s="61"/>
       <c r="G96" s="26"/>
       <c r="H96" s="27"/>
@@ -14695,12 +14706,12 @@
       <c r="EC96" s="27"/>
       <c r="ED96" s="28"/>
     </row>
-    <row r="97" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A97" s="86"/>
-      <c r="B97" s="87"/>
-      <c r="C97" s="78"/>
-      <c r="D97" s="89"/>
-      <c r="E97" s="83"/>
+    <row r="97" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A97" s="77"/>
+      <c r="B97" s="97"/>
+      <c r="C97" s="89"/>
+      <c r="D97" s="93"/>
+      <c r="E97" s="94"/>
       <c r="F97" s="62" t="s">
         <v>32</v>
       </c>
@@ -14816,14 +14827,14 @@
       <c r="DL97" s="27"/>
       <c r="DM97" s="27"/>
       <c r="DN97" s="28"/>
-      <c r="DO97" s="26"/>
-      <c r="DP97" s="27"/>
-      <c r="DQ97" s="27"/>
-      <c r="DR97" s="27"/>
-      <c r="DS97" s="27"/>
-      <c r="DT97" s="27"/>
-      <c r="DU97" s="27"/>
-      <c r="DV97" s="28"/>
+      <c r="DO97" s="68"/>
+      <c r="DP97" s="19"/>
+      <c r="DQ97" s="19"/>
+      <c r="DR97" s="19"/>
+      <c r="DS97" s="19"/>
+      <c r="DT97" s="19"/>
+      <c r="DU97" s="19"/>
+      <c r="DV97" s="30"/>
       <c r="DW97" s="26"/>
       <c r="DX97" s="27"/>
       <c r="DY97" s="27"/>
@@ -14833,12 +14844,12 @@
       <c r="EC97" s="27"/>
       <c r="ED97" s="28"/>
     </row>
-    <row r="98" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A98" s="86"/>
-      <c r="B98" s="87"/>
-      <c r="C98" s="79"/>
-      <c r="D98" s="84"/>
-      <c r="E98" s="85"/>
+    <row r="98" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A98" s="77"/>
+      <c r="B98" s="97"/>
+      <c r="C98" s="90"/>
+      <c r="D98" s="95"/>
+      <c r="E98" s="96"/>
       <c r="F98" s="61"/>
       <c r="G98" s="26"/>
       <c r="H98" s="27"/>
@@ -14952,14 +14963,14 @@
       <c r="DL98" s="27"/>
       <c r="DM98" s="27"/>
       <c r="DN98" s="28"/>
-      <c r="DO98" s="26"/>
-      <c r="DP98" s="27"/>
-      <c r="DQ98" s="27"/>
-      <c r="DR98" s="27"/>
-      <c r="DS98" s="27"/>
-      <c r="DT98" s="27"/>
-      <c r="DU98" s="27"/>
-      <c r="DV98" s="28"/>
+      <c r="DO98" s="68"/>
+      <c r="DP98" s="19"/>
+      <c r="DQ98" s="19"/>
+      <c r="DR98" s="19"/>
+      <c r="DS98" s="19"/>
+      <c r="DT98" s="19"/>
+      <c r="DU98" s="19"/>
+      <c r="DV98" s="30"/>
       <c r="DW98" s="26"/>
       <c r="DX98" s="27"/>
       <c r="DY98" s="27"/>
@@ -14969,18 +14980,18 @@
       <c r="EC98" s="27"/>
       <c r="ED98" s="28"/>
     </row>
-    <row r="99" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A99" s="86">
+    <row r="99" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A99" s="77">
         <v>15</v>
       </c>
-      <c r="B99" s="87"/>
-      <c r="C99" s="90" t="s">
+      <c r="B99" s="97"/>
+      <c r="C99" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="93" t="s">
+      <c r="D99" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E99" s="94"/>
+      <c r="E99" s="83"/>
       <c r="F99" s="60" t="s">
         <v>31</v>
       </c>
@@ -15113,12 +15124,12 @@
       <c r="EC99" s="11"/>
       <c r="ED99" s="12"/>
     </row>
-    <row r="100" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A100" s="86"/>
-      <c r="B100" s="87"/>
-      <c r="C100" s="91"/>
-      <c r="D100" s="95"/>
-      <c r="E100" s="96"/>
+    <row r="100" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A100" s="77"/>
+      <c r="B100" s="97"/>
+      <c r="C100" s="80"/>
+      <c r="D100" s="84"/>
+      <c r="E100" s="85"/>
       <c r="F100" s="61"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -15249,12 +15260,12 @@
       <c r="EC100" s="17"/>
       <c r="ED100" s="18"/>
     </row>
-    <row r="101" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A101" s="86"/>
-      <c r="B101" s="87"/>
-      <c r="C101" s="91"/>
-      <c r="D101" s="95"/>
-      <c r="E101" s="96"/>
+    <row r="101" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A101" s="77"/>
+      <c r="B101" s="97"/>
+      <c r="C101" s="80"/>
+      <c r="D101" s="84"/>
+      <c r="E101" s="85"/>
       <c r="F101" s="62" t="s">
         <v>32</v>
       </c>
@@ -15387,12 +15398,12 @@
       <c r="EC101" s="17"/>
       <c r="ED101" s="18"/>
     </row>
-    <row r="102" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A102" s="86"/>
-      <c r="B102" s="87"/>
-      <c r="C102" s="92"/>
-      <c r="D102" s="97"/>
-      <c r="E102" s="98"/>
+    <row r="102" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A102" s="77"/>
+      <c r="B102" s="97"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="86"/>
+      <c r="E102" s="87"/>
       <c r="F102" s="61"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -15523,18 +15534,18 @@
       <c r="EC102" s="17"/>
       <c r="ED102" s="18"/>
     </row>
-    <row r="103" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A103" s="86">
+    <row r="103" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A103" s="77">
         <v>16</v>
       </c>
-      <c r="B103" s="87"/>
-      <c r="C103" s="77" t="s">
+      <c r="B103" s="97"/>
+      <c r="C103" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="88" t="s">
+      <c r="D103" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="81"/>
+      <c r="E103" s="92"/>
       <c r="F103" s="60" t="s">
         <v>31</v>
       </c>
@@ -15667,12 +15678,12 @@
       <c r="EC103" s="24"/>
       <c r="ED103" s="25"/>
     </row>
-    <row r="104" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A104" s="86"/>
-      <c r="B104" s="87"/>
-      <c r="C104" s="78"/>
-      <c r="D104" s="89"/>
-      <c r="E104" s="83"/>
+    <row r="104" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A104" s="77"/>
+      <c r="B104" s="97"/>
+      <c r="C104" s="89"/>
+      <c r="D104" s="93"/>
+      <c r="E104" s="94"/>
       <c r="F104" s="61"/>
       <c r="G104" s="26"/>
       <c r="H104" s="27"/>
@@ -15803,12 +15814,12 @@
       <c r="EC104" s="27"/>
       <c r="ED104" s="28"/>
     </row>
-    <row r="105" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A105" s="86"/>
-      <c r="B105" s="87"/>
-      <c r="C105" s="78"/>
-      <c r="D105" s="89"/>
-      <c r="E105" s="83"/>
+    <row r="105" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A105" s="77"/>
+      <c r="B105" s="97"/>
+      <c r="C105" s="89"/>
+      <c r="D105" s="93"/>
+      <c r="E105" s="94"/>
       <c r="F105" s="62" t="s">
         <v>32</v>
       </c>
@@ -15941,12 +15952,12 @@
       <c r="EC105" s="27"/>
       <c r="ED105" s="28"/>
     </row>
-    <row r="106" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A106" s="86"/>
-      <c r="B106" s="87"/>
-      <c r="C106" s="79"/>
-      <c r="D106" s="84"/>
-      <c r="E106" s="85"/>
+    <row r="106" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A106" s="77"/>
+      <c r="B106" s="97"/>
+      <c r="C106" s="90"/>
+      <c r="D106" s="95"/>
+      <c r="E106" s="96"/>
       <c r="F106" s="61"/>
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
@@ -16077,14 +16088,14 @@
       <c r="EC106" s="27"/>
       <c r="ED106" s="28"/>
     </row>
-    <row r="107" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A107" s="70"/>
+    <row r="107" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A107" s="100"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="71" t="s">
+      <c r="C107" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="73"/>
-      <c r="E107" s="74"/>
+      <c r="D107" s="103"/>
+      <c r="E107" s="104"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
       <c r="H107" s="44"/>
@@ -16217,12 +16228,12 @@
       <c r="EC107" s="44"/>
       <c r="ED107" s="45"/>
     </row>
-    <row r="108" spans="1:134" x14ac:dyDescent="0.3">
-      <c r="A108" s="70"/>
+    <row r="108" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A108" s="100"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="72"/>
-      <c r="D108" s="75"/>
-      <c r="E108" s="76"/>
+      <c r="C108" s="102"/>
+      <c r="D108" s="105"/>
+      <c r="E108" s="106"/>
       <c r="F108" s="46"/>
       <c r="G108" s="47"/>
       <c r="H108" s="48"/>
@@ -16355,24 +16366,60 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:V1"/>
-    <mergeCell ref="W1:AD1"/>
-    <mergeCell ref="DW1:ED1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="BC1:BJ1"/>
-    <mergeCell ref="BK1:BR1"/>
-    <mergeCell ref="BS1:BZ1"/>
-    <mergeCell ref="CA1:CH1"/>
-    <mergeCell ref="CI1:CP1"/>
-    <mergeCell ref="CQ1:CX1"/>
-    <mergeCell ref="CY1:DF1"/>
-    <mergeCell ref="DG1:DN1"/>
-    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:E108"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:E90"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B106"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:E98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="D99:E102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:E106"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B94"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:E82"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:E94"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:E86"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:E74"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:E78"/>
+    <mergeCell ref="D59:E62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:E66"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:E70"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="D51:E54"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B78"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C35:C38"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B22"/>
     <mergeCell ref="C3:C6"/>
@@ -16389,60 +16436,24 @@
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="D19:E22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B78"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:E26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:E30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:E34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D35:E38"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="D39:E42"/>
-    <mergeCell ref="D47:E50"/>
-    <mergeCell ref="D51:E54"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D55:E58"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:E74"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:E78"/>
-    <mergeCell ref="D59:E62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:E66"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:E70"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B94"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="D79:E82"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:E94"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="D83:E86"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:E108"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:E90"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:E98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:E102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="D103:E106"/>
+    <mergeCell ref="DW1:ED1"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="BC1:BJ1"/>
+    <mergeCell ref="BK1:BR1"/>
+    <mergeCell ref="BS1:BZ1"/>
+    <mergeCell ref="CA1:CH1"/>
+    <mergeCell ref="CI1:CP1"/>
+    <mergeCell ref="CQ1:CX1"/>
+    <mergeCell ref="CY1:DF1"/>
+    <mergeCell ref="DG1:DN1"/>
+    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="AE1:AL1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Gant. Removed accidental comment
</commit_message>
<xml_diff>
--- a/documentation/Gantt.xlsx
+++ b/documentation/Gantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -106,16 +106,10 @@
     <t>Testfälle von 3. Person durchführen lassen</t>
   </si>
   <si>
-    <t>2h/</t>
-  </si>
-  <si>
     <t>4h/</t>
   </si>
   <si>
     <t>8h/</t>
-  </si>
-  <si>
-    <t>6h/</t>
   </si>
   <si>
     <t>6h/6h</t>
@@ -151,9 +145,6 @@
     <t>I18n</t>
   </si>
   <si>
-    <t>16h/</t>
-  </si>
-  <si>
     <t>1h / 1h</t>
   </si>
   <si>
@@ -176,6 +167,39 @@
   </si>
   <si>
     <t>Refactoring</t>
+  </si>
+  <si>
+    <t>16h/18h</t>
+  </si>
+  <si>
+    <t>8h/18h</t>
+  </si>
+  <si>
+    <t>16h/22h</t>
+  </si>
+  <si>
+    <t>4h/7h</t>
+  </si>
+  <si>
+    <t>4h/2h</t>
+  </si>
+  <si>
+    <t>6h/3h</t>
+  </si>
+  <si>
+    <t>0h/17h</t>
+  </si>
+  <si>
+    <t>8h/4h</t>
+  </si>
+  <si>
+    <t>2h/4h</t>
+  </si>
+  <si>
+    <t>4h/1h</t>
+  </si>
+  <si>
+    <t>4h/5h</t>
   </si>
 </sst>
 </file>
@@ -684,65 +708,32 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -771,29 +762,62 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1141,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ED108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BQ71" sqref="BQ71"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,10 +1183,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="51"/>
@@ -1173,168 +1197,168 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="106">
+      <c r="G1" s="76">
         <v>42803</v>
       </c>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="106">
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="76">
         <v>42804</v>
       </c>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="109"/>
-      <c r="U1" s="109"/>
-      <c r="V1" s="110"/>
-      <c r="W1" s="106">
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="76">
         <v>42809</v>
       </c>
-      <c r="X1" s="109"/>
-      <c r="Y1" s="109"/>
-      <c r="Z1" s="109"/>
-      <c r="AA1" s="109"/>
-      <c r="AB1" s="109"/>
-      <c r="AC1" s="109"/>
-      <c r="AD1" s="110"/>
-      <c r="AE1" s="106">
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="76">
         <v>42810</v>
       </c>
-      <c r="AF1" s="109"/>
-      <c r="AG1" s="109"/>
-      <c r="AH1" s="109"/>
-      <c r="AI1" s="109"/>
-      <c r="AJ1" s="109"/>
-      <c r="AK1" s="109"/>
-      <c r="AL1" s="110"/>
-      <c r="AM1" s="106">
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="76">
         <v>42811</v>
       </c>
-      <c r="AN1" s="109"/>
-      <c r="AO1" s="109"/>
-      <c r="AP1" s="109"/>
-      <c r="AQ1" s="109"/>
-      <c r="AR1" s="109"/>
-      <c r="AS1" s="109"/>
-      <c r="AT1" s="110"/>
-      <c r="AU1" s="106">
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="77"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="76">
         <v>42816</v>
       </c>
-      <c r="AV1" s="109"/>
-      <c r="AW1" s="109"/>
-      <c r="AX1" s="109"/>
-      <c r="AY1" s="109"/>
-      <c r="AZ1" s="109"/>
-      <c r="BA1" s="109"/>
-      <c r="BB1" s="110"/>
-      <c r="BC1" s="106">
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="77"/>
+      <c r="AX1" s="77"/>
+      <c r="AY1" s="77"/>
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="77"/>
+      <c r="BB1" s="78"/>
+      <c r="BC1" s="76">
         <v>42817</v>
       </c>
-      <c r="BD1" s="109"/>
-      <c r="BE1" s="109"/>
-      <c r="BF1" s="109"/>
-      <c r="BG1" s="109"/>
-      <c r="BH1" s="109"/>
-      <c r="BI1" s="109"/>
-      <c r="BJ1" s="110"/>
-      <c r="BK1" s="106">
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="77"/>
+      <c r="BG1" s="77"/>
+      <c r="BH1" s="77"/>
+      <c r="BI1" s="77"/>
+      <c r="BJ1" s="78"/>
+      <c r="BK1" s="76">
         <v>42818</v>
       </c>
-      <c r="BL1" s="109"/>
-      <c r="BM1" s="109"/>
-      <c r="BN1" s="109"/>
-      <c r="BO1" s="109"/>
-      <c r="BP1" s="109"/>
-      <c r="BQ1" s="109"/>
-      <c r="BR1" s="110"/>
-      <c r="BS1" s="106">
+      <c r="BL1" s="77"/>
+      <c r="BM1" s="77"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="77"/>
+      <c r="BP1" s="77"/>
+      <c r="BQ1" s="77"/>
+      <c r="BR1" s="78"/>
+      <c r="BS1" s="76">
         <v>42823</v>
       </c>
-      <c r="BT1" s="109"/>
-      <c r="BU1" s="109"/>
-      <c r="BV1" s="109"/>
-      <c r="BW1" s="109"/>
-      <c r="BX1" s="109"/>
-      <c r="BY1" s="109"/>
-      <c r="BZ1" s="110"/>
-      <c r="CA1" s="106">
+      <c r="BT1" s="77"/>
+      <c r="BU1" s="77"/>
+      <c r="BV1" s="77"/>
+      <c r="BW1" s="77"/>
+      <c r="BX1" s="77"/>
+      <c r="BY1" s="77"/>
+      <c r="BZ1" s="78"/>
+      <c r="CA1" s="76">
         <v>42824</v>
       </c>
-      <c r="CB1" s="107"/>
-      <c r="CC1" s="107"/>
-      <c r="CD1" s="107"/>
-      <c r="CE1" s="107"/>
-      <c r="CF1" s="107"/>
-      <c r="CG1" s="107"/>
-      <c r="CH1" s="108"/>
-      <c r="CI1" s="106">
+      <c r="CB1" s="81"/>
+      <c r="CC1" s="81"/>
+      <c r="CD1" s="81"/>
+      <c r="CE1" s="81"/>
+      <c r="CF1" s="81"/>
+      <c r="CG1" s="81"/>
+      <c r="CH1" s="82"/>
+      <c r="CI1" s="76">
         <v>42825</v>
       </c>
-      <c r="CJ1" s="107"/>
-      <c r="CK1" s="107"/>
-      <c r="CL1" s="107"/>
-      <c r="CM1" s="107"/>
-      <c r="CN1" s="107"/>
-      <c r="CO1" s="107"/>
-      <c r="CP1" s="108"/>
-      <c r="CQ1" s="106">
+      <c r="CJ1" s="81"/>
+      <c r="CK1" s="81"/>
+      <c r="CL1" s="81"/>
+      <c r="CM1" s="81"/>
+      <c r="CN1" s="81"/>
+      <c r="CO1" s="81"/>
+      <c r="CP1" s="82"/>
+      <c r="CQ1" s="76">
         <v>42826</v>
       </c>
-      <c r="CR1" s="107"/>
-      <c r="CS1" s="107"/>
-      <c r="CT1" s="107"/>
-      <c r="CU1" s="107"/>
-      <c r="CV1" s="107"/>
-      <c r="CW1" s="107"/>
-      <c r="CX1" s="108"/>
-      <c r="CY1" s="106">
+      <c r="CR1" s="81"/>
+      <c r="CS1" s="81"/>
+      <c r="CT1" s="81"/>
+      <c r="CU1" s="81"/>
+      <c r="CV1" s="81"/>
+      <c r="CW1" s="81"/>
+      <c r="CX1" s="82"/>
+      <c r="CY1" s="76">
         <v>42830</v>
       </c>
-      <c r="CZ1" s="107"/>
-      <c r="DA1" s="107"/>
-      <c r="DB1" s="107"/>
-      <c r="DC1" s="107"/>
-      <c r="DD1" s="107"/>
-      <c r="DE1" s="107"/>
-      <c r="DF1" s="108"/>
-      <c r="DG1" s="106">
+      <c r="CZ1" s="81"/>
+      <c r="DA1" s="81"/>
+      <c r="DB1" s="81"/>
+      <c r="DC1" s="81"/>
+      <c r="DD1" s="81"/>
+      <c r="DE1" s="81"/>
+      <c r="DF1" s="82"/>
+      <c r="DG1" s="76">
         <v>42831</v>
       </c>
-      <c r="DH1" s="107"/>
-      <c r="DI1" s="107"/>
-      <c r="DJ1" s="107"/>
-      <c r="DK1" s="107"/>
-      <c r="DL1" s="107"/>
-      <c r="DM1" s="107"/>
-      <c r="DN1" s="108"/>
-      <c r="DO1" s="106">
+      <c r="DH1" s="81"/>
+      <c r="DI1" s="81"/>
+      <c r="DJ1" s="81"/>
+      <c r="DK1" s="81"/>
+      <c r="DL1" s="81"/>
+      <c r="DM1" s="81"/>
+      <c r="DN1" s="82"/>
+      <c r="DO1" s="76">
         <v>42832</v>
       </c>
-      <c r="DP1" s="107"/>
-      <c r="DQ1" s="107"/>
-      <c r="DR1" s="107"/>
-      <c r="DS1" s="107"/>
-      <c r="DT1" s="107"/>
-      <c r="DU1" s="107"/>
-      <c r="DV1" s="108"/>
-      <c r="DW1" s="106"/>
-      <c r="DX1" s="107"/>
-      <c r="DY1" s="107"/>
-      <c r="DZ1" s="107"/>
-      <c r="EA1" s="107"/>
-      <c r="EB1" s="107"/>
-      <c r="EC1" s="107"/>
-      <c r="ED1" s="108"/>
+      <c r="DP1" s="81"/>
+      <c r="DQ1" s="81"/>
+      <c r="DR1" s="81"/>
+      <c r="DS1" s="81"/>
+      <c r="DT1" s="81"/>
+      <c r="DU1" s="81"/>
+      <c r="DV1" s="82"/>
+      <c r="DW1" s="76"/>
+      <c r="DX1" s="81"/>
+      <c r="DY1" s="81"/>
+      <c r="DZ1" s="81"/>
+      <c r="EA1" s="81"/>
+      <c r="EB1" s="81"/>
+      <c r="EC1" s="81"/>
+      <c r="ED1" s="82"/>
     </row>
     <row r="2" spans="1:134" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1715,21 +1739,21 @@
       <c r="ED2" s="9"/>
     </row>
     <row r="3" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A3" s="92">
+      <c r="A3" s="83">
         <v>1</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="100"/>
+      <c r="D3" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="89"/>
       <c r="F3" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="64"/>
       <c r="H3" s="10"/>
@@ -1861,11 +1885,11 @@
       <c r="ED3" s="12"/>
     </row>
     <row r="4" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="102"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
       <c r="F4" s="61"/>
       <c r="G4" s="65"/>
       <c r="H4" s="16"/>
@@ -1997,13 +2021,13 @@
       <c r="ED4" s="18"/>
     </row>
     <row r="5" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="102"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91"/>
       <c r="F5" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" s="66"/>
       <c r="H5" s="20"/>
@@ -2135,11 +2159,11 @@
       <c r="ED5" s="18"/>
     </row>
     <row r="6" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="61"/>
       <c r="G6" s="67"/>
       <c r="H6" s="22"/>
@@ -2271,19 +2295,19 @@
       <c r="ED6" s="18"/>
     </row>
     <row r="7" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A7" s="92">
+      <c r="A7" s="83">
         <v>2</v>
       </c>
-      <c r="B7" s="105"/>
-      <c r="C7" s="83" t="s">
+      <c r="B7" s="84"/>
+      <c r="C7" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="87"/>
+      <c r="D7" s="97" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="98"/>
       <c r="F7" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="24"/>
@@ -2415,11 +2439,11 @@
       <c r="ED7" s="25"/>
     </row>
     <row r="8" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="89"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="61"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
@@ -2551,13 +2575,13 @@
       <c r="ED8" s="28"/>
     </row>
     <row r="9" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="89"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="100"/>
       <c r="F9" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="27"/>
@@ -2689,11 +2713,11 @@
       <c r="ED9" s="28"/>
     </row>
     <row r="10" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="91"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="102"/>
       <c r="F10" s="61"/>
       <c r="G10" s="26"/>
       <c r="H10" s="27"/>
@@ -2825,19 +2849,19 @@
       <c r="ED10" s="28"/>
     </row>
     <row r="11" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+      <c r="A11" s="83">
         <v>3</v>
       </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="96" t="s">
+      <c r="B11" s="84"/>
+      <c r="C11" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="100"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="11"/>
@@ -2969,11 +2993,11 @@
       <c r="ED11" s="12"/>
     </row>
     <row r="12" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="102"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="91"/>
       <c r="F12" s="61"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3105,13 +3129,13 @@
       <c r="ED12" s="18"/>
     </row>
     <row r="13" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="102"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
       <c r="F13" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -3243,11 +3267,11 @@
       <c r="ED13" s="18"/>
     </row>
     <row r="14" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A14" s="92"/>
-      <c r="B14" s="105"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="61"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -3379,19 +3403,19 @@
       <c r="ED14" s="18"/>
     </row>
     <row r="15" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A15" s="92">
+      <c r="A15" s="83">
         <v>4</v>
       </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="83" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="87"/>
+      <c r="D15" s="97" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="98"/>
       <c r="F15" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="24"/>
@@ -3523,11 +3547,11 @@
       <c r="ED15" s="25"/>
     </row>
     <row r="16" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="89"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="61"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
@@ -3659,13 +3683,13 @@
       <c r="ED16" s="28"/>
     </row>
     <row r="17" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="89"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="100"/>
       <c r="F17" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="27"/>
@@ -3797,11 +3821,11 @@
       <c r="ED17" s="28"/>
     </row>
     <row r="18" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="105"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="102"/>
       <c r="F18" s="61"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27"/>
@@ -3933,19 +3957,19 @@
       <c r="ED18" s="28"/>
     </row>
     <row r="19" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A19" s="92">
+      <c r="A19" s="83">
         <v>5</v>
       </c>
-      <c r="B19" s="105"/>
-      <c r="C19" s="96" t="s">
+      <c r="B19" s="84"/>
+      <c r="C19" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="99" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="100"/>
+      <c r="D19" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="89"/>
       <c r="F19" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="11"/>
@@ -4077,11 +4101,11 @@
       <c r="ED19" s="12"/>
     </row>
     <row r="20" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A20" s="92"/>
-      <c r="B20" s="105"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="102"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="91"/>
       <c r="F20" s="61"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -4213,13 +4237,13 @@
       <c r="ED20" s="18"/>
     </row>
     <row r="21" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
-      <c r="B21" s="105"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="102"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="91"/>
       <c r="F21" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
@@ -4351,11 +4375,11 @@
       <c r="ED21" s="18"/>
     </row>
     <row r="22" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
-      <c r="B22" s="105"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="104"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="93"/>
       <c r="F22" s="61"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -4487,21 +4511,21 @@
       <c r="ED22" s="18"/>
     </row>
     <row r="23" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A23" s="92">
+      <c r="A23" s="83">
         <v>6</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="86" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="87"/>
+      <c r="C23" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="104" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="98"/>
       <c r="F23" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="24"/>
@@ -4633,11 +4657,11 @@
       <c r="ED23" s="25"/>
     </row>
     <row r="24" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="89"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="100"/>
       <c r="F24" s="61"/>
       <c r="G24" s="26"/>
       <c r="H24" s="27"/>
@@ -4769,13 +4793,13 @@
       <c r="ED24" s="28"/>
     </row>
     <row r="25" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="89"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="100"/>
       <c r="F25" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="27"/>
@@ -4907,11 +4931,11 @@
       <c r="ED25" s="28"/>
     </row>
     <row r="26" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
-      <c r="B26" s="93"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="91"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="102"/>
       <c r="F26" s="61"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
@@ -5043,19 +5067,19 @@
       <c r="ED26" s="28"/>
     </row>
     <row r="27" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A27" s="92">
+      <c r="A27" s="83">
         <v>7</v>
       </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="96" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="99" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="100"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="89"/>
       <c r="F27" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="11"/>
@@ -5187,11 +5211,11 @@
       <c r="ED27" s="12"/>
     </row>
     <row r="28" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="102"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="91"/>
       <c r="F28" s="61"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
@@ -5323,13 +5347,13 @@
       <c r="ED28" s="18"/>
     </row>
     <row r="29" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="102"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="91"/>
       <c r="F29" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -5461,11 +5485,11 @@
       <c r="ED29" s="18"/>
     </row>
     <row r="30" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="103"/>
-      <c r="E30" s="104"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="93"/>
       <c r="F30" s="61"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -5597,19 +5621,19 @@
       <c r="ED30" s="18"/>
     </row>
     <row r="31" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A31" s="92">
+      <c r="A31" s="83">
         <v>8</v>
       </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="86" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="87"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="104" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="98"/>
       <c r="F31" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="24"/>
@@ -5741,11 +5765,11 @@
       <c r="ED31" s="25"/>
     </row>
     <row r="32" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="89"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="100"/>
       <c r="F32" s="61"/>
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
@@ -5877,13 +5901,13 @@
       <c r="ED32" s="28"/>
     </row>
     <row r="33" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="93"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="89"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="100"/>
       <c r="F33" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G33" s="26"/>
       <c r="H33" s="27"/>
@@ -6015,11 +6039,11 @@
       <c r="ED33" s="28"/>
     </row>
     <row r="34" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
-      <c r="B34" s="93"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="90"/>
-      <c r="E34" s="91"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="102"/>
       <c r="F34" s="61"/>
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
@@ -6151,19 +6175,19 @@
       <c r="ED34" s="28"/>
     </row>
     <row r="35" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A35" s="92">
+      <c r="A35" s="83">
         <v>9</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="100"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="89"/>
       <c r="F35" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="11"/>
@@ -6295,11 +6319,11 @@
       <c r="ED35" s="12"/>
     </row>
     <row r="36" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="101"/>
-      <c r="E36" s="102"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="91"/>
       <c r="F36" s="61"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -6431,13 +6455,13 @@
       <c r="ED36" s="18"/>
     </row>
     <row r="37" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A37" s="92"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="102"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="91"/>
       <c r="F37" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
@@ -6517,8 +6541,8 @@
       <c r="CD37" s="17"/>
       <c r="CE37" s="19"/>
       <c r="CF37" s="19"/>
-      <c r="CG37" s="19"/>
-      <c r="CH37" s="30"/>
+      <c r="CG37" s="17"/>
+      <c r="CH37" s="18"/>
       <c r="CI37" s="17"/>
       <c r="CJ37" s="17"/>
       <c r="CK37" s="17"/>
@@ -6569,11 +6593,11 @@
       <c r="ED37" s="18"/>
     </row>
     <row r="38" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A38" s="92"/>
-      <c r="B38" s="93"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="104"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="92"/>
+      <c r="E38" s="93"/>
       <c r="F38" s="61"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -6653,8 +6677,8 @@
       <c r="CD38" s="17"/>
       <c r="CE38" s="19"/>
       <c r="CF38" s="19"/>
-      <c r="CG38" s="19"/>
-      <c r="CH38" s="30"/>
+      <c r="CG38" s="17"/>
+      <c r="CH38" s="18"/>
       <c r="CI38" s="17"/>
       <c r="CJ38" s="17"/>
       <c r="CK38" s="17"/>
@@ -6706,16 +6730,16 @@
     </row>
     <row r="39" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="83" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="87"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="98"/>
       <c r="F39" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G39" s="23"/>
       <c r="H39" s="24"/>
@@ -6848,10 +6872,10 @@
     </row>
     <row r="40" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="89"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="100"/>
       <c r="F40" s="61"/>
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
@@ -6984,12 +7008,12 @@
     </row>
     <row r="41" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="89"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="95"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="100"/>
       <c r="F41" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
@@ -7068,7 +7092,7 @@
       <c r="CC41" s="27"/>
       <c r="CD41" s="27"/>
       <c r="CE41" s="27"/>
-      <c r="CF41" s="19"/>
+      <c r="CF41" s="17"/>
       <c r="CG41" s="19"/>
       <c r="CH41" s="30"/>
       <c r="CI41" s="27"/>
@@ -7122,10 +7146,10 @@
     </row>
     <row r="42" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="91"/>
+      <c r="B42" s="103"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="101"/>
+      <c r="E42" s="102"/>
       <c r="F42" s="61"/>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -7204,7 +7228,7 @@
       <c r="CC42" s="27"/>
       <c r="CD42" s="27"/>
       <c r="CE42" s="27"/>
-      <c r="CF42" s="19"/>
+      <c r="CF42" s="17"/>
       <c r="CG42" s="19"/>
       <c r="CH42" s="30"/>
       <c r="CI42" s="27"/>
@@ -7258,16 +7282,16 @@
     </row>
     <row r="43" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="96" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="99" t="s">
+      <c r="B43" s="103"/>
+      <c r="C43" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="89"/>
+      <c r="F43" s="60" t="s">
         <v>29</v>
-      </c>
-      <c r="E43" s="100"/>
-      <c r="F43" s="60" t="s">
-        <v>31</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="11"/>
@@ -7400,10 +7424,10 @@
     </row>
     <row r="44" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="101"/>
-      <c r="E44" s="102"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="91"/>
       <c r="F44" s="61"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -7536,12 +7560,12 @@
     </row>
     <row r="45" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A45" s="51"/>
-      <c r="B45" s="93"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="101"/>
-      <c r="E45" s="102"/>
+      <c r="B45" s="103"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="91"/>
       <c r="F45" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
@@ -7674,10 +7698,10 @@
     </row>
     <row r="46" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A46" s="51"/>
-      <c r="B46" s="93"/>
-      <c r="C46" s="98"/>
-      <c r="D46" s="103"/>
-      <c r="E46" s="104"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="92"/>
+      <c r="E46" s="93"/>
       <c r="F46" s="61"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -7810,16 +7834,16 @@
     </row>
     <row r="47" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A47" s="51"/>
-      <c r="B47" s="93"/>
-      <c r="C47" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="E47" s="87"/>
+      <c r="B47" s="103"/>
+      <c r="C47" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="98"/>
       <c r="F47" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="24"/>
@@ -7952,10 +7976,10 @@
     </row>
     <row r="48" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A48" s="51"/>
-      <c r="B48" s="93"/>
-      <c r="C48" s="84"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="89"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="105"/>
+      <c r="E48" s="100"/>
       <c r="F48" s="61"/>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -8088,12 +8112,12 @@
     </row>
     <row r="49" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
-      <c r="B49" s="93"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="88"/>
-      <c r="E49" s="89"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="105"/>
+      <c r="E49" s="100"/>
       <c r="F49" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="27"/>
@@ -8226,10 +8250,10 @@
     </row>
     <row r="50" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
-      <c r="B50" s="93"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="91"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="102"/>
       <c r="F50" s="61"/>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
@@ -8362,16 +8386,16 @@
     </row>
     <row r="51" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A51" s="51"/>
-      <c r="B51" s="93"/>
+      <c r="B51" s="103"/>
       <c r="C51" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" s="99" t="s">
-        <v>44</v>
-      </c>
-      <c r="E51" s="100"/>
+        <v>36</v>
+      </c>
+      <c r="D51" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="89"/>
       <c r="F51" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="11"/>
@@ -8504,10 +8528,10 @@
     </row>
     <row r="52" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A52" s="51"/>
-      <c r="B52" s="93"/>
+      <c r="B52" s="103"/>
       <c r="C52" s="53"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="102"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="91"/>
       <c r="F52" s="61"/>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
@@ -8640,12 +8664,12 @@
     </row>
     <row r="53" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A53" s="51"/>
-      <c r="B53" s="93"/>
+      <c r="B53" s="103"/>
       <c r="C53" s="53"/>
-      <c r="D53" s="101"/>
-      <c r="E53" s="102"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="91"/>
       <c r="F53" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
@@ -8778,10 +8802,10 @@
     </row>
     <row r="54" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A54" s="51"/>
-      <c r="B54" s="93"/>
+      <c r="B54" s="103"/>
       <c r="C54" s="54"/>
-      <c r="D54" s="103"/>
-      <c r="E54" s="104"/>
+      <c r="D54" s="92"/>
+      <c r="E54" s="93"/>
       <c r="F54" s="61"/>
       <c r="G54" s="17"/>
       <c r="H54" s="17"/>
@@ -8914,16 +8938,16 @@
     </row>
     <row r="55" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A55" s="51"/>
-      <c r="B55" s="93"/>
+      <c r="B55" s="103"/>
       <c r="C55" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="87"/>
+        <v>37</v>
+      </c>
+      <c r="D55" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="98"/>
       <c r="F55" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G55" s="23"/>
       <c r="H55" s="24"/>
@@ -9056,10 +9080,10 @@
     </row>
     <row r="56" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A56" s="51"/>
-      <c r="B56" s="93"/>
+      <c r="B56" s="103"/>
       <c r="C56" s="56"/>
-      <c r="D56" s="88"/>
-      <c r="E56" s="89"/>
+      <c r="D56" s="105"/>
+      <c r="E56" s="100"/>
       <c r="F56" s="61"/>
       <c r="G56" s="26"/>
       <c r="H56" s="27"/>
@@ -9192,12 +9216,12 @@
     </row>
     <row r="57" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A57" s="51"/>
-      <c r="B57" s="93"/>
+      <c r="B57" s="103"/>
       <c r="C57" s="56"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="89"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="100"/>
       <c r="F57" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G57" s="26"/>
       <c r="H57" s="27"/>
@@ -9330,10 +9354,10 @@
     </row>
     <row r="58" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A58" s="51"/>
-      <c r="B58" s="93"/>
+      <c r="B58" s="103"/>
       <c r="C58" s="57"/>
-      <c r="D58" s="90"/>
-      <c r="E58" s="91"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="102"/>
       <c r="F58" s="61"/>
       <c r="G58" s="26"/>
       <c r="H58" s="27"/>
@@ -9466,16 +9490,16 @@
     </row>
     <row r="59" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A59" s="51"/>
-      <c r="B59" s="93"/>
+      <c r="B59" s="103"/>
       <c r="C59" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D59" s="99" t="s">
-        <v>28</v>
-      </c>
-      <c r="E59" s="100"/>
+        <v>38</v>
+      </c>
+      <c r="D59" s="88" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="89"/>
       <c r="F59" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="11"/>
@@ -9608,10 +9632,10 @@
     </row>
     <row r="60" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A60" s="51"/>
-      <c r="B60" s="93"/>
+      <c r="B60" s="103"/>
       <c r="C60" s="53"/>
-      <c r="D60" s="101"/>
-      <c r="E60" s="102"/>
+      <c r="D60" s="90"/>
+      <c r="E60" s="91"/>
       <c r="F60" s="61"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -9744,12 +9768,12 @@
     </row>
     <row r="61" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A61" s="51"/>
-      <c r="B61" s="93"/>
+      <c r="B61" s="103"/>
       <c r="C61" s="53"/>
-      <c r="D61" s="101"/>
-      <c r="E61" s="102"/>
+      <c r="D61" s="90"/>
+      <c r="E61" s="91"/>
       <c r="F61" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
@@ -9882,10 +9906,10 @@
     </row>
     <row r="62" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A62" s="51"/>
-      <c r="B62" s="93"/>
+      <c r="B62" s="103"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="103"/>
-      <c r="E62" s="104"/>
+      <c r="D62" s="92"/>
+      <c r="E62" s="93"/>
       <c r="F62" s="61"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
@@ -10018,14 +10042,16 @@
     </row>
     <row r="63" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A63" s="51"/>
-      <c r="B63" s="93"/>
-      <c r="C63" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="86"/>
-      <c r="E63" s="87"/>
+      <c r="B63" s="103"/>
+      <c r="C63" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="104" t="s">
+        <v>53</v>
+      </c>
+      <c r="E63" s="98"/>
       <c r="F63" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G63" s="23"/>
       <c r="H63" s="24"/>
@@ -10158,10 +10184,10 @@
     </row>
     <row r="64" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A64" s="51"/>
-      <c r="B64" s="93"/>
-      <c r="C64" s="84"/>
-      <c r="D64" s="88"/>
-      <c r="E64" s="89"/>
+      <c r="B64" s="103"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="105"/>
+      <c r="E64" s="100"/>
       <c r="F64" s="61"/>
       <c r="G64" s="26"/>
       <c r="H64" s="27"/>
@@ -10294,12 +10320,12 @@
     </row>
     <row r="65" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A65" s="51"/>
-      <c r="B65" s="93"/>
-      <c r="C65" s="84"/>
-      <c r="D65" s="88"/>
-      <c r="E65" s="89"/>
+      <c r="B65" s="103"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="105"/>
+      <c r="E65" s="100"/>
       <c r="F65" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G65" s="26"/>
       <c r="H65" s="27"/>
@@ -10432,10 +10458,10 @@
     </row>
     <row r="66" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A66" s="51"/>
-      <c r="B66" s="93"/>
-      <c r="C66" s="85"/>
-      <c r="D66" s="90"/>
-      <c r="E66" s="91"/>
+      <c r="B66" s="103"/>
+      <c r="C66" s="96"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="102"/>
       <c r="F66" s="61"/>
       <c r="G66" s="26"/>
       <c r="H66" s="27"/>
@@ -10568,12 +10594,12 @@
     </row>
     <row r="67" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A67" s="51"/>
-      <c r="B67" s="93"/>
-      <c r="C67" s="96"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="100"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="88"/>
+      <c r="E67" s="89"/>
       <c r="F67" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="11"/>
@@ -10706,10 +10732,10 @@
     </row>
     <row r="68" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A68" s="51"/>
-      <c r="B68" s="93"/>
-      <c r="C68" s="97"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="102"/>
+      <c r="B68" s="103"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="90"/>
+      <c r="E68" s="91"/>
       <c r="F68" s="61"/>
       <c r="G68" s="17"/>
       <c r="H68" s="17"/>
@@ -10842,12 +10868,12 @@
     </row>
     <row r="69" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A69" s="51"/>
-      <c r="B69" s="93"/>
-      <c r="C69" s="97"/>
-      <c r="D69" s="101"/>
-      <c r="E69" s="102"/>
+      <c r="B69" s="103"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="90"/>
+      <c r="E69" s="91"/>
       <c r="F69" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
@@ -10980,10 +11006,10 @@
     </row>
     <row r="70" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A70" s="51"/>
-      <c r="B70" s="93"/>
-      <c r="C70" s="98"/>
-      <c r="D70" s="103"/>
-      <c r="E70" s="104"/>
+      <c r="B70" s="103"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="92"/>
+      <c r="E70" s="93"/>
       <c r="F70" s="61"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -11116,12 +11142,12 @@
     </row>
     <row r="71" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A71" s="51"/>
-      <c r="B71" s="93"/>
-      <c r="C71" s="83"/>
-      <c r="D71" s="86"/>
-      <c r="E71" s="87"/>
+      <c r="B71" s="103"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="104"/>
+      <c r="E71" s="98"/>
       <c r="F71" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G71" s="23"/>
       <c r="H71" s="24"/>
@@ -11254,10 +11280,10 @@
     </row>
     <row r="72" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A72" s="51"/>
-      <c r="B72" s="93"/>
-      <c r="C72" s="84"/>
-      <c r="D72" s="88"/>
-      <c r="E72" s="89"/>
+      <c r="B72" s="103"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="105"/>
+      <c r="E72" s="100"/>
       <c r="F72" s="61"/>
       <c r="G72" s="27"/>
       <c r="H72" s="27"/>
@@ -11390,12 +11416,12 @@
     </row>
     <row r="73" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A73" s="51"/>
-      <c r="B73" s="93"/>
-      <c r="C73" s="84"/>
-      <c r="D73" s="88"/>
-      <c r="E73" s="89"/>
+      <c r="B73" s="103"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="105"/>
+      <c r="E73" s="100"/>
       <c r="F73" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G73" s="27"/>
       <c r="H73" s="27"/>
@@ -11528,10 +11554,10 @@
     </row>
     <row r="74" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A74" s="51"/>
-      <c r="B74" s="93"/>
-      <c r="C74" s="85"/>
-      <c r="D74" s="90"/>
-      <c r="E74" s="91"/>
+      <c r="B74" s="103"/>
+      <c r="C74" s="96"/>
+      <c r="D74" s="101"/>
+      <c r="E74" s="102"/>
       <c r="F74" s="61"/>
       <c r="G74" s="27"/>
       <c r="H74" s="27"/>
@@ -11664,12 +11690,12 @@
     </row>
     <row r="75" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A75" s="51"/>
-      <c r="B75" s="93"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="100"/>
+      <c r="B75" s="103"/>
+      <c r="C75" s="85"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="89"/>
       <c r="F75" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="11"/>
@@ -11802,10 +11828,10 @@
     </row>
     <row r="76" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A76" s="51"/>
-      <c r="B76" s="93"/>
-      <c r="C76" s="97"/>
-      <c r="D76" s="101"/>
-      <c r="E76" s="102"/>
+      <c r="B76" s="103"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="90"/>
+      <c r="E76" s="91"/>
       <c r="F76" s="61"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
@@ -11938,12 +11964,12 @@
     </row>
     <row r="77" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A77" s="51"/>
-      <c r="B77" s="93"/>
-      <c r="C77" s="97"/>
-      <c r="D77" s="101"/>
-      <c r="E77" s="102"/>
+      <c r="B77" s="103"/>
+      <c r="C77" s="86"/>
+      <c r="D77" s="90"/>
+      <c r="E77" s="91"/>
       <c r="F77" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G77" s="17"/>
       <c r="H77" s="17"/>
@@ -12076,10 +12102,10 @@
     </row>
     <row r="78" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A78" s="51"/>
-      <c r="B78" s="93"/>
-      <c r="C78" s="98"/>
-      <c r="D78" s="103"/>
-      <c r="E78" s="104"/>
+      <c r="B78" s="103"/>
+      <c r="C78" s="87"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="93"/>
       <c r="F78" s="61"/>
       <c r="G78" s="17"/>
       <c r="H78" s="17"/>
@@ -12211,21 +12237,21 @@
       <c r="ED78" s="18"/>
     </row>
     <row r="79" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A79" s="92">
+      <c r="A79" s="83">
         <v>11</v>
       </c>
-      <c r="B79" s="105" t="s">
+      <c r="B79" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="83" t="s">
+      <c r="C79" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="E79" s="87"/>
+      <c r="D79" s="104" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="98"/>
       <c r="F79" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G79" s="23"/>
       <c r="H79" s="24"/>
@@ -12357,11 +12383,11 @@
       <c r="ED79" s="25"/>
     </row>
     <row r="80" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A80" s="92"/>
-      <c r="B80" s="105"/>
-      <c r="C80" s="84"/>
-      <c r="D80" s="88"/>
-      <c r="E80" s="89"/>
+      <c r="A80" s="83"/>
+      <c r="B80" s="84"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="105"/>
+      <c r="E80" s="100"/>
       <c r="F80" s="61"/>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -12493,13 +12519,13 @@
       <c r="ED80" s="28"/>
     </row>
     <row r="81" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A81" s="92"/>
-      <c r="B81" s="105"/>
-      <c r="C81" s="84"/>
-      <c r="D81" s="88"/>
-      <c r="E81" s="89"/>
+      <c r="A81" s="83"/>
+      <c r="B81" s="84"/>
+      <c r="C81" s="95"/>
+      <c r="D81" s="105"/>
+      <c r="E81" s="100"/>
       <c r="F81" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G81" s="27"/>
       <c r="H81" s="27"/>
@@ -12631,11 +12657,11 @@
       <c r="ED81" s="28"/>
     </row>
     <row r="82" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A82" s="92"/>
-      <c r="B82" s="105"/>
-      <c r="C82" s="85"/>
-      <c r="D82" s="90"/>
-      <c r="E82" s="91"/>
+      <c r="A82" s="83"/>
+      <c r="B82" s="84"/>
+      <c r="C82" s="96"/>
+      <c r="D82" s="101"/>
+      <c r="E82" s="102"/>
       <c r="F82" s="61"/>
       <c r="G82" s="27"/>
       <c r="H82" s="27"/>
@@ -12768,16 +12794,16 @@
     </row>
     <row r="83" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A83" s="51"/>
-      <c r="B83" s="105"/>
-      <c r="C83" s="96" t="s">
+      <c r="B83" s="84"/>
+      <c r="C83" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="99" t="s">
-        <v>48</v>
-      </c>
-      <c r="E83" s="100"/>
+      <c r="D83" s="88" t="s">
+        <v>45</v>
+      </c>
+      <c r="E83" s="89"/>
       <c r="F83" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="11"/>
@@ -12910,10 +12936,10 @@
     </row>
     <row r="84" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A84" s="51"/>
-      <c r="B84" s="105"/>
-      <c r="C84" s="97"/>
-      <c r="D84" s="101"/>
-      <c r="E84" s="102"/>
+      <c r="B84" s="84"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="90"/>
+      <c r="E84" s="91"/>
       <c r="F84" s="61"/>
       <c r="G84" s="17"/>
       <c r="H84" s="17"/>
@@ -13046,12 +13072,12 @@
     </row>
     <row r="85" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A85" s="51"/>
-      <c r="B85" s="105"/>
-      <c r="C85" s="97"/>
-      <c r="D85" s="101"/>
-      <c r="E85" s="102"/>
+      <c r="B85" s="84"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="90"/>
+      <c r="E85" s="91"/>
       <c r="F85" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="17"/>
@@ -13184,10 +13210,10 @@
     </row>
     <row r="86" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A86" s="51"/>
-      <c r="B86" s="105"/>
-      <c r="C86" s="98"/>
-      <c r="D86" s="103"/>
-      <c r="E86" s="104"/>
+      <c r="B86" s="84"/>
+      <c r="C86" s="87"/>
+      <c r="D86" s="92"/>
+      <c r="E86" s="93"/>
       <c r="F86" s="61"/>
       <c r="G86" s="17"/>
       <c r="H86" s="17"/>
@@ -13320,16 +13346,16 @@
     </row>
     <row r="87" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A87" s="51"/>
-      <c r="B87" s="105"/>
-      <c r="C87" s="83" t="s">
+      <c r="B87" s="84"/>
+      <c r="C87" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="D87" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" s="87"/>
+      <c r="D87" s="104" t="s">
+        <v>57</v>
+      </c>
+      <c r="E87" s="98"/>
       <c r="F87" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G87" s="23"/>
       <c r="H87" s="24"/>
@@ -13462,10 +13488,10 @@
     </row>
     <row r="88" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A88" s="51"/>
-      <c r="B88" s="105"/>
-      <c r="C88" s="84"/>
-      <c r="D88" s="88"/>
-      <c r="E88" s="89"/>
+      <c r="B88" s="84"/>
+      <c r="C88" s="95"/>
+      <c r="D88" s="105"/>
+      <c r="E88" s="100"/>
       <c r="F88" s="61"/>
       <c r="G88" s="27"/>
       <c r="H88" s="27"/>
@@ -13598,12 +13624,12 @@
     </row>
     <row r="89" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A89" s="51"/>
-      <c r="B89" s="105"/>
-      <c r="C89" s="84"/>
-      <c r="D89" s="88"/>
-      <c r="E89" s="89"/>
+      <c r="B89" s="84"/>
+      <c r="C89" s="95"/>
+      <c r="D89" s="105"/>
+      <c r="E89" s="100"/>
       <c r="F89" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G89" s="27"/>
       <c r="H89" s="27"/>
@@ -13736,10 +13762,10 @@
     </row>
     <row r="90" spans="1:134" x14ac:dyDescent="0.25">
       <c r="A90" s="51"/>
-      <c r="B90" s="105"/>
-      <c r="C90" s="85"/>
-      <c r="D90" s="90"/>
-      <c r="E90" s="91"/>
+      <c r="B90" s="84"/>
+      <c r="C90" s="96"/>
+      <c r="D90" s="101"/>
+      <c r="E90" s="102"/>
       <c r="F90" s="61"/>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
@@ -13871,19 +13897,19 @@
       <c r="ED90" s="28"/>
     </row>
     <row r="91" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A91" s="92">
+      <c r="A91" s="83">
         <v>13</v>
       </c>
-      <c r="B91" s="105"/>
-      <c r="C91" s="96" t="s">
+      <c r="B91" s="84"/>
+      <c r="C91" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="E91" s="100"/>
+      <c r="D91" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E91" s="89"/>
       <c r="F91" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="11"/>
@@ -14015,11 +14041,11 @@
       <c r="ED91" s="12"/>
     </row>
     <row r="92" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A92" s="92"/>
-      <c r="B92" s="105"/>
-      <c r="C92" s="97"/>
-      <c r="D92" s="101"/>
-      <c r="E92" s="102"/>
+      <c r="A92" s="83"/>
+      <c r="B92" s="84"/>
+      <c r="C92" s="86"/>
+      <c r="D92" s="90"/>
+      <c r="E92" s="91"/>
       <c r="F92" s="61"/>
       <c r="G92" s="17"/>
       <c r="H92" s="17"/>
@@ -14151,13 +14177,13 @@
       <c r="ED92" s="18"/>
     </row>
     <row r="93" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A93" s="92"/>
-      <c r="B93" s="105"/>
-      <c r="C93" s="97"/>
-      <c r="D93" s="101"/>
-      <c r="E93" s="102"/>
+      <c r="A93" s="83"/>
+      <c r="B93" s="84"/>
+      <c r="C93" s="86"/>
+      <c r="D93" s="90"/>
+      <c r="E93" s="91"/>
       <c r="F93" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G93" s="17"/>
       <c r="H93" s="17"/>
@@ -14289,11 +14315,11 @@
       <c r="ED93" s="18"/>
     </row>
     <row r="94" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A94" s="92"/>
-      <c r="B94" s="105"/>
-      <c r="C94" s="98"/>
-      <c r="D94" s="103"/>
-      <c r="E94" s="104"/>
+      <c r="A94" s="83"/>
+      <c r="B94" s="84"/>
+      <c r="C94" s="87"/>
+      <c r="D94" s="92"/>
+      <c r="E94" s="93"/>
       <c r="F94" s="61"/>
       <c r="G94" s="17"/>
       <c r="H94" s="17"/>
@@ -14425,21 +14451,21 @@
       <c r="ED94" s="18"/>
     </row>
     <row r="95" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A95" s="92">
+      <c r="A95" s="83">
         <v>14</v>
       </c>
-      <c r="B95" s="93" t="s">
+      <c r="B95" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="83" t="s">
+      <c r="C95" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="E95" s="87"/>
+      <c r="D95" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="E95" s="98"/>
       <c r="F95" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G95" s="23"/>
       <c r="H95" s="24"/>
@@ -14571,11 +14597,11 @@
       <c r="ED95" s="25"/>
     </row>
     <row r="96" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A96" s="92"/>
-      <c r="B96" s="93"/>
-      <c r="C96" s="84"/>
-      <c r="D96" s="95"/>
-      <c r="E96" s="89"/>
+      <c r="A96" s="83"/>
+      <c r="B96" s="103"/>
+      <c r="C96" s="95"/>
+      <c r="D96" s="99"/>
+      <c r="E96" s="100"/>
       <c r="F96" s="61"/>
       <c r="G96" s="26"/>
       <c r="H96" s="27"/>
@@ -14707,13 +14733,13 @@
       <c r="ED96" s="28"/>
     </row>
     <row r="97" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A97" s="92"/>
-      <c r="B97" s="93"/>
-      <c r="C97" s="84"/>
-      <c r="D97" s="95"/>
-      <c r="E97" s="89"/>
+      <c r="A97" s="83"/>
+      <c r="B97" s="103"/>
+      <c r="C97" s="95"/>
+      <c r="D97" s="99"/>
+      <c r="E97" s="100"/>
       <c r="F97" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G97" s="26"/>
       <c r="H97" s="27"/>
@@ -14845,11 +14871,11 @@
       <c r="ED97" s="28"/>
     </row>
     <row r="98" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A98" s="92"/>
-      <c r="B98" s="93"/>
-      <c r="C98" s="85"/>
-      <c r="D98" s="90"/>
-      <c r="E98" s="91"/>
+      <c r="A98" s="83"/>
+      <c r="B98" s="103"/>
+      <c r="C98" s="96"/>
+      <c r="D98" s="101"/>
+      <c r="E98" s="102"/>
       <c r="F98" s="61"/>
       <c r="G98" s="26"/>
       <c r="H98" s="27"/>
@@ -14981,19 +15007,19 @@
       <c r="ED98" s="28"/>
     </row>
     <row r="99" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A99" s="92">
+      <c r="A99" s="83">
         <v>15</v>
       </c>
-      <c r="B99" s="93"/>
-      <c r="C99" s="96" t="s">
+      <c r="B99" s="103"/>
+      <c r="C99" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="99" t="s">
-        <v>47</v>
-      </c>
-      <c r="E99" s="100"/>
+      <c r="D99" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" s="89"/>
       <c r="F99" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G99" s="15"/>
       <c r="H99" s="11"/>
@@ -15125,11 +15151,11 @@
       <c r="ED99" s="12"/>
     </row>
     <row r="100" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A100" s="92"/>
-      <c r="B100" s="93"/>
-      <c r="C100" s="97"/>
-      <c r="D100" s="101"/>
-      <c r="E100" s="102"/>
+      <c r="A100" s="83"/>
+      <c r="B100" s="103"/>
+      <c r="C100" s="86"/>
+      <c r="D100" s="90"/>
+      <c r="E100" s="91"/>
       <c r="F100" s="61"/>
       <c r="G100" s="17"/>
       <c r="H100" s="17"/>
@@ -15261,13 +15287,13 @@
       <c r="ED100" s="18"/>
     </row>
     <row r="101" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A101" s="92"/>
-      <c r="B101" s="93"/>
-      <c r="C101" s="97"/>
-      <c r="D101" s="101"/>
-      <c r="E101" s="102"/>
+      <c r="A101" s="83"/>
+      <c r="B101" s="103"/>
+      <c r="C101" s="86"/>
+      <c r="D101" s="90"/>
+      <c r="E101" s="91"/>
       <c r="F101" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G101" s="17"/>
       <c r="H101" s="17"/>
@@ -15399,11 +15425,11 @@
       <c r="ED101" s="18"/>
     </row>
     <row r="102" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A102" s="92"/>
-      <c r="B102" s="93"/>
-      <c r="C102" s="98"/>
-      <c r="D102" s="103"/>
-      <c r="E102" s="104"/>
+      <c r="A102" s="83"/>
+      <c r="B102" s="103"/>
+      <c r="C102" s="87"/>
+      <c r="D102" s="92"/>
+      <c r="E102" s="93"/>
       <c r="F102" s="61"/>
       <c r="G102" s="17"/>
       <c r="H102" s="17"/>
@@ -15535,19 +15561,19 @@
       <c r="ED102" s="18"/>
     </row>
     <row r="103" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A103" s="92">
+      <c r="A103" s="83">
         <v>16</v>
       </c>
-      <c r="B103" s="93"/>
-      <c r="C103" s="83" t="s">
+      <c r="B103" s="103"/>
+      <c r="C103" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="D103" s="94" t="s">
-        <v>28</v>
-      </c>
-      <c r="E103" s="87"/>
+      <c r="D103" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="E103" s="98"/>
       <c r="F103" s="60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G103" s="23"/>
       <c r="H103" s="24"/>
@@ -15679,11 +15705,11 @@
       <c r="ED103" s="25"/>
     </row>
     <row r="104" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A104" s="92"/>
-      <c r="B104" s="93"/>
-      <c r="C104" s="84"/>
-      <c r="D104" s="95"/>
-      <c r="E104" s="89"/>
+      <c r="A104" s="83"/>
+      <c r="B104" s="103"/>
+      <c r="C104" s="95"/>
+      <c r="D104" s="99"/>
+      <c r="E104" s="100"/>
       <c r="F104" s="61"/>
       <c r="G104" s="26"/>
       <c r="H104" s="27"/>
@@ -15815,13 +15841,13 @@
       <c r="ED104" s="28"/>
     </row>
     <row r="105" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A105" s="92"/>
-      <c r="B105" s="93"/>
-      <c r="C105" s="84"/>
-      <c r="D105" s="95"/>
-      <c r="E105" s="89"/>
+      <c r="A105" s="83"/>
+      <c r="B105" s="103"/>
+      <c r="C105" s="95"/>
+      <c r="D105" s="99"/>
+      <c r="E105" s="100"/>
       <c r="F105" s="62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G105" s="26"/>
       <c r="H105" s="27"/>
@@ -15953,11 +15979,11 @@
       <c r="ED105" s="28"/>
     </row>
     <row r="106" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A106" s="92"/>
-      <c r="B106" s="93"/>
-      <c r="C106" s="85"/>
-      <c r="D106" s="90"/>
-      <c r="E106" s="91"/>
+      <c r="A106" s="83"/>
+      <c r="B106" s="103"/>
+      <c r="C106" s="96"/>
+      <c r="D106" s="101"/>
+      <c r="E106" s="102"/>
       <c r="F106" s="61"/>
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
@@ -16089,13 +16115,13 @@
       <c r="ED106" s="28"/>
     </row>
     <row r="107" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A107" s="76"/>
+      <c r="A107" s="106"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="77" t="s">
+      <c r="C107" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="79"/>
-      <c r="E107" s="80"/>
+      <c r="D107" s="109"/>
+      <c r="E107" s="110"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
       <c r="H107" s="44"/>
@@ -16229,11 +16255,11 @@
       <c r="ED107" s="45"/>
     </row>
     <row r="108" spans="1:134" x14ac:dyDescent="0.25">
-      <c r="A108" s="76"/>
+      <c r="A108" s="106"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="78"/>
-      <c r="D108" s="81"/>
-      <c r="E108" s="82"/>
+      <c r="C108" s="108"/>
+      <c r="D108" s="111"/>
+      <c r="E108" s="112"/>
       <c r="F108" s="46"/>
       <c r="G108" s="47"/>
       <c r="H108" s="48"/>
@@ -16366,24 +16392,60 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="AE1:AL1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:V1"/>
-    <mergeCell ref="W1:AD1"/>
-    <mergeCell ref="DW1:ED1"/>
-    <mergeCell ref="AM1:AT1"/>
-    <mergeCell ref="AU1:BB1"/>
-    <mergeCell ref="BC1:BJ1"/>
-    <mergeCell ref="BK1:BR1"/>
-    <mergeCell ref="BS1:BZ1"/>
-    <mergeCell ref="CA1:CH1"/>
-    <mergeCell ref="CI1:CP1"/>
-    <mergeCell ref="CQ1:CX1"/>
-    <mergeCell ref="CY1:DF1"/>
-    <mergeCell ref="DG1:DN1"/>
-    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="D107:E108"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:E90"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B106"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:E98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="D99:E102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="D103:E106"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B94"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:E82"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:E94"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:E86"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:E74"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:E78"/>
+    <mergeCell ref="D59:E62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:E66"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:E70"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="D51:E54"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D55:E58"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B78"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C35:C38"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B22"/>
     <mergeCell ref="C3:C6"/>
@@ -16400,60 +16462,24 @@
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="C19:C22"/>
     <mergeCell ref="D19:E22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B78"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:E26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:E30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:E34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D35:E38"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="D39:E42"/>
-    <mergeCell ref="D47:E50"/>
-    <mergeCell ref="D51:E54"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D55:E58"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:E74"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:E78"/>
-    <mergeCell ref="D59:E62"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:E66"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:E70"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B94"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="D79:E82"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="D91:E94"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="D83:E86"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="D107:E108"/>
-    <mergeCell ref="C87:C90"/>
-    <mergeCell ref="D87:E90"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:E98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:E102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="D103:E106"/>
+    <mergeCell ref="DW1:ED1"/>
+    <mergeCell ref="AM1:AT1"/>
+    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="BC1:BJ1"/>
+    <mergeCell ref="BK1:BR1"/>
+    <mergeCell ref="BS1:BZ1"/>
+    <mergeCell ref="CA1:CH1"/>
+    <mergeCell ref="CI1:CP1"/>
+    <mergeCell ref="CQ1:CX1"/>
+    <mergeCell ref="CY1:DF1"/>
+    <mergeCell ref="DG1:DN1"/>
+    <mergeCell ref="DO1:DV1"/>
+    <mergeCell ref="AE1:AL1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>